<commit_message>
Update SKU generation logic and product import file
Modify the `generateSKU` function in `server/storage.ts` to create SKUs with more letters derived from the product name and two random letters at the end, replacing the previous numeric suffix. Regenerate the `products-import-final.xlsx` file with the updated SKU format.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 8436b268-12fd-450e-b517-e55adeb71af1
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 4d91ef6a-a828-485d-9abd-eb87043e4c0d
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/6e81966b-af7d-438d-b68d-89d915c5170b/8436b268-12fd-450e-b517-e55adeb71af1/pCPGKM5
</commit_message>
<xml_diff>
--- a/attached_assets/products-import-final.xlsx
+++ b/attached_assets/products-import-final.xlsx
@@ -404,7 +404,7 @@
   <cols>
     <col min="1" max="1" width="40.83203125" customWidth="1"/>
     <col min="2" max="2" width="40.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="45.83203125" customWidth="1"/>
@@ -510,7 +510,7 @@
         <v>4XC - 5in1</v>
       </c>
       <c r="C2" t="str">
-        <v>DAU-4XC5IN-001</v>
+        <v>DAU-4XC5IN1FH</v>
       </c>
       <c r="D2" t="str">
         <v/>
@@ -584,7 +584,7 @@
         <v>M - nhỏ tròn</v>
       </c>
       <c r="C3" t="str">
-        <v>DAU-MNHOTR-002</v>
+        <v>DAU-MNHOTRONTP</v>
       </c>
       <c r="D3" t="str">
         <v/>
@@ -658,7 +658,7 @@
         <v>XF - nhỏ</v>
       </c>
       <c r="C4" t="str">
-        <v>DAU-XFNHO-003</v>
+        <v>DAU-XFNHORH</v>
       </c>
       <c r="D4" t="str">
         <v/>
@@ -732,7 +732,7 @@
         <v>Sticker - 5D</v>
       </c>
       <c r="C5" t="str">
-        <v>DES-STICKE-004</v>
+        <v>DES-STICKER5DQG</v>
       </c>
       <c r="D5" t="str">
         <v/>
@@ -806,7 +806,7 @@
         <v>Sticker - 3D</v>
       </c>
       <c r="C6" t="str">
-        <v>DES-STICKE-005</v>
+        <v>DES-STICKER3DNW</v>
       </c>
       <c r="D6" t="str">
         <v/>
@@ -880,7 +880,7 @@
         <v>Sticker - 2D</v>
       </c>
       <c r="C7" t="str">
-        <v>DES-STICKE-006</v>
+        <v>DES-STICKER2DHH</v>
       </c>
       <c r="D7" t="str">
         <v/>
@@ -954,7 +954,7 @@
         <v>Foil sticker</v>
       </c>
       <c r="C8" t="str">
-        <v>DES-FOILST-007</v>
+        <v>DES-FOILSTICKEQA</v>
       </c>
       <c r="D8" t="str">
         <v/>
@@ -1028,7 +1028,7 @@
         <v>Tips natur nhọn ngắn</v>
       </c>
       <c r="C9" t="str">
-        <v>TIP-TIPSNA-008</v>
+        <v>TIP-TIPSNATURNKB</v>
       </c>
       <c r="D9" t="str">
         <v/>
@@ -1102,7 +1102,7 @@
         <v>Tips natur thẳng ngắn</v>
       </c>
       <c r="C10" t="str">
-        <v>TIP-TIPSNA-009</v>
+        <v>TIP-TIPSNATURTNM</v>
       </c>
       <c r="D10" t="str">
         <v/>
@@ -1176,7 +1176,7 @@
         <v>Tips natur nhọn dài</v>
       </c>
       <c r="C11" t="str">
-        <v>TIP-TIPSNA-010</v>
+        <v>TIP-TIPSNATURNQK</v>
       </c>
       <c r="D11" t="str">
         <v/>
@@ -1250,7 +1250,7 @@
         <v>Tips trong nhọn ngắn</v>
       </c>
       <c r="C12" t="str">
-        <v>TIP-TIPSTR-011</v>
+        <v>TIP-TIPSTRONGNBM</v>
       </c>
       <c r="D12" t="str">
         <v/>
@@ -1324,7 +1324,7 @@
         <v>Đá nhỏ 7mầu</v>
       </c>
       <c r="C13" t="str">
-        <v>DES-DANHO7-012</v>
+        <v>DES-DANHO7MAUPR</v>
       </c>
       <c r="D13" t="str">
         <v/>
@@ -1398,7 +1398,7 @@
         <v>Bút vẽ (1set=3c)</v>
       </c>
       <c r="C14" t="str">
-        <v>BUT-BUTVE1-013</v>
+        <v>BUT-BUTVE1SET3UK</v>
       </c>
       <c r="D14" t="str">
         <v/>
@@ -1472,7 +1472,7 @@
         <v>Hộp đựng móng (0-9)</v>
       </c>
       <c r="C15" t="str">
-        <v>TOO-HOPDUN-014</v>
+        <v>TOO-HOPDUNGMONLU</v>
       </c>
       <c r="D15" t="str">
         <v/>
@@ -1546,7 +1546,7 @@
         <v>Cây fen - V shape</v>
       </c>
       <c r="C16" t="str">
-        <v>TOO-CAYFEN-015</v>
+        <v>TOO-CAYFENVSHAEW</v>
       </c>
       <c r="D16" t="str">
         <v/>
@@ -1620,7 +1620,7 @@
         <v>Cây fen - U shape</v>
       </c>
       <c r="C17" t="str">
-        <v>TOO-CAYFEN-016</v>
+        <v>TOO-CAYFENUSHACF</v>
       </c>
       <c r="D17" t="str">
         <v/>
@@ -1694,7 +1694,7 @@
         <v>Mịn Fusion</v>
       </c>
       <c r="C18" t="str">
-        <v>DAU-MINFUS-017</v>
+        <v>DAU-MINFUSIONBC</v>
       </c>
       <c r="D18" t="str">
         <v/>
@@ -1768,7 +1768,7 @@
         <v>French A</v>
       </c>
       <c r="C19" t="str">
-        <v>TOO-FRENCH-018</v>
+        <v>TOO-FRENCHAKI</v>
       </c>
       <c r="D19" t="str">
         <v/>
@@ -1842,7 +1842,7 @@
         <v>French B</v>
       </c>
       <c r="C20" t="str">
-        <v>TOO-FRENCH-019</v>
+        <v>TOO-FRENCHBZG</v>
       </c>
       <c r="D20" t="str">
         <v/>
@@ -1916,7 +1916,7 @@
         <v>Sticker lửa</v>
       </c>
       <c r="C21" t="str">
-        <v>DES-STICKE-020</v>
+        <v>DES-STICKERLUATD</v>
       </c>
       <c r="D21" t="str">
         <v/>
@@ -1990,7 +1990,7 @@
         <v>Bút vẽ 2 đầu - 7/11mm</v>
       </c>
       <c r="C22" t="str">
-        <v>BUT-BUTVE2-021</v>
+        <v>BUT-BUTVE2DAU7PA</v>
       </c>
       <c r="D22" t="str">
         <v/>
@@ -2064,7 +2064,7 @@
         <v>Chrome Red</v>
       </c>
       <c r="C23" t="str">
-        <v>DES-CHROME-022</v>
+        <v>DES-CHROMEREDJL</v>
       </c>
       <c r="D23" t="str">
         <v/>
@@ -2138,7 +2138,7 @@
         <v>Sơn Ultra Black</v>
       </c>
       <c r="C24" t="str">
-        <v>HOA-SONULT-023</v>
+        <v>HOA-SONULTRABLFG</v>
       </c>
       <c r="D24" t="str">
         <v/>
@@ -2212,7 +2212,7 @@
         <v>Sơn Ultra White</v>
       </c>
       <c r="C25" t="str">
-        <v>HOA-SONULT-024</v>
+        <v>HOA-SONULTRAWHRT</v>
       </c>
       <c r="D25" t="str">
         <v/>
@@ -2286,7 +2286,7 @@
         <v>Vỏ nhám tím ⌗60 - C</v>
       </c>
       <c r="C26" t="str">
-        <v>TOO-VONHAM-025</v>
+        <v>TOO-VONHAMTIM6BJ</v>
       </c>
       <c r="D26" t="str">
         <v/>
@@ -2360,7 +2360,7 @@
         <v>Bút fen</v>
       </c>
       <c r="C27" t="str">
-        <v>BUT-BUTFEN-026</v>
+        <v>BUT-BUTFENEL</v>
       </c>
       <c r="D27" t="str">
         <v/>
@@ -2434,7 +2434,7 @@
         <v>Bút ombre</v>
       </c>
       <c r="C28" t="str">
-        <v>BUT-BUTOMB-027</v>
+        <v>BUT-BUTOMBRESA</v>
       </c>
       <c r="D28" t="str">
         <v/>
@@ -2508,7 +2508,7 @@
         <v>Vỏ nhám trắng ⌗60 - C</v>
       </c>
       <c r="C29" t="str">
-        <v>TOO-VONHAM-028</v>
+        <v>TOO-VONHAMTRANFI</v>
       </c>
       <c r="D29" t="str">
         <v/>
@@ -2582,7 +2582,7 @@
         <v>Set sơn mầu vẽ 12 lọ</v>
       </c>
       <c r="C30" t="str">
-        <v>HOA-SETSON-029</v>
+        <v>HOA-SETSONMAUVEF</v>
       </c>
       <c r="D30" t="str">
         <v/>
@@ -2656,7 +2656,7 @@
         <v>Đá kê sơn</v>
       </c>
       <c r="C31" t="str">
-        <v>TOO-DAKESO-030</v>
+        <v>TOO-DAKESONPI</v>
       </c>
       <c r="D31" t="str">
         <v/>
@@ -2730,7 +2730,7 @@
         <v>Sticker Bướm</v>
       </c>
       <c r="C32" t="str">
-        <v>DES-STICKE-031</v>
+        <v>DES-STICKERBUOEF</v>
       </c>
       <c r="D32" t="str">
         <v/>
@@ -2804,7 +2804,7 @@
         <v>Đá rắc 28g</v>
       </c>
       <c r="C33" t="str">
-        <v>DES-DARAC2-032</v>
+        <v>DES-DARAC28GWB</v>
       </c>
       <c r="D33" t="str">
         <v/>
@@ -2878,7 +2878,7 @@
         <v>Kê tay Silicon</v>
       </c>
       <c r="C34" t="str">
-        <v>TOO-KETAYS-033</v>
+        <v>TOO-KETAYSILICMZ</v>
       </c>
       <c r="D34" t="str">
         <v/>
@@ -2952,7 +2952,7 @@
         <v>Bút mực vẽ</v>
       </c>
       <c r="C35" t="str">
-        <v>DES-BUTMUC-034</v>
+        <v>DES-BUTMUCVEOJ</v>
       </c>
       <c r="D35" t="str">
         <v/>
@@ -3026,7 +3026,7 @@
         <v>5in1 Phá 2XC</v>
       </c>
       <c r="C36" t="str">
-        <v>DAU-5IN1PH-035</v>
+        <v>DAU-5IN1PHA2XCVB</v>
       </c>
       <c r="D36" t="str">
         <v/>
@@ -3100,7 +3100,7 @@
         <v>Bút đắp gel sz14</v>
       </c>
       <c r="C37" t="str">
-        <v>BUT-BUTDAP-036</v>
+        <v>BUT-BUTDAPGELSEF</v>
       </c>
       <c r="D37" t="str">
         <v/>
@@ -3174,7 +3174,7 @@
         <v>Tips thường gói 50c</v>
       </c>
       <c r="C38" t="str">
-        <v>TIP-TIPSTH-037</v>
+        <v>TIP-TIPSTHUONGJG</v>
       </c>
       <c r="D38" t="str">
         <v/>
@@ -3248,7 +3248,7 @@
         <v>Bút gel đỏ sz8</v>
       </c>
       <c r="C39" t="str">
-        <v>BUT-BUTGEL-038</v>
+        <v>BUT-BUTGELDOSZZF</v>
       </c>
       <c r="D39" t="str">
         <v/>
@@ -3322,7 +3322,7 @@
         <v>In French</v>
       </c>
       <c r="C40" t="str">
-        <v>DES-INFREN-039</v>
+        <v>DES-INFRENCHSZ</v>
       </c>
       <c r="D40" t="str">
         <v/>
@@ -3396,7 +3396,7 @@
         <v>Dao cắt fen</v>
       </c>
       <c r="C41" t="str">
-        <v>TOO-DAOCAT-040</v>
+        <v>TOO-DAOCATFENRY</v>
       </c>
       <c r="D41" t="str">
         <v/>
@@ -3470,7 +3470,7 @@
         <v>Sticker playboy</v>
       </c>
       <c r="C42" t="str">
-        <v>DES-STICKE-041</v>
+        <v>DES-STICKERPLARY</v>
       </c>
       <c r="D42" t="str">
         <v/>
@@ -3544,7 +3544,7 @@
         <v>Gold foil</v>
       </c>
       <c r="C43" t="str">
-        <v>DES-GOLDFO-042</v>
+        <v>DES-GOLDFOILBT</v>
       </c>
       <c r="D43" t="str">
         <v/>
@@ -3618,7 +3618,7 @@
         <v>Bút gel - tròn 10</v>
       </c>
       <c r="C44" t="str">
-        <v>BUT-BUTGEL-043</v>
+        <v>BUT-BUTGELTRONLW</v>
       </c>
       <c r="D44" t="str">
         <v/>
@@ -3692,7 +3692,7 @@
         <v>Bút gel quét mầu - tròn 8</v>
       </c>
       <c r="C45" t="str">
-        <v>BUT-BUTGEL-044</v>
+        <v>BUT-BUTGELQUETYP</v>
       </c>
       <c r="D45" t="str">
         <v/>
@@ -3766,7 +3766,7 @@
         <v>Set bào &amp; vỏ mịn da chân</v>
       </c>
       <c r="C46" t="str">
-        <v>DAU-SETBAO-045</v>
+        <v>DAU-SETBAOVOMIVA</v>
       </c>
       <c r="D46" t="str">
         <v/>
@@ -3840,7 +3840,7 @@
         <v>Tips Vuông trong XXL</v>
       </c>
       <c r="C47" t="str">
-        <v>TIP-TIPSVU-046</v>
+        <v>TIP-TIPSVUONGTRK</v>
       </c>
       <c r="D47" t="str">
         <v/>
@@ -3914,7 +3914,7 @@
         <v>Bấm móng 777 Korea</v>
       </c>
       <c r="C48" t="str">
-        <v>TOO-BAMMON-047</v>
+        <v>TOO-BAMMONG777EE</v>
       </c>
       <c r="D48" t="str">
         <v/>
@@ -3988,7 +3988,7 @@
         <v>Sticker Halloween Phát sáng</v>
       </c>
       <c r="C49" t="str">
-        <v>DES-STICKE-048</v>
+        <v>DES-STICKERHALYL</v>
       </c>
       <c r="D49" t="str">
         <v/>
@@ -4062,7 +4062,7 @@
         <v>Top matte 15ml</v>
       </c>
       <c r="C50" t="str">
-        <v>HOA-TOPMAT-049</v>
+        <v>HOA-TOPMATTE15LM</v>
       </c>
       <c r="D50" t="str">
         <v/>
@@ -4136,7 +4136,7 @@
         <v>Foil gel</v>
       </c>
       <c r="C51" t="str">
-        <v>HOA-FOILGE-050</v>
+        <v>HOA-FOILGELPT</v>
       </c>
       <c r="D51" t="str">
         <v/>
@@ -4210,7 +4210,7 @@
         <v>Sticker Playboy</v>
       </c>
       <c r="C52" t="str">
-        <v>DES-STICKE-051</v>
+        <v>DES-STICKERPLADA</v>
       </c>
       <c r="D52" t="str">
         <v/>
@@ -4284,7 +4284,7 @@
         <v>Bình xịt ombre bột</v>
       </c>
       <c r="C53" t="str">
-        <v>TOO-BINHXI-052</v>
+        <v>TOO-BINHXITOMBNK</v>
       </c>
       <c r="D53" t="str">
         <v/>
@@ -4358,7 +4358,7 @@
         <v>Tay giả mềm</v>
       </c>
       <c r="C54" t="str">
-        <v>TOO-TAYGIA-053</v>
+        <v>TOO-TAYGIAMEMYL</v>
       </c>
       <c r="D54" t="str">
         <v/>
@@ -4432,7 +4432,7 @@
         <v>Tay giả khớp</v>
       </c>
       <c r="C55" t="str">
-        <v>TOO-TAYGIA-054</v>
+        <v>TOO-TAYGIAKHOPOJ</v>
       </c>
       <c r="D55" t="str">
         <v/>
@@ -4506,7 +4506,7 @@
         <v>Bút Gradient</v>
       </c>
       <c r="C56" t="str">
-        <v>BUT-BUTGRA-055</v>
+        <v>BUT-BUTGRADIENVR</v>
       </c>
       <c r="D56" t="str">
         <v/>
@@ -4580,7 +4580,7 @@
         <v>Đầu Chổi sắt</v>
       </c>
       <c r="C57" t="str">
-        <v>DAU-DAUCHO-056</v>
+        <v>DAU-DAUCHOISATYH</v>
       </c>
       <c r="D57" t="str">
         <v/>
@@ -4654,7 +4654,7 @@
         <v>3in1 Mịn C - ngắn</v>
       </c>
       <c r="C58" t="str">
-        <v>DAU-3IN1MI-057</v>
+        <v>DAU-3IN1MINCNGGD</v>
       </c>
       <c r="D58" t="str">
         <v/>
@@ -4728,7 +4728,7 @@
         <v>3XC ULTRA</v>
       </c>
       <c r="C59" t="str">
-        <v>DAU-3XCULT-058</v>
+        <v>DAU-3XCULTRABP</v>
       </c>
       <c r="D59" t="str">
         <v/>
@@ -4802,7 +4802,7 @@
         <v>5XC - Titan</v>
       </c>
       <c r="C60" t="str">
-        <v>DAU-5XCTIT-059</v>
+        <v>DAU-5XCTITANLX</v>
       </c>
       <c r="D60" t="str">
         <v/>
@@ -4876,7 +4876,7 @@
         <v>Bào nhám Diamond nhỏ - M</v>
       </c>
       <c r="C61" t="str">
-        <v>DAU-BAONHA-060</v>
+        <v>DAU-BAONHAMDIAIH</v>
       </c>
       <c r="D61" t="str">
         <v/>
@@ -4950,7 +4950,7 @@
         <v>Bào nhám Diamond to - C</v>
       </c>
       <c r="C62" t="str">
-        <v>DAU-BAONHA-061</v>
+        <v>DAU-BAONHAMDIAHI</v>
       </c>
       <c r="D62" t="str">
         <v/>
@@ -5024,7 +5024,7 @@
         <v>Hoa 3D Design</v>
       </c>
       <c r="C63" t="str">
-        <v>DES-HOA3DD-062</v>
+        <v>DES-HOA3DDESIGKO</v>
       </c>
       <c r="D63" t="str">
         <v/>
@@ -5098,7 +5098,7 @@
         <v>Sticker chữ</v>
       </c>
       <c r="C64" t="str">
-        <v>DES-STICKE-063</v>
+        <v>DES-STICKERCHUJP</v>
       </c>
       <c r="D64" t="str">
         <v/>
@@ -5172,7 +5172,7 @@
         <v>Tips Ballerina trong XXL</v>
       </c>
       <c r="C65" t="str">
-        <v>TIP-TIPSBA-064</v>
+        <v>TIP-TIPSBALLERKQ</v>
       </c>
       <c r="D65" t="str">
         <v/>
@@ -5246,7 +5246,7 @@
         <v>Tip ballerina ngắn 4/5/5/6</v>
       </c>
       <c r="C66" t="str">
-        <v>TOO-TIPBAL-065</v>
+        <v>TOO-TIPBALLERIUQ</v>
       </c>
       <c r="D66" t="str">
         <v/>
@@ -5320,7 +5320,7 @@
         <v>Tip trong nhọn 4/5/5/6</v>
       </c>
       <c r="C67" t="str">
-        <v>TOO-TIPTRO-066</v>
+        <v>TOO-TIPTRONGNHFG</v>
       </c>
       <c r="D67" t="str">
         <v/>
@@ -5394,7 +5394,7 @@
         <v>Lá Trái tim set</v>
       </c>
       <c r="C68" t="str">
-        <v>DES-LATRAI-067</v>
+        <v>DES-LATRAITIMSDJ</v>
       </c>
       <c r="D68" t="str">
         <v/>
@@ -5468,7 +5468,7 @@
         <v>Bột màu 56g</v>
       </c>
       <c r="C69" t="str">
-        <v>HOA-BOTMAU-068</v>
+        <v>HOA-BOTMAU56GOU</v>
       </c>
       <c r="D69" t="str">
         <v/>
@@ -5542,7 +5542,7 @@
         <v>Máy xịt ombre gel</v>
       </c>
       <c r="C70" t="str">
-        <v>DOD-MAYXIT-069</v>
+        <v>DOD-MAYXITOMBRDY</v>
       </c>
       <c r="D70" t="str">
         <v/>
@@ -5616,7 +5616,7 @@
         <v>Sơn vẽ hũ Metallic 5g</v>
       </c>
       <c r="C71" t="str">
-        <v>DES-SONVEH-070</v>
+        <v>DES-SONVEHUMETEM</v>
       </c>
       <c r="D71" t="str">
         <v/>
@@ -5690,7 +5690,7 @@
         <v>Sơn vẽ hũ 5g</v>
       </c>
       <c r="C72" t="str">
-        <v>DES-SONVEH-071</v>
+        <v>DES-SONVEHU5GUN</v>
       </c>
       <c r="D72" t="str">
         <v/>
@@ -5764,7 +5764,7 @@
         <v>Cuticle oil 15ml</v>
       </c>
       <c r="C73" t="str">
-        <v>HOA-CUTICL-072</v>
+        <v>HOA-CUTICLEOILHX</v>
       </c>
       <c r="D73" t="str">
         <v/>
@@ -5838,7 +5838,7 @@
         <v>Gel vẽ màng nhện 5g</v>
       </c>
       <c r="C74" t="str">
-        <v>DES-GELVEM-073</v>
+        <v>DES-GELVEMANGNVY</v>
       </c>
       <c r="D74" t="str">
         <v/>
@@ -5912,7 +5912,7 @@
         <v>Nhám trắng M ⌗240 (1000c)</v>
       </c>
       <c r="C75" t="str">
-        <v>TOO-NHAMTR-074</v>
+        <v>TOO-NHAMTRANGMLR</v>
       </c>
       <c r="D75" t="str">
         <v/>
@@ -5986,7 +5986,7 @@
         <v>Tips trong nhọn dài</v>
       </c>
       <c r="C76" t="str">
-        <v>TIP-TIPSTR-075</v>
+        <v>TIP-TIPSTRONGNIY</v>
       </c>
       <c r="D76" t="str">
         <v/>
@@ -6060,7 +6060,7 @@
         <v>Lẻ - Tip Trong nhọn</v>
       </c>
       <c r="C77" t="str">
-        <v>TIP-LETIPT-076</v>
+        <v>TIP-LETIPTRONGKP</v>
       </c>
       <c r="D77" t="str">
         <v/>
@@ -6134,7 +6134,7 @@
         <v>Bào Diamond Cuticle 2.5mm</v>
       </c>
       <c r="C78" t="str">
-        <v>DAU-BAODIA-077</v>
+        <v>DAU-BAODIAMONDOJ</v>
       </c>
       <c r="D78" t="str">
         <v/>
@@ -6208,7 +6208,7 @@
         <v>Sticker F Noel - 3D</v>
       </c>
       <c r="C79" t="str">
-        <v>DES-STICKE-078</v>
+        <v>DES-STICKERFNORT</v>
       </c>
       <c r="D79" t="str">
         <v/>
@@ -6282,7 +6282,7 @@
         <v>Sticker STZ Noel - 5D</v>
       </c>
       <c r="C80" t="str">
-        <v>DES-STICKE-079</v>
+        <v>DES-STICKERSTZGZ</v>
       </c>
       <c r="D80" t="str">
         <v/>
@@ -6356,7 +6356,7 @@
         <v>Kéo</v>
       </c>
       <c r="C81" t="str">
-        <v>TOO-KEO-080</v>
+        <v>TOO-KEOZQ</v>
       </c>
       <c r="D81" t="str">
         <v/>
@@ -6430,7 +6430,7 @@
         <v>Máy Bào Btmarathon 3</v>
       </c>
       <c r="C82" t="str">
-        <v>DOD-MAYBAO-081</v>
+        <v>DOD-MAYBAOBTMADA</v>
       </c>
       <c r="D82" t="str">
         <v/>
@@ -6504,7 +6504,7 @@
         <v>Bút chấm bi set 5c</v>
       </c>
       <c r="C83" t="str">
-        <v>TOO-BUTCHA-082</v>
+        <v>TOO-BUTCHAMBISXF</v>
       </c>
       <c r="D83" t="str">
         <v/>
@@ -6578,7 +6578,7 @@
         <v>Cán dao cạo chân - hồng</v>
       </c>
       <c r="C84" t="str">
-        <v>TOO-CANDAO-083</v>
+        <v>TOO-CANDAOCAOCOF</v>
       </c>
       <c r="D84" t="str">
         <v/>
@@ -6652,7 +6652,7 @@
         <v>Đèn LED pin cầm tay</v>
       </c>
       <c r="C85" t="str">
-        <v>DOD-DENLED-084</v>
+        <v>DOD-DENLEDPINCZR</v>
       </c>
       <c r="D85" t="str">
         <v/>
@@ -6726,7 +6726,7 @@
         <v>Khay inox</v>
       </c>
       <c r="C86" t="str">
-        <v>TOO-KHAYIN-085</v>
+        <v>TOO-KHAYINOXHS</v>
       </c>
       <c r="D86" t="str">
         <v/>
@@ -6800,7 +6800,7 @@
         <v>Tay thay máy bào di động</v>
       </c>
       <c r="C87" t="str">
-        <v>DOD-TAYTHA-086</v>
+        <v>DOD-TAYTHAYMAYAJ</v>
       </c>
       <c r="D87" t="str">
         <v/>
@@ -6874,7 +6874,7 @@
         <v>Cây đẩy da inox japan</v>
       </c>
       <c r="C88" t="str">
-        <v>TOO-CAYDAY-087</v>
+        <v>TOO-CAYDAYDAINKX</v>
       </c>
       <c r="D88" t="str">
         <v/>
@@ -6948,7 +6948,7 @@
         <v>3XC Hoa cúc ULTRA</v>
       </c>
       <c r="C89" t="str">
-        <v>DAU-3XCHOA-088</v>
+        <v>DAU-3XCHOACUCUBC</v>
       </c>
       <c r="D89" t="str">
         <v/>
@@ -7022,7 +7022,7 @@
         <v>Bút quan tài</v>
       </c>
       <c r="C90" t="str">
-        <v>BUT-BUTQUA-089</v>
+        <v>BUT-BUTQUANTAIYM</v>
       </c>
       <c r="D90" t="str">
         <v/>
@@ -7096,7 +7096,7 @@
         <v>Bút vẽ 2 đầu - 10/20mm</v>
       </c>
       <c r="C91" t="str">
-        <v>BUT-BUTVE2-090</v>
+        <v>BUT-BUTVE2DAU1ZI</v>
       </c>
       <c r="D91" t="str">
         <v/>
@@ -7170,7 +7170,7 @@
         <v>Kéo - dài</v>
       </c>
       <c r="C92" t="str">
-        <v>TOO-KEODAI-091</v>
+        <v>TOO-KEODAIAV</v>
       </c>
       <c r="D92" t="str">
         <v/>
@@ -7244,7 +7244,7 @@
         <v>4XC - Titan</v>
       </c>
       <c r="C93" t="str">
-        <v>DAU-4XCTIT-092</v>
+        <v>DAU-4XCTITANUC</v>
       </c>
       <c r="D93" t="str">
         <v/>
@@ -7318,7 +7318,7 @@
         <v>4XC trục nhỏ</v>
       </c>
       <c r="C94" t="str">
-        <v>DAU-4XCTRU-093</v>
+        <v>DAU-4XCTRUCNHOYE</v>
       </c>
       <c r="D94" t="str">
         <v/>
@@ -7392,7 +7392,7 @@
         <v>Vỏ nhám trắng M ⌗240 (100c)</v>
       </c>
       <c r="C95" t="str">
-        <v>TOO-VONHAM-094</v>
+        <v>TOO-VONHAMTRANBO</v>
       </c>
       <c r="D95" t="str">
         <v/>
@@ -7466,7 +7466,7 @@
         <v>Găng tay Latex trắng - S</v>
       </c>
       <c r="C96" t="str">
-        <v>TOO-GANGTA-095</v>
+        <v>TOO-GANGTAYLATQD</v>
       </c>
       <c r="D96" t="str">
         <v/>
@@ -7540,7 +7540,7 @@
         <v>Găng tay Latex trắng - M</v>
       </c>
       <c r="C97" t="str">
-        <v>TOO-GANGTA-096</v>
+        <v>TOO-GANGTAYLATXC</v>
       </c>
       <c r="D97" t="str">
         <v/>
@@ -7614,7 +7614,7 @@
         <v>Chà chân 2 mặt</v>
       </c>
       <c r="C98" t="str">
-        <v>TOO-CHACHA-097</v>
+        <v>TOO-CHACHAN2MAHP</v>
       </c>
       <c r="D98" t="str">
         <v/>
@@ -7688,7 +7688,7 @@
         <v>Nước rửa cọ 120ml</v>
       </c>
       <c r="C99" t="str">
-        <v>HOA-NUOCRU-098</v>
+        <v>HOA-NUOCRUACO1FN</v>
       </c>
       <c r="D99" t="str">
         <v/>
@@ -7762,7 +7762,7 @@
         <v>Bào gầm</v>
       </c>
       <c r="C100" t="str">
-        <v>DAU-BAOGAM-099</v>
+        <v>DAU-BAOGAMQK</v>
       </c>
       <c r="D100" t="str">
         <v/>
@@ -7836,7 +7836,7 @@
         <v>Gel đính đá</v>
       </c>
       <c r="C101" t="str">
-        <v>HOA-GELDIN-100</v>
+        <v>HOA-GELDINHDAVQ</v>
       </c>
       <c r="D101" t="str">
         <v/>
@@ -7910,7 +7910,7 @@
         <v>BNS keo</v>
       </c>
       <c r="C102" t="str">
-        <v>HOA-BNSKEO-101</v>
+        <v>HOA-BNSKEOQK</v>
       </c>
       <c r="D102" t="str">
         <v/>
@@ -7984,7 +7984,7 @@
         <v>15ml top coat tím loãng</v>
       </c>
       <c r="C103" t="str">
-        <v>TOP-15MLTO-102</v>
+        <v>TOP-15MLTOPCOAYI</v>
       </c>
       <c r="D103" t="str">
         <v/>
@@ -8058,7 +8058,7 @@
         <v>Tip Trong Vuông XXL - Lẻ</v>
       </c>
       <c r="C104" t="str">
-        <v>TIP-TIPTRO-103</v>
+        <v>TIP-TIPTRONGVUFU</v>
       </c>
       <c r="D104" t="str">
         <v/>
@@ -8132,7 +8132,7 @@
         <v>Chổi phủi bàn</v>
       </c>
       <c r="C105" t="str">
-        <v>TOO-CHOIPH-104</v>
+        <v>TOO-CHOIPHUIBADO</v>
       </c>
       <c r="D105" t="str">
         <v/>
@@ -8206,7 +8206,7 @@
         <v>Spa tablets 2gal 4000 viên</v>
       </c>
       <c r="C106" t="str">
-        <v>HOA-SPATAB-105</v>
+        <v>HOA-SPATABLETSOY</v>
       </c>
       <c r="D106" t="str">
         <v/>
@@ -8280,7 +8280,7 @@
         <v>Nhũ đường</v>
       </c>
       <c r="C107" t="str">
-        <v>DES-NHUDUO-106</v>
+        <v>DES-NHUDUONGHY</v>
       </c>
       <c r="D107" t="str">
         <v/>
@@ -8354,7 +8354,7 @@
         <v>Bút quan tài sz18</v>
       </c>
       <c r="C108" t="str">
-        <v>BUT-BUTQUA-107</v>
+        <v>BUT-BUTQUANTAIBL</v>
       </c>
       <c r="D108" t="str">
         <v/>
@@ -8428,7 +8428,7 @@
         <v>Bút gel - vuông 10</v>
       </c>
       <c r="C109" t="str">
-        <v>BUT-BUTGEL-108</v>
+        <v>BUT-BUTGELVUONXO</v>
       </c>
       <c r="D109" t="str">
         <v/>
@@ -8502,7 +8502,7 @@
         <v>Súng bào korea</v>
       </c>
       <c r="C110" t="str">
-        <v>DOD-SUNGBA-109</v>
+        <v>DOD-SUNGBAOKORES</v>
       </c>
       <c r="D110" t="str">
         <v/>
@@ -8576,7 +8576,7 @@
         <v>XC</v>
       </c>
       <c r="C111" t="str">
-        <v>DAU-XC-110</v>
+        <v>DAU-XCNE</v>
       </c>
       <c r="D111" t="str">
         <v/>
@@ -8650,7 +8650,7 @@
         <v>Bao ngón cái 500c</v>
       </c>
       <c r="C112" t="str">
-        <v>TOO-BAONGO-111</v>
+        <v>TOO-BAONGONCAIVT</v>
       </c>
       <c r="D112" t="str">
         <v/>
@@ -8724,7 +8724,7 @@
         <v>Top coat 500ml</v>
       </c>
       <c r="C113" t="str">
-        <v>TOP-TOPCOA-112</v>
+        <v>TOP-TOPCOAT500ZG</v>
       </c>
       <c r="D113" t="str">
         <v/>
@@ -8798,7 +8798,7 @@
         <v>Chrome trắng gương 1g</v>
       </c>
       <c r="C114" t="str">
-        <v>DES-CHROME-113</v>
+        <v>DES-CHROMETRANWE</v>
       </c>
       <c r="D114" t="str">
         <v/>
@@ -8872,7 +8872,7 @@
         <v>Top matte 250ml</v>
       </c>
       <c r="C115" t="str">
-        <v>HOA-TOPMAT-114</v>
+        <v>HOA-TOPMATTE25HB</v>
       </c>
       <c r="D115" t="str">
         <v/>
@@ -8946,7 +8946,7 @@
         <v>Chà chân 1 lần 400c</v>
       </c>
       <c r="C116" t="str">
-        <v>TOO-CHACHA-115</v>
+        <v>TOO-CHACHAN1LAHS</v>
       </c>
       <c r="D116" t="str">
         <v/>
@@ -9020,7 +9020,7 @@
         <v>Bào mịn Diamond - M</v>
       </c>
       <c r="C117" t="str">
-        <v>DAU-BAOMIN-116</v>
+        <v>DAU-BAOMINDIAMWD</v>
       </c>
       <c r="D117" t="str">
         <v/>
@@ -9094,7 +9094,7 @@
         <v>Mịn Fusion - C</v>
       </c>
       <c r="C118" t="str">
-        <v>DAU-MINFUS-117</v>
+        <v>DAU-MINFUSIONCXM</v>
       </c>
       <c r="D118" t="str">
         <v/>
@@ -9168,7 +9168,7 @@
         <v>Mịn Fusion - F</v>
       </c>
       <c r="C119" t="str">
-        <v>DAU-MINFUS-118</v>
+        <v>DAU-MINFUSIONFCG</v>
       </c>
       <c r="D119" t="str">
         <v/>
@@ -9242,7 +9242,7 @@
         <v>3XC răng thẳng</v>
       </c>
       <c r="C120" t="str">
-        <v>DAU-3XCRAN-119</v>
+        <v>DAU-3XCRANGTHAWO</v>
       </c>
       <c r="D120" t="str">
         <v/>
@@ -9316,7 +9316,7 @@
         <v>4XC răng thẳng</v>
       </c>
       <c r="C121" t="str">
-        <v>DAU-4XCRAN-120</v>
+        <v>DAU-4XCRANGTHACX</v>
       </c>
       <c r="D121" t="str">
         <v/>
@@ -9390,7 +9390,7 @@
         <v>Trục nhám rẻ</v>
       </c>
       <c r="C122" t="str">
-        <v>DAU-TRUCNH-121</v>
+        <v>DAU-TRUCNHAMREOB</v>
       </c>
       <c r="D122" t="str">
         <v/>
@@ -9464,7 +9464,7 @@
         <v>Bút cán gỗ sz18</v>
       </c>
       <c r="C123" t="str">
-        <v>BUT-BUTCAN-122</v>
+        <v>BUT-BUTCANGOSZFO</v>
       </c>
       <c r="D123" t="str">
         <v/>
@@ -9538,7 +9538,7 @@
         <v>Chrome liquid - ngọc trai</v>
       </c>
       <c r="C124" t="str">
-        <v>DES-CHROME-123</v>
+        <v>DES-CHROMELIQUUW</v>
       </c>
       <c r="D124" t="str">
         <v/>
@@ -9612,7 +9612,7 @@
         <v>Base coat 250ml</v>
       </c>
       <c r="C125" t="str">
-        <v>HOA-BASECO-124</v>
+        <v>HOA-BASECOAT25XF</v>
       </c>
       <c r="D125" t="str">
         <v/>
@@ -9686,7 +9686,7 @@
         <v>Top loang - Blooming gel 15ml</v>
       </c>
       <c r="C126" t="str">
-        <v>HOA-TOPLOA-125</v>
+        <v>HOA-TOPLOANGBLZC</v>
       </c>
       <c r="D126" t="str">
         <v/>
@@ -9760,7 +9760,7 @@
         <v>5in1 Pedicure kit xanh</v>
       </c>
       <c r="C127" t="str">
-        <v>TOO-5IN1PE-126</v>
+        <v>TOO-5IN1PEDICULJ</v>
       </c>
       <c r="D127" t="str">
         <v/>
@@ -9834,7 +9834,7 @@
         <v>Buffer đen cam 3 mặt</v>
       </c>
       <c r="C128" t="str">
-        <v>TOO-BUFFER-127</v>
+        <v>TOO-BUFFERDENCPY</v>
       </c>
       <c r="D128" t="str">
         <v/>
@@ -9908,7 +9908,7 @@
         <v>Tip ballerina - lẻ</v>
       </c>
       <c r="C129" t="str">
-        <v>TIP-TIPBAL-128</v>
+        <v>TIP-TIPBALLERIZY</v>
       </c>
       <c r="D129" t="str">
         <v/>
@@ -9982,7 +9982,7 @@
         <v>Kim tuyến DL10-18</v>
       </c>
       <c r="C130" t="str">
-        <v>DES-KIMTUY-129</v>
+        <v>DES-KIMTUYENDLHR</v>
       </c>
       <c r="D130" t="str">
         <v/>
@@ -10056,7 +10056,7 @@
         <v>Kim tuyến DL01-09</v>
       </c>
       <c r="C131" t="str">
-        <v>DES-KIMTUY-130</v>
+        <v>DES-KIMTUYENDLGT</v>
       </c>
       <c r="D131" t="str">
         <v/>
@@ -10130,7 +10130,7 @@
         <v>Kim tuyến sáng 23g DL01-09</v>
       </c>
       <c r="C132" t="str">
-        <v>DES-KIMTUY-131</v>
+        <v>DES-KIMTUYENSASC</v>
       </c>
       <c r="D132" t="str">
         <v/>
@@ -10204,7 +10204,7 @@
         <v>Cốc liquid</v>
       </c>
       <c r="C133" t="str">
-        <v>TOO-COCLIQ-132</v>
+        <v>TOO-COCLIQUIDOV</v>
       </c>
       <c r="D133" t="str">
         <v/>
@@ -10278,7 +10278,7 @@
         <v>XXS - Đầu tròn ULTRA</v>
       </c>
       <c r="C134" t="str">
-        <v>DAU-XXSDAU-133</v>
+        <v>DAU-XXSDAUTRONTF</v>
       </c>
       <c r="D134" t="str">
         <v/>
@@ -10352,7 +10352,7 @@
         <v>Bào viên đạn</v>
       </c>
       <c r="C135" t="str">
-        <v>DAU-BAOVIE-134</v>
+        <v>DAU-BAOVIENDANWH</v>
       </c>
       <c r="D135" t="str">
         <v/>
@@ -10426,7 +10426,7 @@
         <v>4XC Đầu tròn ULTRA</v>
       </c>
       <c r="C136" t="str">
-        <v>DAU-4XCDAU-135</v>
+        <v>DAU-4XCDAUTRONXM</v>
       </c>
       <c r="D136" t="str">
         <v/>
@@ -10500,7 +10500,7 @@
         <v>Cán dao cạo chân - đen</v>
       </c>
       <c r="C137" t="str">
-        <v>TOO-CANDAO-136</v>
+        <v>TOO-CANDAOCAOCII</v>
       </c>
       <c r="D137" t="str">
         <v/>
@@ -10574,7 +10574,7 @@
         <v>Nhũ đường - T</v>
       </c>
       <c r="C138" t="str">
-        <v>DES-NHUDUO-137</v>
+        <v>DES-NHUDUONGTAX</v>
       </c>
       <c r="D138" t="str">
         <v/>
@@ -10648,7 +10648,7 @@
         <v>Kem mềm da</v>
       </c>
       <c r="C139" t="str">
-        <v>HOA-KEMMEM-138</v>
+        <v>HOA-KEMMEMDACC</v>
       </c>
       <c r="D139" t="str">
         <v/>
@@ -10722,7 +10722,7 @@
         <v>Liquid mango</v>
       </c>
       <c r="C140" t="str">
-        <v>HOA-LIQUID-139</v>
+        <v>HOA-LIQUIDMANGZH</v>
       </c>
       <c r="D140" t="str">
         <v/>
@@ -10796,7 +10796,7 @@
         <v>Vỏ nhám Mini - 100c</v>
       </c>
       <c r="C141" t="str">
-        <v>TOO-VONHAM-140</v>
+        <v>TOO-VONHAMMINIQJ</v>
       </c>
       <c r="D141" t="str">
         <v/>
@@ -10870,7 +10870,7 @@
         <v>Vỏ nhám Mini - 1000c</v>
       </c>
       <c r="C142" t="str">
-        <v>TOO-VONHAM-141</v>
+        <v>TOO-VONHAMMINIZU</v>
       </c>
       <c r="D142" t="str">
         <v/>
@@ -10944,7 +10944,7 @@
         <v>Vỏ nhám trắng ⌗150 - M</v>
       </c>
       <c r="C143" t="str">
-        <v>TOO-VONHAM-142</v>
+        <v>TOO-VONHAMTRANBY</v>
       </c>
       <c r="D143" t="str">
         <v/>
@@ -11018,7 +11018,7 @@
         <v>Súng bào máy tím</v>
       </c>
       <c r="C144" t="str">
-        <v>DOD-SUNGBA-143</v>
+        <v>DOD-SUNGBAOMAYJA</v>
       </c>
       <c r="D144" t="str">
         <v/>
@@ -11092,7 +11092,7 @@
         <v>Vòng bi dưới máy tím - to</v>
       </c>
       <c r="C145" t="str">
-        <v>DOD-VONGBI-144</v>
+        <v>DOD-VONGBIDUOIMF</v>
       </c>
       <c r="D145" t="str">
         <v/>
@@ -11166,7 +11166,7 @@
         <v>Vòng bi dưới máy tím - nhỏ</v>
       </c>
       <c r="C146" t="str">
-        <v>DOD-VONGBI-145</v>
+        <v>DOD-VONGBIDUOIIP</v>
       </c>
       <c r="D146" t="str">
         <v/>
@@ -11240,7 +11240,7 @@
         <v>Bột - Natural white</v>
       </c>
       <c r="C147" t="str">
-        <v>BOT-BOTNAT-146</v>
+        <v>BOT-BOTNATURALIB</v>
       </c>
       <c r="D147" t="str">
         <v/>
@@ -11314,7 +11314,7 @@
         <v>Xô Gel Scrub - Mint 23KG</v>
       </c>
       <c r="C148" t="str">
-        <v>HOA-XOGELS-147</v>
+        <v>HOA-XOGELSCRUBMD</v>
       </c>
       <c r="D148" t="str">
         <v/>
@@ -11388,7 +11388,7 @@
         <v>Cuticle Oil - Pineapple 1gal</v>
       </c>
       <c r="C149" t="str">
-        <v>HOA-CUTICL-148</v>
+        <v>HOA-CUTICLEOILGS</v>
       </c>
       <c r="D149" t="str">
         <v/>
@@ -11462,7 +11462,7 @@
         <v>Top coat tím Medium 500ml</v>
       </c>
       <c r="C150" t="str">
-        <v>TOP-TOPCOA-149</v>
+        <v>TOP-TOPCOATTIMDK</v>
       </c>
       <c r="D150" t="str">
         <v/>
@@ -11536,7 +11536,7 @@
         <v>Top coat tím Medium 15ml</v>
       </c>
       <c r="C151" t="str">
-        <v>TOP-TOPCOA-150</v>
+        <v>TOP-TOPCOATTIMZO</v>
       </c>
       <c r="D151" t="str">
         <v/>
@@ -11610,7 +11610,7 @@
         <v>Color Acrylic powder 2oz</v>
       </c>
       <c r="C152" t="str">
-        <v>BOT-COLORA-151</v>
+        <v>BOT-COLORACRYLPO</v>
       </c>
       <c r="D152" t="str">
         <v/>
@@ -11684,7 +11684,7 @@
         <v>Tay bào Trắng Korea</v>
       </c>
       <c r="C153" t="str">
-        <v>DOD-TAYBAO-152</v>
+        <v>DOD-TAYBAOTRANVA</v>
       </c>
       <c r="D153" t="str">
         <v/>
@@ -11758,7 +11758,7 @@
         <v>Súng tay bào Trắng Korea</v>
       </c>
       <c r="C154" t="str">
-        <v>DOD-SUNGTA-153</v>
+        <v>DOD-SUNGTAYBAOGI</v>
       </c>
       <c r="D154" t="str">
         <v/>
@@ -11832,7 +11832,7 @@
         <v>Máy bào Korea Trắng</v>
       </c>
       <c r="C155" t="str">
-        <v>DOD-MAYBAO-154</v>
+        <v>DOD-MAYBAOKOREQX</v>
       </c>
       <c r="D155" t="str">
         <v/>
@@ -11906,7 +11906,7 @@
         <v>Típ làm mẫu 20 màu 10 bảng/set</v>
       </c>
       <c r="C156" t="str">
-        <v>TOO-TIPLAM-155</v>
+        <v>TOO-TIPLAMMAU2YW</v>
       </c>
       <c r="D156" t="str">
         <v/>
@@ -11980,7 +11980,7 @@
         <v>Tay cầm bấm móng inox</v>
       </c>
       <c r="C157" t="str">
-        <v>TOO-TAYCAM-156</v>
+        <v>TOO-TAYCAMBAMMCI</v>
       </c>
       <c r="D157" t="str">
         <v/>
@@ -12054,7 +12054,7 @@
         <v>Dũa nhỏ Precision 100/100</v>
       </c>
       <c r="C158" t="str">
-        <v>DUA-DUANHO-157</v>
+        <v>DUA-DUANHOPRECRY</v>
       </c>
       <c r="D158" t="str">
         <v/>
@@ -12128,7 +12128,7 @@
         <v>Tips natur ballerina ngắn</v>
       </c>
       <c r="C159" t="str">
-        <v>TIP-TIPSNA-158</v>
+        <v>TIP-TIPSNATURBPA</v>
       </c>
       <c r="D159" t="str">
         <v/>
@@ -12202,7 +12202,7 @@
         <v>Lõi súng G5</v>
       </c>
       <c r="C160" t="str">
-        <v>DOD-LOISUN-159</v>
+        <v>DOD-LOISUNGG5EQ</v>
       </c>
       <c r="D160" t="str">
         <v/>
@@ -12276,7 +12276,7 @@
         <v>Dây tay máy tím 3 chân</v>
       </c>
       <c r="C161" t="str">
-        <v>DOD-DAYTAY-160</v>
+        <v>DOD-DAYTAYMAYTSY</v>
       </c>
       <c r="D161" t="str">
         <v/>
@@ -12350,7 +12350,7 @@
         <v>Bột - Intense Pink</v>
       </c>
       <c r="C162" t="str">
-        <v>BOT-BOTINT-161</v>
+        <v>BOT-BOTINTENSECQ</v>
       </c>
       <c r="D162" t="str">
         <v/>
@@ -12424,7 +12424,7 @@
         <v>Bút đắp hoa 3D 2 đầu</v>
       </c>
       <c r="C163" t="str">
-        <v>BUT-BUTDAP-162</v>
+        <v>BUT-BUTDAPHOA3DF</v>
       </c>
       <c r="D163" t="str">
         <v/>
@@ -12498,7 +12498,7 @@
         <v>Bút đắp bột Davie sz16</v>
       </c>
       <c r="C164" t="str">
-        <v>BUT-BUTDAP-163</v>
+        <v>BUT-BUTDAPBOTDUA</v>
       </c>
       <c r="D164" t="str">
         <v/>
@@ -12572,7 +12572,7 @@
         <v>Chổi rắc nhũ</v>
       </c>
       <c r="C165" t="str">
-        <v>BUT-CHOIRA-164</v>
+        <v>BUT-CHOIRACNHUEA</v>
       </c>
       <c r="D165" t="str">
         <v/>
@@ -12646,7 +12646,7 @@
         <v>Bút vẽ cọ</v>
       </c>
       <c r="C166" t="str">
-        <v>BUT-BUTVEC-165</v>
+        <v>BUT-BUTVECOIJ</v>
       </c>
       <c r="D166" t="str">
         <v/>
@@ -12720,7 +12720,7 @@
         <v>Bút vẽ hoa cúc</v>
       </c>
       <c r="C167" t="str">
-        <v>BUT-BUTVEH-166</v>
+        <v>BUT-BUTVEHOACUUC</v>
       </c>
       <c r="D167" t="str">
         <v/>
@@ -12794,7 +12794,7 @@
         <v>Dây cắm O japan</v>
       </c>
       <c r="C168" t="str">
-        <v>DOD-DAYCAM-167</v>
+        <v>DOD-DAYCAMOJAPUB</v>
       </c>
       <c r="D168" t="str">
         <v/>
@@ -12868,7 +12868,7 @@
         <v>Mịn thông XF</v>
       </c>
       <c r="C169" t="str">
-        <v>DAU-MINTHO-168</v>
+        <v>DAU-MINTHONGXFCV</v>
       </c>
       <c r="D169" t="str">
         <v/>
@@ -12942,7 +12942,7 @@
         <v>5in1 Phá volcano 4XC</v>
       </c>
       <c r="C170" t="str">
-        <v>DAU-5IN1PH-169</v>
+        <v>DAU-5IN1PHAVOLHJ</v>
       </c>
       <c r="D170" t="str">
         <v/>
@@ -13016,7 +13016,7 @@
         <v>5XC</v>
       </c>
       <c r="C171" t="str">
-        <v>DAU-5XC-170</v>
+        <v>DAU-5XCVQ</v>
       </c>
       <c r="D171" t="str">
         <v/>
@@ -13090,7 +13090,7 @@
         <v>XXS đầu vác</v>
       </c>
       <c r="C172" t="str">
-        <v>DAU-XXSDAU-171</v>
+        <v>DAU-XXSDAUVACRL</v>
       </c>
       <c r="D172" t="str">
         <v/>
@@ -13164,7 +13164,7 @@
         <v>Biển google review</v>
       </c>
       <c r="C173" t="str">
-        <v>TOO-BIENGO-172</v>
+        <v>TOO-BIENGOOGLEEL</v>
       </c>
       <c r="D173" t="str">
         <v/>
@@ -13238,7 +13238,7 @@
         <v>Trục nhám Mini</v>
       </c>
       <c r="C174" t="str">
-        <v>TOO-TRUCNH-173</v>
+        <v>TOO-TRUCNHAMMIDJ</v>
       </c>
       <c r="D174" t="str">
         <v/>
@@ -13312,7 +13312,7 @@
         <v>Bút gel - vuông 6</v>
       </c>
       <c r="C175" t="str">
-        <v>BUT-BUTGEL-174</v>
+        <v>BUT-BUTGELVUONZV</v>
       </c>
       <c r="D175" t="str">
         <v/>
@@ -13386,7 +13386,7 @@
         <v>Bút gel quét mầu - vuông 8</v>
       </c>
       <c r="C176" t="str">
-        <v>BUT-BUTGEL-175</v>
+        <v>BUT-BUTGELQUETMT</v>
       </c>
       <c r="D176" t="str">
         <v/>
@@ -13460,7 +13460,7 @@
         <v>Keo DNS Pro 1s</v>
       </c>
       <c r="C177" t="str">
-        <v>HOA-KEODNS-176</v>
+        <v>HOA-KEODNSPRO1IH</v>
       </c>
       <c r="D177" t="str">
         <v/>
@@ -13534,7 +13534,7 @@
         <v>Ultraschall reiniger 5L</v>
       </c>
       <c r="C178" t="str">
-        <v>HOA-ULTRAS-177</v>
+        <v>HOA-ULTRASCHALOH</v>
       </c>
       <c r="D178" t="str">
         <v/>
@@ -13608,7 +13608,7 @@
         <v>Kìm Nghĩa D555</v>
       </c>
       <c r="C179" t="str">
-        <v>TOO-KIMNGH-178</v>
+        <v>TOO-KIMNGHIAD5UL</v>
       </c>
       <c r="D179" t="str">
         <v/>
@@ -13682,7 +13682,7 @@
         <v>50ml - Gel đắp IBD PINK</v>
       </c>
       <c r="C180" t="str">
-        <v>GEL-50MLGE-179</v>
+        <v>GEL-50MLGELDAPZX</v>
       </c>
       <c r="D180" t="str">
         <v/>
@@ -13756,7 +13756,7 @@
         <v>Chrome base coat 15ml</v>
       </c>
       <c r="C181" t="str">
-        <v>TOP-CHROME-180</v>
+        <v>TOP-CHROMEBASERM</v>
       </c>
       <c r="D181" t="str">
         <v/>
@@ -13830,7 +13830,7 @@
         <v>Nam châm Mắt mèo thường</v>
       </c>
       <c r="C182" t="str">
-        <v>TOO-NAMCHA-181</v>
+        <v>TOO-NAMCHAMMATNV</v>
       </c>
       <c r="D182" t="str">
         <v/>
@@ -13904,7 +13904,7 @@
         <v>Chrome ngọc trai 1g</v>
       </c>
       <c r="C183" t="str">
-        <v>DES-CHROME-182</v>
+        <v>DES-CHROMENGOCYV</v>
       </c>
       <c r="D183" t="str">
         <v/>
@@ -13978,7 +13978,7 @@
         <v>Nhũ đường D hũ 50gram</v>
       </c>
       <c r="C184" t="str">
-        <v>DES-NHUDUO-183</v>
+        <v>DES-NHUDUONGDHPO</v>
       </c>
       <c r="D184" t="str">
         <v/>
@@ -14052,7 +14052,7 @@
         <v>15ml top coat tím đặc</v>
       </c>
       <c r="C185" t="str">
-        <v>TOP-15MLTO-184</v>
+        <v>TOP-15MLTOPCOADM</v>
       </c>
       <c r="D185" t="str">
         <v/>
@@ -14126,7 +14126,7 @@
         <v>Khẩu trang y tế</v>
       </c>
       <c r="C186" t="str">
-        <v>TOO-KHAUTR-185</v>
+        <v>TOO-KHAUTRANGYZH</v>
       </c>
       <c r="D186" t="str">
         <v/>
@@ -14200,7 +14200,7 @@
         <v>Bào nâng gầm</v>
       </c>
       <c r="C187" t="str">
-        <v>DAU-BAONAN-186</v>
+        <v>DAU-BAONANGGAMRV</v>
       </c>
       <c r="D187" t="str">
         <v/>
@@ -14274,7 +14274,7 @@
         <v>4XC - Đầu tròn v2</v>
       </c>
       <c r="C188" t="str">
-        <v>DAU-4XCDAU-187</v>
+        <v>DAU-4XCDAUTRONGO</v>
       </c>
       <c r="D188" t="str">
         <v/>
@@ -14348,7 +14348,7 @@
         <v>3in1 Mịn C - dài</v>
       </c>
       <c r="C189" t="str">
-        <v>DAU-3IN1MI-188</v>
+        <v>DAU-3IN1MINCDAYW</v>
       </c>
       <c r="D189" t="str">
         <v/>
@@ -14422,7 +14422,7 @@
         <v>Bút đắp bột - kim cương - sz18</v>
       </c>
       <c r="C190" t="str">
-        <v>BUT-BUTDAP-189</v>
+        <v>BUT-BUTDAPBOTKQM</v>
       </c>
       <c r="D190" t="str">
         <v/>
@@ -14496,7 +14496,7 @@
         <v>Nhám đỏ manicure</v>
       </c>
       <c r="C191" t="str">
-        <v>TOO-NHAMDO-190</v>
+        <v>TOO-NHAMDOMANIUR</v>
       </c>
       <c r="D191" t="str">
         <v/>
@@ -14570,7 +14570,7 @@
         <v>Máy bào Marathon 3 bạc</v>
       </c>
       <c r="C192" t="str">
-        <v>DOD-MAYBAO-191</v>
+        <v>DOD-MAYBAOMARAPX</v>
       </c>
       <c r="D192" t="str">
         <v/>
@@ -14644,7 +14644,7 @@
         <v>Dây cắm 3 châm Korea</v>
       </c>
       <c r="C193" t="str">
-        <v>DOD-DAYCAM-192</v>
+        <v>DOD-DAYCAM3CHAYM</v>
       </c>
       <c r="D193" t="str">
         <v/>
@@ -14718,7 +14718,7 @@
         <v>Đèn bàn LED đen</v>
       </c>
       <c r="C194" t="str">
-        <v>DOD-DENBAN-193</v>
+        <v>DOD-DENBANLEDDPX</v>
       </c>
       <c r="D194" t="str">
         <v/>
@@ -14792,7 +14792,7 @@
         <v>Cốc nắp vặn liquid</v>
       </c>
       <c r="C195" t="str">
-        <v>TOO-COCNAP-194</v>
+        <v>TOO-COCNAPVANLPK</v>
       </c>
       <c r="D195" t="str">
         <v/>
@@ -14866,7 +14866,7 @@
         <v>Set lọ inox đựng bột liquid</v>
       </c>
       <c r="C196" t="str">
-        <v>TOO-SETLOI-195</v>
+        <v>TOO-SETLOINOXDXP</v>
       </c>
       <c r="D196" t="str">
         <v/>
@@ -14940,7 +14940,7 @@
         <v>Kê bàn trưng bày</v>
       </c>
       <c r="C197" t="str">
-        <v>TOO-KEBANT-196</v>
+        <v>TOO-KEBANTRUNGYT</v>
       </c>
       <c r="D197" t="str">
         <v/>
@@ -15014,7 +15014,7 @@
         <v>Cốc đựng bột trái tim</v>
       </c>
       <c r="C198" t="str">
-        <v>TOO-COCDUN-197</v>
+        <v>TOO-COCDUNGBOTCG</v>
       </c>
       <c r="D198" t="str">
         <v/>
@@ -15088,7 +15088,7 @@
         <v>Hộp đựng dụng cụ</v>
       </c>
       <c r="C199" t="str">
-        <v>TOO-HOPDUN-198</v>
+        <v>TOO-HOPDUNGDUNWT</v>
       </c>
       <c r="D199" t="str">
         <v/>
@@ -15162,7 +15162,7 @@
         <v>Túi Đá nhỏ - bạc</v>
       </c>
       <c r="C200" t="str">
-        <v>DES-TUIDAN-199</v>
+        <v>DES-TUIDANHOBAXB</v>
       </c>
       <c r="D200" t="str">
         <v/>
@@ -15236,7 +15236,7 @@
         <v>Túi Đá nhỏ - 7 màu</v>
       </c>
       <c r="C201" t="str">
-        <v>DES-TUIDAN-200</v>
+        <v>DES-TUIDANHO7MKM</v>
       </c>
       <c r="D201" t="str">
         <v/>
@@ -15310,7 +15310,7 @@
         <v>Biển mẫu 50 NailArt</v>
       </c>
       <c r="C202" t="str">
-        <v>TOO-BIENMA-201</v>
+        <v>TOO-BIENMAU50NWR</v>
       </c>
       <c r="D202" t="str">
         <v/>
@@ -15384,7 +15384,7 @@
         <v>Típ cho bảng tip display</v>
       </c>
       <c r="C203" t="str">
-        <v>TOO-TIPCHO-202</v>
+        <v>TOO-TIPCHOBANGHG</v>
       </c>
       <c r="D203" t="str">
         <v/>
@@ -15458,7 +15458,7 @@
         <v>Quyển bảng màu marble 160</v>
       </c>
       <c r="C204" t="str">
-        <v>TOO-QUYENB-203</v>
+        <v>TOO-QUYENBANGMOB</v>
       </c>
       <c r="D204" t="str">
         <v/>
@@ -15532,7 +15532,7 @@
         <v>Quyển bảng màu gold 120</v>
       </c>
       <c r="C205" t="str">
-        <v>TOO-QUYENB-204</v>
+        <v>TOO-QUYENBANGMPV</v>
       </c>
       <c r="D205" t="str">
         <v/>
@@ -15606,7 +15606,7 @@
         <v>Quyển bảng màu gold 216</v>
       </c>
       <c r="C206" t="str">
-        <v>TOO-QUYENB-205</v>
+        <v>TOO-QUYENBANGMKU</v>
       </c>
       <c r="D206" t="str">
         <v/>
@@ -15680,7 +15680,7 @@
         <v>Quyển bảng màu to 300</v>
       </c>
       <c r="C207" t="str">
-        <v>TOO-QUYENB-206</v>
+        <v>TOO-QUYENBANGMRN</v>
       </c>
       <c r="D207" t="str">
         <v/>
@@ -15754,7 +15754,7 @@
         <v>Dũa nhỏ Precision 80/80</v>
       </c>
       <c r="C208" t="str">
-        <v>DUA-DUANHO-207</v>
+        <v>DUA-DUANHOPRECZP</v>
       </c>
       <c r="D208" t="str">
         <v/>
@@ -15828,7 +15828,7 @@
         <v>Đèn vòng bàn - trắng</v>
       </c>
       <c r="C209" t="str">
-        <v>DOD-DENVON-208</v>
+        <v>DOD-DENVONGBANFW</v>
       </c>
       <c r="D209" t="str">
         <v/>
@@ -15902,7 +15902,7 @@
         <v>Thùng Túi y tế 4000c</v>
       </c>
       <c r="C210" t="str">
-        <v>PED-THUNGT-209</v>
+        <v>PED-THUNGTUIYTPK</v>
       </c>
       <c r="D210" t="str">
         <v/>
@@ -15976,7 +15976,7 @@
         <v>Thùng Mini buffer 1500c</v>
       </c>
       <c r="C211" t="str">
-        <v>PED-THUNGM-210</v>
+        <v>PED-THUNGMINIBWK</v>
       </c>
       <c r="D211" t="str">
         <v/>
@@ -16050,7 +16050,7 @@
         <v>Thùng Dũa mini 5000c</v>
       </c>
       <c r="C212" t="str">
-        <v>PED-THUNGD-211</v>
+        <v>PED-THUNGDUAMIJL</v>
       </c>
       <c r="D212" t="str">
         <v/>
@@ -16124,7 +16124,7 @@
         <v>5XC - Titan Xanh</v>
       </c>
       <c r="C213" t="str">
-        <v>DAU-5XCTIT-212</v>
+        <v>DAU-5XCTITANXALD</v>
       </c>
       <c r="D213" t="str">
         <v/>
@@ -16198,7 +16198,7 @@
         <v>4XC - tròn nhỏ</v>
       </c>
       <c r="C214" t="str">
-        <v>DAU-4XCTRO-213</v>
+        <v>DAU-4XCTRONNHOND</v>
       </c>
       <c r="D214" t="str">
         <v/>
@@ -16272,7 +16272,7 @@
         <v>Bút quan tài sz16</v>
       </c>
       <c r="C215" t="str">
-        <v>BUT-BUTQUA-214</v>
+        <v>BUT-BUTQUANTAIRH</v>
       </c>
       <c r="D215" t="str">
         <v/>
@@ -16346,7 +16346,7 @@
         <v>Tay bào Korea bạc</v>
       </c>
       <c r="C216" t="str">
-        <v>DOD-TAYBAO-215</v>
+        <v>DOD-TAYBAOKORESA</v>
       </c>
       <c r="D216" t="str">
         <v/>
@@ -16420,7 +16420,7 @@
         <v>Chổi than japan</v>
       </c>
       <c r="C217" t="str">
-        <v>DOD-CHOITH-216</v>
+        <v>DOD-CHOITHANJABQ</v>
       </c>
       <c r="D217" t="str">
         <v/>
@@ -16494,7 +16494,7 @@
         <v>Mài da khoé</v>
       </c>
       <c r="C218" t="str">
-        <v>DAU-MAIDAK-217</v>
+        <v>DAU-MAIDAKHOEOT</v>
       </c>
       <c r="D218" t="str">
         <v/>
@@ -16568,7 +16568,7 @@
         <v>Bào mịn 3in1 - F</v>
       </c>
       <c r="C219" t="str">
-        <v>DAU-BAOMIN-218</v>
+        <v>DAU-BAOMIN3IN1JE</v>
       </c>
       <c r="D219" t="str">
         <v/>
@@ -16642,7 +16642,7 @@
         <v>Đèn cầu vòng đính đá</v>
       </c>
       <c r="C220" t="str">
-        <v>DOD-DENCAU-219</v>
+        <v>DOD-DENCAUVONGMI</v>
       </c>
       <c r="D220" t="str">
         <v/>
@@ -16716,7 +16716,7 @@
         <v>Chrome ngọc trai 7 màu</v>
       </c>
       <c r="C221" t="str">
-        <v>DES-CHROME-220</v>
+        <v>DES-CHROMENGOCWT</v>
       </c>
       <c r="D221" t="str">
         <v/>
@@ -16790,7 +16790,7 @@
         <v>Chả gọt chân Inox</v>
       </c>
       <c r="C222" t="str">
-        <v>TOO-CHAGOT-221</v>
+        <v>TOO-CHAGOTCHANKD</v>
       </c>
       <c r="D222" t="str">
         <v/>
@@ -16864,7 +16864,7 @@
         <v>Xốp kẹp chân 1000c</v>
       </c>
       <c r="C223" t="str">
-        <v>TOO-XOPKEP-222</v>
+        <v>TOO-XOPKEPCHANBR</v>
       </c>
       <c r="D223" t="str">
         <v/>
@@ -16938,7 +16938,7 @@
         <v>Kê tay da - ghi</v>
       </c>
       <c r="C224" t="str">
-        <v>TOO-KETAYD-223</v>
+        <v>TOO-KETAYDAGHIIY</v>
       </c>
       <c r="D224" t="str">
         <v/>
@@ -17012,7 +17012,7 @@
         <v>Bào gầm khoé nhọn</v>
       </c>
       <c r="C225" t="str">
-        <v>DAU-BAOGAM-224</v>
+        <v>DAU-BAOGAMKHOENC</v>
       </c>
       <c r="D225" t="str">
         <v/>
@@ -17086,7 +17086,7 @@
         <v>Bào gầm mỏng</v>
       </c>
       <c r="C226" t="str">
-        <v>DAU-BAOGAM-225</v>
+        <v>DAU-BAOGAMMONGQV</v>
       </c>
       <c r="D226" t="str">
         <v/>
@@ -17160,7 +17160,7 @@
         <v>Chổi đánh bóng</v>
       </c>
       <c r="C227" t="str">
-        <v>DAU-CHOIDA-226</v>
+        <v>DAU-CHOIDANHBOZV</v>
       </c>
       <c r="D227" t="str">
         <v/>
@@ -17234,7 +17234,7 @@
         <v>Bào gầm răng thẳng</v>
       </c>
       <c r="C228" t="str">
-        <v>DAU-BAOGAM-227</v>
+        <v>DAU-BAOGAMRANGOV</v>
       </c>
       <c r="D228" t="str">
         <v/>
@@ -17308,7 +17308,7 @@
         <v>5XC - đầu tròn</v>
       </c>
       <c r="C229" t="str">
-        <v>DAU-5XCDAU-228</v>
+        <v>DAU-5XCDAUTRONLD</v>
       </c>
       <c r="D229" t="str">
         <v/>
@@ -17382,7 +17382,7 @@
         <v>M - to tròn</v>
       </c>
       <c r="C230" t="str">
-        <v>DAU-MTOTRO-229</v>
+        <v>DAU-MTOTRONFL</v>
       </c>
       <c r="D230" t="str">
         <v/>
@@ -17456,7 +17456,7 @@
         <v>M - nhỏ</v>
       </c>
       <c r="C231" t="str">
-        <v>DAU-MNHO-230</v>
+        <v>DAU-MNHOAS</v>
       </c>
       <c r="D231" t="str">
         <v/>
@@ -17530,7 +17530,7 @@
         <v>Bào mịn 3in1 - M</v>
       </c>
       <c r="C232" t="str">
-        <v>DAU-BAOMIN-231</v>
+        <v>DAU-BAOMIN3IN1MU</v>
       </c>
       <c r="D232" t="str">
         <v/>
@@ -17604,7 +17604,7 @@
         <v>2XC Đầu vát</v>
       </c>
       <c r="C233" t="str">
-        <v>DAU-2XCDAU-232</v>
+        <v>DAU-2XCDAUVATJP</v>
       </c>
       <c r="D233" t="str">
         <v/>
@@ -17678,7 +17678,7 @@
         <v>Bột màu 56g Nude collection</v>
       </c>
       <c r="C234" t="str">
-        <v>BOT-BOTMAU-233</v>
+        <v>BOT-BOTMAU56GNNL</v>
       </c>
       <c r="D234" t="str">
         <v/>
@@ -17752,7 +17752,7 @@
         <v>Bột - VIP Natural Pink</v>
       </c>
       <c r="C235" t="str">
-        <v>BOT-BOTVIP-234</v>
+        <v>BOT-BOTVIPNATUDN</v>
       </c>
       <c r="D235" t="str">
         <v/>
@@ -17826,7 +17826,7 @@
         <v>Muối ngâm chân 5kg</v>
       </c>
       <c r="C236" t="str">
-        <v>PED-MUOING-235</v>
+        <v>PED-MUOINGAMCHRW</v>
       </c>
       <c r="D236" t="str">
         <v/>
@@ -17900,7 +17900,7 @@
         <v>Sugar Scrub - Orange 20kg</v>
       </c>
       <c r="C237" t="str">
-        <v>PED-SUGARS-236</v>
+        <v>PED-SUGARSCRUBHA</v>
       </c>
       <c r="D237" t="str">
         <v/>
@@ -17974,7 +17974,7 @@
         <v>Kem Mango Vera 600ml</v>
       </c>
       <c r="C238" t="str">
-        <v>HOA-KEMMAN-237</v>
+        <v>HOA-KEMMANGOVEHQ</v>
       </c>
       <c r="D238" t="str">
         <v/>
@@ -18048,7 +18048,7 @@
         <v>Sơn Enjoy super trắng</v>
       </c>
       <c r="C239" t="str">
-        <v>HOA-SONENJ-238</v>
+        <v>HOA-SONENJOYSURV</v>
       </c>
       <c r="D239" t="str">
         <v/>
@@ -18122,7 +18122,7 @@
         <v>Sơn Enjoy super đen</v>
       </c>
       <c r="C240" t="str">
-        <v>HOA-SONENJ-239</v>
+        <v>HOA-SONENJOYSUEZ</v>
       </c>
       <c r="D240" t="str">
         <v/>
@@ -18196,7 +18196,7 @@
         <v>Máy Ultraschall 2L</v>
       </c>
       <c r="C241" t="str">
-        <v>DOD-MAYULT-240</v>
+        <v>DOD-MAYULTRASCEN</v>
       </c>
       <c r="D241" t="str">
         <v/>
@@ -18270,7 +18270,7 @@
         <v>Nhũ đường A 50g</v>
       </c>
       <c r="C242" t="str">
-        <v>DES-NHUDUO-241</v>
+        <v>DES-NHUDUONGA5ST</v>
       </c>
       <c r="D242" t="str">
         <v/>
@@ -18344,7 +18344,7 @@
         <v>Nhũ đường B 50g</v>
       </c>
       <c r="C243" t="str">
-        <v>DES-NHUDUO-242</v>
+        <v>DES-NHUDUONGB5VJ</v>
       </c>
       <c r="D243" t="str">
         <v/>
@@ -18418,7 +18418,7 @@
         <v>Nhũ đường C 50g</v>
       </c>
       <c r="C244" t="str">
-        <v>DES-NHUDUO-243</v>
+        <v>DES-NHUDUONGC5ZP</v>
       </c>
       <c r="D244" t="str">
         <v/>
@@ -18492,7 +18492,7 @@
         <v>Nhũ bạc phản quang mịn R1 50g</v>
       </c>
       <c r="C245" t="str">
-        <v>DES-NHUBAC-244</v>
+        <v>DES-NHUBACPHANKW</v>
       </c>
       <c r="D245" t="str">
         <v/>
@@ -18566,7 +18566,7 @@
         <v>Bát nhựa ngâm tay</v>
       </c>
       <c r="C246" t="str">
-        <v>TOO-BATNHU-245</v>
+        <v>TOO-BATNHUANGAWW</v>
       </c>
       <c r="D246" t="str">
         <v/>
@@ -18640,7 +18640,7 @@
         <v>Bạc Foil 3g</v>
       </c>
       <c r="C247" t="str">
-        <v>DES-BACFOI-246</v>
+        <v>DES-BACFOIL3GQC</v>
       </c>
       <c r="D247" t="str">
         <v/>
@@ -18714,7 +18714,7 @@
         <v>Típ làm mẫu trong tròn 50c set</v>
       </c>
       <c r="C248" t="str">
-        <v>TOO-TIPLAM-247</v>
+        <v>TOO-TIPLAMMAUTXJ</v>
       </c>
       <c r="D248" t="str">
         <v/>
@@ -18788,7 +18788,7 @@
         <v>Nam châm mắt mèo - 5in1</v>
       </c>
       <c r="C249" t="str">
-        <v>TOO-NAMCHA-248</v>
+        <v>TOO-NAMCHAMMATQE</v>
       </c>
       <c r="D249" t="str">
         <v/>
@@ -18862,7 +18862,7 @@
         <v>Chổi vệ sinh đầu mài</v>
       </c>
       <c r="C250" t="str">
-        <v>TOO-CHOIVE-249</v>
+        <v>TOO-CHOIVESINHHE</v>
       </c>
       <c r="D250" t="str">
         <v/>
@@ -18936,7 +18936,7 @@
         <v>Chai sơn không 15ml</v>
       </c>
       <c r="C251" t="str">
-        <v>TOO-CHAISO-250</v>
+        <v>TOO-CHAISONKHOLF</v>
       </c>
       <c r="D251" t="str">
         <v/>
@@ -19010,7 +19010,7 @@
         <v>Chai primer không 15ml</v>
       </c>
       <c r="C252" t="str">
-        <v>TOO-CHAIPR-251</v>
+        <v>TOO-CHAIPRIMERSH</v>
       </c>
       <c r="D252" t="str">
         <v/>
@@ -19084,7 +19084,7 @@
         <v>Chai bond không 15ml</v>
       </c>
       <c r="C253" t="str">
-        <v>TOO-CHAIBO-252</v>
+        <v>TOO-CHAIBONDKHWS</v>
       </c>
       <c r="D253" t="str">
         <v/>
@@ -19158,7 +19158,7 @@
         <v>Hộp đựng phá tròn trắng</v>
       </c>
       <c r="C254" t="str">
-        <v>TOO-HOPDUN-253</v>
+        <v>TOO-HOPDUNGPHAFQ</v>
       </c>
       <c r="D254" t="str">
         <v/>
@@ -19232,7 +19232,7 @@
         <v>Bút cán gỗ sz16</v>
       </c>
       <c r="C255" t="str">
-        <v>BUT-BUTCAN-254</v>
+        <v>BUT-BUTCANGOSZCG</v>
       </c>
       <c r="D255" t="str">
         <v/>
@@ -19306,7 +19306,7 @@
         <v>Bút đắp bột - kim cương - sz16</v>
       </c>
       <c r="C256" t="str">
-        <v>BUT-BUTDAP-255</v>
+        <v>BUT-BUTDAPBOTKBW</v>
       </c>
       <c r="D256" t="str">
         <v/>
@@ -19380,7 +19380,7 @@
         <v>Tay bào trắng Korea SH20N</v>
       </c>
       <c r="C257" t="str">
-        <v>DOD-TAYBAO-256</v>
+        <v>DOD-TAYBAOTRANMV</v>
       </c>
       <c r="D257" t="str">
         <v/>
@@ -19454,7 +19454,7 @@
         <v>Vòng bi to Japan</v>
       </c>
       <c r="C258" t="str">
-        <v>TOO-VONGBI-257</v>
+        <v>TOO-VONGBITOJAOT</v>
       </c>
       <c r="D258" t="str">
         <v/>
@@ -19528,7 +19528,7 @@
         <v>Vòng bi nhỏ Japan</v>
       </c>
       <c r="C259" t="str">
-        <v>TOO-VONGBI-258</v>
+        <v>TOO-VONGBINHOJUN</v>
       </c>
       <c r="D259" t="str">
         <v/>
@@ -19602,7 +19602,7 @@
         <v>1KG - Gel đắp CLEAR</v>
       </c>
       <c r="C260" t="str">
-        <v>GEL-1KGGEL-259</v>
+        <v>GEL-1KGGELDAPCTU</v>
       </c>
       <c r="D260" t="str">
         <v/>
@@ -19676,7 +19676,7 @@
         <v>1KG - Gel đắp NATURAL PINK</v>
       </c>
       <c r="C261" t="str">
-        <v>GEL-1KGGEL-260</v>
+        <v>GEL-1KGGELDAPNJI</v>
       </c>
       <c r="D261" t="str">
         <v/>
@@ -19750,7 +19750,7 @@
         <v>1KG - Gel đắp MAKEUP ⌗1</v>
       </c>
       <c r="C262" t="str">
-        <v>GEL-1KGGEL-261</v>
+        <v>GEL-1KGGELDAPMHL</v>
       </c>
       <c r="D262" t="str">
         <v/>
@@ -19824,7 +19824,7 @@
         <v>1KG - Gel đắp MAKEUP ⌗2</v>
       </c>
       <c r="C263" t="str">
-        <v>GEL-1KGGEL-262</v>
+        <v>GEL-1KGGELDAPMZQ</v>
       </c>
       <c r="D263" t="str">
         <v/>
@@ -19898,7 +19898,7 @@
         <v>1KG - Gel đắp MAKEUP ⌗3</v>
       </c>
       <c r="C264" t="str">
-        <v>GEL-1KGGEL-263</v>
+        <v>GEL-1KGGELDAPMGO</v>
       </c>
       <c r="D264" t="str">
         <v/>
@@ -19972,7 +19972,7 @@
         <v>Cắt fen thường</v>
       </c>
       <c r="C265" t="str">
-        <v>TOO-CATFEN-264</v>
+        <v>TOO-CATFENTHUOVP</v>
       </c>
       <c r="D265" t="str">
         <v/>
@@ -20046,7 +20046,7 @@
         <v>Cắt fen sâu - E</v>
       </c>
       <c r="C266" t="str">
-        <v>TOO-CATFEN-265</v>
+        <v>TOO-CATFENSAUEJH</v>
       </c>
       <c r="D266" t="str">
         <v/>
@@ -20120,7 +20120,7 @@
         <v>XXS ULTRA</v>
       </c>
       <c r="C267" t="str">
-        <v>DAU-XXSULT-266</v>
+        <v>DAU-XXSULTRAEL</v>
       </c>
       <c r="D267" t="str">
         <v/>
@@ -20194,7 +20194,7 @@
         <v>XC - tròn</v>
       </c>
       <c r="C268" t="str">
-        <v>DAU-XCTRON-267</v>
+        <v>DAU-XCTRONEM</v>
       </c>
       <c r="D268" t="str">
         <v/>
@@ -20268,7 +20268,7 @@
         <v>Bào Mịn SM</v>
       </c>
       <c r="C269" t="str">
-        <v>DAU-BAOMIN-268</v>
+        <v>DAU-BAOMINSMID</v>
       </c>
       <c r="D269" t="str">
         <v/>
@@ -20342,7 +20342,7 @@
         <v>C - bào lửa</v>
       </c>
       <c r="C270" t="str">
-        <v>DAU-CBAOLU-269</v>
+        <v>DAU-CBAOLUAEQ</v>
       </c>
       <c r="D270" t="str">
         <v/>
@@ -20416,7 +20416,7 @@
         <v>Bào khoé tròn</v>
       </c>
       <c r="C271" t="str">
-        <v>DAU-BAOKHO-270</v>
+        <v>DAU-BAOKHOETROEL</v>
       </c>
       <c r="D271" t="str">
         <v/>
@@ -20490,7 +20490,7 @@
         <v>XXS Hoa cúc ULTRA</v>
       </c>
       <c r="C272" t="str">
-        <v>DAU-XXSHOA-271</v>
+        <v>DAU-XXSHOACUCUPL</v>
       </c>
       <c r="D272" t="str">
         <v/>
@@ -20564,7 +20564,7 @@
         <v>Base coat 15ml</v>
       </c>
       <c r="C273" t="str">
-        <v>HOA-BASECO-272</v>
+        <v>HOA-BASECOAT15LS</v>
       </c>
       <c r="D273" t="str">
         <v/>
@@ -20638,7 +20638,7 @@
         <v>Sơn màu SORAH 15ml</v>
       </c>
       <c r="C274" t="str">
-        <v>SON-SONMAU-273</v>
+        <v>SON-SONMAUSORABU</v>
       </c>
       <c r="D274" t="str">
         <v/>
@@ -20712,7 +20712,7 @@
         <v>SORAH 144 quyển màu</v>
       </c>
       <c r="C275" t="str">
-        <v>SON-SORAH1-274</v>
+        <v>SON-SORAH144QUST</v>
       </c>
       <c r="D275" t="str">
         <v/>
@@ -20786,7 +20786,7 @@
         <v>Máy hút bụi bàn di dộng</v>
       </c>
       <c r="C276" t="str">
-        <v>DOD-MAYHUT-275</v>
+        <v>DOD-MAYHUTBUIBFS</v>
       </c>
       <c r="D276" t="str">
         <v/>
@@ -20860,7 +20860,7 @@
         <v>Dũa Bông hoa đen 80/80</v>
       </c>
       <c r="C277" t="str">
-        <v>DUA-DUABON-276</v>
+        <v>DUA-DUABONGHOABE</v>
       </c>
       <c r="D277" t="str">
         <v/>
@@ -20934,7 +20934,7 @@
         <v>Tip Thẳng Straight jet - Lẻ (50c)</v>
       </c>
       <c r="C278" t="str">
-        <v>TIP-TIPTHA-277</v>
+        <v>TIP-TIPTHANGSTNX</v>
       </c>
       <c r="D278" t="str">
         <v/>
@@ -21008,7 +21008,7 @@
         <v>Vỏ nhám trắng ⌗150 (1000c)</v>
       </c>
       <c r="C279" t="str">
-        <v>TOO-VONHAM-278</v>
+        <v>TOO-VONHAMTRANRM</v>
       </c>
       <c r="D279" t="str">
         <v/>
@@ -21082,7 +21082,7 @@
         <v>Vỏ nhám trắng ⌗120 - C (1000c)</v>
       </c>
       <c r="C280" t="str">
-        <v>TOO-VONHAM-279</v>
+        <v>TOO-VONHAMTRANYR</v>
       </c>
       <c r="D280" t="str">
         <v/>
@@ -21156,7 +21156,7 @@
         <v>Vỏ nhám trắng ⌗180 - F (1000c)</v>
       </c>
       <c r="C281" t="str">
-        <v>TOO-VONHAM-280</v>
+        <v>TOO-VONHAMTRANBC</v>
       </c>
       <c r="D281" t="str">
         <v/>
@@ -21230,7 +21230,7 @@
         <v>Set Hộp đá - 7 màu</v>
       </c>
       <c r="C282" t="str">
-        <v>DES-SETHOP-281</v>
+        <v>DES-SETHOPDA7MEH</v>
       </c>
       <c r="D282" t="str">
         <v/>
@@ -21304,7 +21304,7 @@
         <v>Set Hộp đá - bạc</v>
       </c>
       <c r="C283" t="str">
-        <v>DES-SETHOP-282</v>
+        <v>DES-SETHOPDABAMS</v>
       </c>
       <c r="D283" t="str">
         <v/>
@@ -21378,7 +21378,7 @@
         <v>Set Hộp đá - vàng</v>
       </c>
       <c r="C284" t="str">
-        <v>DOD-SETHOP-283</v>
+        <v>DOD-SETHOPDAVAIF</v>
       </c>
       <c r="D284" t="str">
         <v/>
@@ -21452,7 +21452,7 @@
         <v>Set Hộp đá - chữ vàng</v>
       </c>
       <c r="C285" t="str">
-        <v>DES-SETHOP-284</v>
+        <v>DES-SETHOPDACHZT</v>
       </c>
       <c r="D285" t="str">
         <v/>
@@ -21526,7 +21526,7 @@
         <v>Kem Mango Vera 5kg</v>
       </c>
       <c r="C286" t="str">
-        <v>HOA-KEMMAN-285</v>
+        <v>HOA-KEMMANGOVEWU</v>
       </c>
       <c r="D286" t="str">
         <v/>
@@ -21600,7 +21600,7 @@
         <v>Callus Remover 5kg</v>
       </c>
       <c r="C287" t="str">
-        <v>PED-CALLUS-286</v>
+        <v>PED-CALLUSREMOME</v>
       </c>
       <c r="D287" t="str">
         <v/>
@@ -21674,7 +21674,7 @@
         <v>Xô Muối ngâm chân - mịn 23kg</v>
       </c>
       <c r="C288" t="str">
-        <v>HOA-XOMUOI-287</v>
+        <v>HOA-XOMUOINGAMQE</v>
       </c>
       <c r="D288" t="str">
         <v/>
@@ -21748,7 +21748,7 @@
         <v>Chổi quét bàn to</v>
       </c>
       <c r="C289" t="str">
-        <v>TOO-CHOIQU-288</v>
+        <v>TOO-CHOIQUETBARI</v>
       </c>
       <c r="D289" t="str">
         <v/>
@@ -21822,7 +21822,7 @@
         <v>4XC đầu vát</v>
       </c>
       <c r="C290" t="str">
-        <v>DAU-4XCDAU-289</v>
+        <v>DAU-4XCDAUVATTZ</v>
       </c>
       <c r="D290" t="str">
         <v/>
@@ -21896,7 +21896,7 @@
         <v>Kìm Nghĩa D01 Mũi 16</v>
       </c>
       <c r="C291" t="str">
-        <v>TOO-KIMNGH-290</v>
+        <v>TOO-KIMNGHIAD0HS</v>
       </c>
       <c r="D291" t="str">
         <v/>
@@ -21970,7 +21970,7 @@
         <v>Cây đẩy da</v>
       </c>
       <c r="C292" t="str">
-        <v>TOO-CAYDAY-291</v>
+        <v>TOO-CAYDAYDAUT</v>
       </c>
       <c r="D292" t="str">
         <v/>
@@ -22044,7 +22044,7 @@
         <v>Aceton 5L</v>
       </c>
       <c r="C293" t="str">
-        <v>HOA-ACETON-292</v>
+        <v>HOA-ACETON5LVY</v>
       </c>
       <c r="D293" t="str">
         <v/>
@@ -22118,7 +22118,7 @@
         <v>Cồn IPA70 5L</v>
       </c>
       <c r="C294" t="str">
-        <v>HOA-CONIPA-293</v>
+        <v>HOA-CONIPA705LWG</v>
       </c>
       <c r="D294" t="str">
         <v/>
@@ -22192,7 +22192,7 @@
         <v>Aceton 1L</v>
       </c>
       <c r="C295" t="str">
-        <v>HOA-ACETON-294</v>
+        <v>HOA-ACETON1LZP</v>
       </c>
       <c r="D295" t="str">
         <v/>
@@ -22266,7 +22266,7 @@
         <v>Típ thường 50c</v>
       </c>
       <c r="C296" t="str">
-        <v>TOO-TIPTHU-295</v>
+        <v>TOO-TIPTHUONG5VH</v>
       </c>
       <c r="D296" t="str">
         <v/>
@@ -22340,7 +22340,7 @@
         <v>Gel vẽ trắng French 50ml</v>
       </c>
       <c r="C297" t="str">
-        <v>DES-GELVET-296</v>
+        <v>DES-GELVETRANGJG</v>
       </c>
       <c r="D297" t="str">
         <v/>
@@ -22414,7 +22414,7 @@
         <v>Sơn màu Milky White 15ml</v>
       </c>
       <c r="C298" t="str">
-        <v>SON-SONMAU-297</v>
+        <v>SON-SONMAUMILKIQ</v>
       </c>
       <c r="D298" t="str">
         <v/>
@@ -22488,7 +22488,7 @@
         <v>Flash Disco Cat Eye 12 màu</v>
       </c>
       <c r="C299" t="str">
-        <v>SON-FLASHD-298</v>
+        <v>SON-FLASHDISCOTX</v>
       </c>
       <c r="D299" t="str">
         <v/>
@@ -22562,7 +22562,7 @@
         <v>Set Phấn nén làm ombre</v>
       </c>
       <c r="C300" t="str">
-        <v>DES-SETPHA-299</v>
+        <v>DES-SETPHANNENWH</v>
       </c>
       <c r="D300" t="str">
         <v/>
@@ -22636,7 +22636,7 @@
         <v>1KG - Gel đắp MILKY WHITE</v>
       </c>
       <c r="C301" t="str">
-        <v>GEL-1KGGEL-300</v>
+        <v>GEL-1KGGELDAPMCI</v>
       </c>
       <c r="D301" t="str">
         <v/>
@@ -22710,7 +22710,7 @@
         <v>1KG - Gel đắp MILKY PINK</v>
       </c>
       <c r="C302" t="str">
-        <v>GEL-1KGGEL-301</v>
+        <v>GEL-1KGGELDAPMZV</v>
       </c>
       <c r="D302" t="str">
         <v/>
@@ -22784,7 +22784,7 @@
         <v>M - to</v>
       </c>
       <c r="C303" t="str">
-        <v>DAU-MTO-302</v>
+        <v>DAU-MTODE</v>
       </c>
       <c r="D303" t="str">
         <v/>
@@ -22858,7 +22858,7 @@
         <v>Bào gầm 2.0</v>
       </c>
       <c r="C304" t="str">
-        <v>DAU-BAOGAM-303</v>
+        <v>DAU-BAOGAM20WL</v>
       </c>
       <c r="D304" t="str">
         <v/>
@@ -22932,7 +22932,7 @@
         <v>Phá Shellac</v>
       </c>
       <c r="C305" t="str">
-        <v>DAU-PHASHE-304</v>
+        <v>DAU-PHASHELLACVD</v>
       </c>
       <c r="D305" t="str">
         <v/>
@@ -23006,7 +23006,7 @@
         <v>Mịn thông M</v>
       </c>
       <c r="C306" t="str">
-        <v>DAU-MINTHO-305</v>
+        <v>DAU-MINTHONGMHO</v>
       </c>
       <c r="D306" t="str">
         <v/>
@@ -23080,7 +23080,7 @@
         <v>Top coat tím đặc 500ml</v>
       </c>
       <c r="C307" t="str">
-        <v>TOP-TOPCOA-306</v>
+        <v>TOP-TOPCOATTIMMF</v>
       </c>
       <c r="D307" t="str">
         <v/>
@@ -23154,7 +23154,7 @@
         <v>Liner gel vẽ Platinum</v>
       </c>
       <c r="C308" t="str">
-        <v>DES-LINERG-307</v>
+        <v>DES-LINERGELVEDL</v>
       </c>
       <c r="D308" t="str">
         <v/>
@@ -23228,7 +23228,7 @@
         <v>Đèn bàn trắng 18W</v>
       </c>
       <c r="C309" t="str">
-        <v>DOD-DENBAN-308</v>
+        <v>DOD-DENBANTRANGL</v>
       </c>
       <c r="D309" t="str">
         <v/>
@@ -23302,7 +23302,7 @@
         <v>Dũa mỏng nhỏ tròn 100/100</v>
       </c>
       <c r="C310" t="str">
-        <v>DUA-DUAMON-309</v>
+        <v>DUA-DUAMONGNHOWG</v>
       </c>
       <c r="D310" t="str">
         <v/>
@@ -23376,7 +23376,7 @@
         <v>Dũa mỏng nhỏ tròn 80/80</v>
       </c>
       <c r="C311" t="str">
-        <v>DUA-DUAMON-310</v>
+        <v>DUA-DUAMONGNHODK</v>
       </c>
       <c r="D311" t="str">
         <v/>
@@ -23450,7 +23450,7 @@
         <v>Bột - Clear Nhanh khô</v>
       </c>
       <c r="C312" t="str">
-        <v>BOT-BOTCLE-311</v>
+        <v>BOT-BOTCLEARNHUL</v>
       </c>
       <c r="D312" t="str">
         <v/>
@@ -23524,7 +23524,7 @@
         <v>Bột - Natural Dark Pink</v>
       </c>
       <c r="C313" t="str">
-        <v>BOT-BOTNAT-312</v>
+        <v>BOT-BOTNATURALSP</v>
       </c>
       <c r="D313" t="str">
         <v/>
@@ -23598,7 +23598,7 @@
         <v>Chrome base coat 250ml</v>
       </c>
       <c r="C314" t="str">
-        <v>HOA-CHROME-313</v>
+        <v>HOA-CHROMEBASEAK</v>
       </c>
       <c r="D314" t="str">
         <v/>
@@ -23672,7 +23672,7 @@
         <v>Giấy làm chân 50x70cm</v>
       </c>
       <c r="C315" t="str">
-        <v>TOO-GIAYLA-314</v>
+        <v>TOO-GIAYLAMCHAVJ</v>
       </c>
       <c r="D315" t="str">
         <v/>
@@ -23746,7 +23746,7 @@
         <v>Găng tay Nitril đen - S</v>
       </c>
       <c r="C316" t="str">
-        <v>TOO-GANGTA-315</v>
+        <v>TOO-GANGTAYNITNX</v>
       </c>
       <c r="D316" t="str">
         <v/>
@@ -23820,7 +23820,7 @@
         <v>Găng tay Nitril đen - M</v>
       </c>
       <c r="C317" t="str">
-        <v>TOO-GANGTA-316</v>
+        <v>TOO-GANGTAYNITDO</v>
       </c>
       <c r="D317" t="str">
         <v/>
@@ -23894,7 +23894,7 @@
         <v>Vỏ nhám tím ⌗150 - M</v>
       </c>
       <c r="C318" t="str">
-        <v>TOO-VONHAM-317</v>
+        <v>TOO-VONHAMTIM1NP</v>
       </c>
       <c r="D318" t="str">
         <v/>
@@ -23968,7 +23968,7 @@
         <v>Cốc đựng bột nhỏ</v>
       </c>
       <c r="C319" t="str">
-        <v>TOO-COCDUN-318</v>
+        <v>TOO-COCDUNGBOTMU</v>
       </c>
       <c r="D319" t="str">
         <v/>
@@ -24042,7 +24042,7 @@
         <v>Hộp đựng tip 0-10</v>
       </c>
       <c r="C320" t="str">
-        <v>TOO-HOPDUN-319</v>
+        <v>TOO-HOPDUNGTIPIH</v>
       </c>
       <c r="D320" t="str">
         <v/>
@@ -24116,7 +24116,7 @@
         <v>Típ làm mẫu 36 màu</v>
       </c>
       <c r="C321" t="str">
-        <v>TOO-TIPLAM-320</v>
+        <v>TOO-TIPLAMMAU3HQ</v>
       </c>
       <c r="D321" t="str">
         <v/>
@@ -24190,7 +24190,7 @@
         <v>Kê tay cao - hồng</v>
       </c>
       <c r="C322" t="str">
-        <v>TOO-KETAYC-321</v>
+        <v>TOO-KETAYCAOHODP</v>
       </c>
       <c r="D322" t="str">
         <v/>
@@ -24264,7 +24264,7 @@
         <v>Kê tay cao - be</v>
       </c>
       <c r="C323" t="str">
-        <v>TOO-KETAYC-322</v>
+        <v>TOO-KETAYCAOBEUH</v>
       </c>
       <c r="D323" t="str">
         <v/>
@@ -24338,7 +24338,7 @@
         <v>Kê tay cao - vàng</v>
       </c>
       <c r="C324" t="str">
-        <v>TOO-KETAYC-323</v>
+        <v>TOO-KETAYCAOVAEY</v>
       </c>
       <c r="D324" t="str">
         <v/>
@@ -24412,7 +24412,7 @@
         <v>Máy bào di động - đen</v>
       </c>
       <c r="C325" t="str">
-        <v>DOD-MAYBAO-324</v>
+        <v>DOD-MAYBAODIDOIK</v>
       </c>
       <c r="D325" t="str">
         <v/>
@@ -24486,7 +24486,7 @@
         <v>Đèn pin cầm tay v2</v>
       </c>
       <c r="C326" t="str">
-        <v>DOD-DENPIN-325</v>
+        <v>DOD-DENPINCAMTKW</v>
       </c>
       <c r="D326" t="str">
         <v/>
@@ -24560,7 +24560,7 @@
         <v>Pin thay đèn sạc</v>
       </c>
       <c r="C327" t="str">
-        <v>DOD-PINTHA-326</v>
+        <v>DOD-PINTHAYDENHS</v>
       </c>
       <c r="D327" t="str">
         <v/>
@@ -24634,7 +24634,7 @@
         <v>Tinh dầu trị nấm 15ml</v>
       </c>
       <c r="C328" t="str">
-        <v>HOA-TINHDA-327</v>
+        <v>HOA-TINHDAUTRIOV</v>
       </c>
       <c r="D328" t="str">
         <v/>
@@ -24708,7 +24708,7 @@
         <v>Nước cầm máu</v>
       </c>
       <c r="C329" t="str">
-        <v>HOA-NUOCCA-328</v>
+        <v>HOA-NUOCCAMMAUSZ</v>
       </c>
       <c r="D329" t="str">
         <v/>
@@ -24782,7 +24782,7 @@
         <v>Bột - Natural pink</v>
       </c>
       <c r="C330" t="str">
-        <v>BOT-BOTNAT-329</v>
+        <v>BOT-BOTNATURALQF</v>
       </c>
       <c r="D330" t="str">
         <v/>
@@ -24856,7 +24856,7 @@
         <v>Bột - Crystal clear</v>
       </c>
       <c r="C331" t="str">
-        <v>BOT-BOTCRY-330</v>
+        <v>BOT-BOTCRYSTALJX</v>
       </c>
       <c r="D331" t="str">
         <v/>
@@ -24930,7 +24930,7 @@
         <v>Liquid Mango J2000M C2</v>
       </c>
       <c r="C332" t="str">
-        <v>HOA-LIQUID-331</v>
+        <v>HOA-LIQUIDMANGOP</v>
       </c>
       <c r="D332" t="str">
         <v/>
@@ -25004,7 +25004,7 @@
         <v>Liquid J-2000 C2</v>
       </c>
       <c r="C333" t="str">
-        <v>HOA-LIQUID-332</v>
+        <v>HOA-LIQUIDJ200BT</v>
       </c>
       <c r="D333" t="str">
         <v/>
@@ -25078,7 +25078,7 @@
         <v>Liquid J2000 C0</v>
       </c>
       <c r="C334" t="str">
-        <v>HOA-LIQUID-333</v>
+        <v>HOA-LIQUIDJ200BJ</v>
       </c>
       <c r="D334" t="str">
         <v/>
@@ -25152,7 +25152,7 @@
         <v>Bột - Super white</v>
       </c>
       <c r="C335" t="str">
-        <v>BOT-BOTSUP-334</v>
+        <v>BOT-BOTSUPERWHGA</v>
       </c>
       <c r="D335" t="str">
         <v/>
@@ -25226,7 +25226,7 @@
         <v>Bột - Ombre white</v>
       </c>
       <c r="C336" t="str">
-        <v>BOT-BOTOMB-335</v>
+        <v>BOT-BOTOMBREWHCG</v>
       </c>
       <c r="D336" t="str">
         <v/>
@@ -25300,7 +25300,7 @@
         <v>Bột - Milky white</v>
       </c>
       <c r="C337" t="str">
-        <v>BOT-BOTMIL-336</v>
+        <v>BOT-BOTMILKYWHEM</v>
       </c>
       <c r="D337" t="str">
         <v/>
@@ -25374,7 +25374,7 @@
         <v>Bột - Makeup nude</v>
       </c>
       <c r="C338" t="str">
-        <v>BOT-BOTMAK-337</v>
+        <v>BOT-BOTMAKEUPNCD</v>
       </c>
       <c r="D338" t="str">
         <v/>
@@ -25448,7 +25448,7 @@
         <v>Bột - Makeup peach</v>
       </c>
       <c r="C339" t="str">
-        <v>BOT-BOTMAK-338</v>
+        <v>BOT-BOTMAKEUPPRS</v>
       </c>
       <c r="D339" t="str">
         <v/>
@@ -25522,7 +25522,7 @@
         <v>Bột - Makeup pink</v>
       </c>
       <c r="C340" t="str">
-        <v>BOT-BOTMAK-339</v>
+        <v>BOT-BOTMAKEUPPZN</v>
       </c>
       <c r="D340" t="str">
         <v/>
@@ -25596,7 +25596,7 @@
         <v>Bột - Clear</v>
       </c>
       <c r="C341" t="str">
-        <v>BOT-BOTCLE-340</v>
+        <v>BOT-BOTCLEARTL</v>
       </c>
       <c r="D341" t="str">
         <v/>
@@ -25670,7 +25670,7 @@
         <v>Primer 500ml</v>
       </c>
       <c r="C342" t="str">
-        <v>HOA-PRIMER-341</v>
+        <v>HOA-PRIMER500MYX</v>
       </c>
       <c r="D342" t="str">
         <v/>
@@ -25744,7 +25744,7 @@
         <v>Bond dry 500ml</v>
       </c>
       <c r="C343" t="str">
-        <v>HOA-BONDDR-342</v>
+        <v>HOA-BONDDRY500BP</v>
       </c>
       <c r="D343" t="str">
         <v/>
@@ -25818,7 +25818,7 @@
         <v>Tay bào Marathon bạc</v>
       </c>
       <c r="C344" t="str">
-        <v>DOD-TAYBAO-343</v>
+        <v>DOD-TAYBAOMARARO</v>
       </c>
       <c r="D344" t="str">
         <v/>
@@ -25892,7 +25892,7 @@
         <v>Cắt fen thường USA</v>
       </c>
       <c r="C345" t="str">
-        <v>TOO-CATFEN-344</v>
+        <v>TOO-CATFENTHUOID</v>
       </c>
       <c r="D345" t="str">
         <v/>
@@ -25966,7 +25966,7 @@
         <v>Cắt fen sâu USA</v>
       </c>
       <c r="C346" t="str">
-        <v>TOO-CATFEN-345</v>
+        <v>TOO-CATFENSAUUQJ</v>
       </c>
       <c r="D346" t="str">
         <v/>
@@ -26040,7 +26040,7 @@
         <v>Diamond Top Coat 500ml</v>
       </c>
       <c r="C347" t="str">
-        <v>TOP-DIAMON-346</v>
+        <v>TOP-DIAMONDTOPRZ</v>
       </c>
       <c r="D347" t="str">
         <v/>
@@ -26114,7 +26114,7 @@
         <v>Top coat tím Medium 1KG</v>
       </c>
       <c r="C348" t="str">
-        <v>TOP-TOPCOA-347</v>
+        <v>TOP-TOPCOATTIMMX</v>
       </c>
       <c r="D348" t="str">
         <v/>
@@ -26188,7 +26188,7 @@
         <v>1KG top coat tím loãng</v>
       </c>
       <c r="C349" t="str">
-        <v>TOP-1KGTOP-348</v>
+        <v>TOP-1KGTOPCOATUR</v>
       </c>
       <c r="D349" t="str">
         <v/>
@@ -26262,7 +26262,7 @@
         <v>Top coat tím loãng 500ml</v>
       </c>
       <c r="C350" t="str">
-        <v>TOP-TOPCOA-349</v>
+        <v>TOP-TOPCOATTIMBP</v>
       </c>
       <c r="D350" t="str">
         <v/>
@@ -26336,7 +26336,7 @@
         <v>Chà chân xanh 400c</v>
       </c>
       <c r="C351" t="str">
-        <v>TOO-CHACHA-350</v>
+        <v>TOO-CHACHANXANDL</v>
       </c>
       <c r="D351" t="str">
         <v/>
@@ -26410,7 +26410,7 @@
         <v>Buffer cam 3 mặt</v>
       </c>
       <c r="C352" t="str">
-        <v>TOO-BUFFER-351</v>
+        <v>TOO-BUFFERCAM3YF</v>
       </c>
       <c r="D352" t="str">
         <v/>
@@ -26484,7 +26484,7 @@
         <v>Buffer trắng 4 mặt</v>
       </c>
       <c r="C353" t="str">
-        <v>PED-BUFFER-352</v>
+        <v>PED-BUFFERTRANSO</v>
       </c>
       <c r="D353" t="str">
         <v/>
@@ -26558,7 +26558,7 @@
         <v>Tay bào máy tím</v>
       </c>
       <c r="C354" t="str">
-        <v>DOD-TAYBAO-353</v>
+        <v>DOD-TAYBAOMAYTLJ</v>
       </c>
       <c r="D354" t="str">
         <v/>
@@ -26632,7 +26632,7 @@
         <v>Tay bào máy G5</v>
       </c>
       <c r="C355" t="str">
-        <v>DOD-TAYBAO-354</v>
+        <v>DOD-TAYBAOMAYGGT</v>
       </c>
       <c r="D355" t="str">
         <v/>
@@ -26706,7 +26706,7 @@
         <v>Đèn LED 96W</v>
       </c>
       <c r="C356" t="str">
-        <v>DOD-DENLED-355</v>
+        <v>DOD-DENLED96WRH</v>
       </c>
       <c r="D356" t="str">
         <v/>
@@ -26780,7 +26780,7 @@
         <v>Đèn LED 48W</v>
       </c>
       <c r="C357" t="str">
-        <v>DOD-DENLED-356</v>
+        <v>DOD-DENLED48WYF</v>
       </c>
       <c r="D357" t="str">
         <v/>
@@ -26854,7 +26854,7 @@
         <v>Tip làm chân set</v>
       </c>
       <c r="C358" t="str">
-        <v>PED-TIPLAM-357</v>
+        <v>PED-TIPLAMCHANVL</v>
       </c>
       <c r="D358" t="str">
         <v/>
@@ -26928,7 +26928,7 @@
         <v>Chai sơn trống 15ml</v>
       </c>
       <c r="C359" t="str">
-        <v>TOO-CHAISO-358</v>
+        <v>TOO-CHAISONTROTL</v>
       </c>
       <c r="D359" t="str">
         <v/>
@@ -27002,7 +27002,7 @@
         <v>Túi ni lông xanh 800c</v>
       </c>
       <c r="C360" t="str">
-        <v>TOO-TUINIL-359</v>
+        <v>TOO-TUINILONGXGV</v>
       </c>
       <c r="D360" t="str">
         <v/>
@@ -27076,7 +27076,7 @@
         <v>5in1 Pedicure kit - 200c</v>
       </c>
       <c r="C361" t="str">
-        <v>TOO-5IN1PE-360</v>
+        <v>TOO-5IN1PEDICUHE</v>
       </c>
       <c r="D361" t="str">
         <v/>
@@ -27150,7 +27150,7 @@
         <v>Thùng Dũa mini 5000c</v>
       </c>
       <c r="C362" t="str">
-        <v>PED-THUNGD-361</v>
+        <v>PED-THUNGDUAMINR</v>
       </c>
       <c r="D362" t="str">
         <v/>
@@ -27224,7 +27224,7 @@
         <v>Thùng Slim buffer 500c</v>
       </c>
       <c r="C363" t="str">
-        <v>PED-THUNGS-362</v>
+        <v>PED-THUNGSLIMBPI</v>
       </c>
       <c r="D363" t="str">
         <v/>
@@ -27298,7 +27298,7 @@
         <v>Thùng que tăm 800c</v>
       </c>
       <c r="C364" t="str">
-        <v>PED-THUNGQ-363</v>
+        <v>PED-THUNGQUETAGD</v>
       </c>
       <c r="D364" t="str">
         <v/>
@@ -27372,7 +27372,7 @@
         <v>Đèn cầu vòng đính đá v2</v>
       </c>
       <c r="C365" t="str">
-        <v>DOD-DENCAU-364</v>
+        <v>DOD-DENCAUVONGSH</v>
       </c>
       <c r="D365" t="str">
         <v/>
@@ -27446,7 +27446,7 @@
         <v>Đèn cầu vòng trắng v2</v>
       </c>
       <c r="C366" t="str">
-        <v>DOD-DENCAU-365</v>
+        <v>DOD-DENCAUVONGQO</v>
       </c>
       <c r="D366" t="str">
         <v/>
@@ -27520,7 +27520,7 @@
         <v>4XC - Titan Xanh</v>
       </c>
       <c r="C367" t="str">
-        <v>DAU-4XCTIT-366</v>
+        <v>DAU-4XCTITANXAFA</v>
       </c>
       <c r="D367" t="str">
         <v/>
@@ -27594,7 +27594,7 @@
         <v>2XC Titan xanh</v>
       </c>
       <c r="C368" t="str">
-        <v>DAU-2XCTIT-367</v>
+        <v>DAU-2XCTITANXAHC</v>
       </c>
       <c r="D368" t="str">
         <v/>
@@ -27668,7 +27668,7 @@
         <v>Lọ không 500ml</v>
       </c>
       <c r="C369" t="str">
-        <v>TOO-LOKHON-368</v>
+        <v>TOO-LOKHONG500RE</v>
       </c>
       <c r="D369" t="str">
         <v/>
@@ -27742,7 +27742,7 @@
         <v>Cán dao cạo chân Inox</v>
       </c>
       <c r="C370" t="str">
-        <v>PED-CANDAO-369</v>
+        <v>PED-CANDAOCAOCJQ</v>
       </c>
       <c r="D370" t="str">
         <v/>
@@ -27816,7 +27816,7 @@
         <v>Dao lam Micra</v>
       </c>
       <c r="C371" t="str">
-        <v>PED-DAOLAM-370</v>
+        <v>PED-DAOLAMMICRTZ</v>
       </c>
       <c r="D371" t="str">
         <v/>
@@ -27890,7 +27890,7 @@
         <v>Dũa 80/80 Luxfile</v>
       </c>
       <c r="C372" t="str">
-        <v>DUA-DUA808-371</v>
+        <v>DUA-DUA8080LUXPI</v>
       </c>
       <c r="D372" t="str">
         <v/>
@@ -27964,7 +27964,7 @@
         <v>Dũa 100/100 Luxfile</v>
       </c>
       <c r="C373" t="str">
-        <v>DUA-DUA100-372</v>
+        <v>DUA-DUA100100LMY</v>
       </c>
       <c r="D373" t="str">
         <v/>
@@ -28038,7 +28038,7 @@
         <v>Máy sấy khô</v>
       </c>
       <c r="C374" t="str">
-        <v>DOD-MAYSAY-373</v>
+        <v>DOD-MAYSAYKHOOJ</v>
       </c>
       <c r="D374" t="str">
         <v/>
@@ -28112,7 +28112,7 @@
         <v>Tip fan 120 màu - tip nhọn trong</v>
       </c>
       <c r="C375" t="str">
-        <v>TOO-TIPFAN-374</v>
+        <v>TOO-TIPFAN120MCU</v>
       </c>
       <c r="D375" t="str">
         <v/>
@@ -28186,7 +28186,7 @@
         <v>Tip fan 120 màu - tip nhọn đục</v>
       </c>
       <c r="C376" t="str">
-        <v>TOO-TIPFAN-375</v>
+        <v>TOO-TIPFAN120MCV</v>
       </c>
       <c r="D376" t="str">
         <v/>
@@ -28260,7 +28260,7 @@
         <v>Tip fan 120 màu - tip natur trong</v>
       </c>
       <c r="C377" t="str">
-        <v>TOO-TIPFAN-376</v>
+        <v>TOO-TIPFAN120MZQ</v>
       </c>
       <c r="D377" t="str">
         <v/>
@@ -28334,7 +28334,7 @@
         <v>Tip fan 120 màu - tip natur đục</v>
       </c>
       <c r="C378" t="str">
-        <v>TOO-TIPFAN-377</v>
+        <v>TOO-TIPFAN120MKA</v>
       </c>
       <c r="D378" t="str">
         <v/>
@@ -28408,7 +28408,7 @@
         <v>Barbicide Concentrate 500ml</v>
       </c>
       <c r="C379" t="str">
-        <v>HOA-BARBIC-378</v>
+        <v>HOA-BARBICIDECML</v>
       </c>
       <c r="D379" t="str">
         <v/>
@@ -28482,7 +28482,7 @@
         <v>liner gel vẽ 12ml - trắng</v>
       </c>
       <c r="C380" t="str">
-        <v>HOA-LINERG-379</v>
+        <v>HOA-LINERGELVETR</v>
       </c>
       <c r="D380" t="str">
         <v/>
@@ -28556,7 +28556,7 @@
         <v>liner gel vẽ 12ml - đen</v>
       </c>
       <c r="C381" t="str">
-        <v>HOA-LINERG-380</v>
+        <v>HOA-LINERGELVEVJ</v>
       </c>
       <c r="D381" t="str">
         <v/>
@@ -28630,7 +28630,7 @@
         <v>4XC - Hoa cúc 2.0</v>
       </c>
       <c r="C382" t="str">
-        <v>DAU-4XCHOA-381</v>
+        <v>DAU-4XCHOACUC2VD</v>
       </c>
       <c r="D382" t="str">
         <v/>
@@ -28704,7 +28704,7 @@
         <v>Liner gel vẽ metallic - vàng 15ml</v>
       </c>
       <c r="C383" t="str">
-        <v>DES-LINERG-382</v>
+        <v>DES-LINERGELVEPS</v>
       </c>
       <c r="D383" t="str">
         <v/>
@@ -28778,7 +28778,7 @@
         <v>Liner gel vẽ metallic - bạc 15ml</v>
       </c>
       <c r="C384" t="str">
-        <v>DES-LINERG-383</v>
+        <v>DES-LINERGELVEOG</v>
       </c>
       <c r="D384" t="str">
         <v/>
@@ -28852,7 +28852,7 @@
         <v>1KG top coat tím đặc</v>
       </c>
       <c r="C385" t="str">
-        <v>TOP-1KGTOP-384</v>
+        <v>TOP-1KGTOPCOATSF</v>
       </c>
       <c r="D385" t="str">
         <v/>
@@ -28926,7 +28926,7 @@
         <v>4XC</v>
       </c>
       <c r="C386" t="str">
-        <v>DAU-4XC-385</v>
+        <v>DAU-4XCXR</v>
       </c>
       <c r="D386" t="str">
         <v/>
@@ -29000,7 +29000,7 @@
         <v>Trục nhám sắt v2</v>
       </c>
       <c r="C387" t="str">
-        <v>DAU-TRUCNH-386</v>
+        <v>DAU-TRUCNHAMSARG</v>
       </c>
       <c r="D387" t="str">
         <v/>
@@ -29074,7 +29074,7 @@
         <v>Trục nhám chắc chắn v2</v>
       </c>
       <c r="C388" t="str">
-        <v>DAU-TRUCNH-387</v>
+        <v>DAU-TRUCNHAMCHMJ</v>
       </c>
       <c r="D388" t="str">
         <v/>
@@ -29148,7 +29148,7 @@
         <v>Liquid J-2000 C7</v>
       </c>
       <c r="C389" t="str">
-        <v>HOA-LIQUID-388</v>
+        <v>HOA-LIQUIDJ200QO</v>
       </c>
       <c r="D389" t="str">
         <v/>
@@ -29222,7 +29222,7 @@
         <v>Bột - Ombre Pink I</v>
       </c>
       <c r="C390" t="str">
-        <v>BOT-BOTOMB-389</v>
+        <v>BOT-BOTOMBREPIMU</v>
       </c>
       <c r="D390" t="str">
         <v/>
@@ -29296,7 +29296,7 @@
         <v>Liquid EMA J-2 C7</v>
       </c>
       <c r="C391" t="str">
-        <v>HOA-LIQUID-390</v>
+        <v>HOA-LIQUIDEMAJFM</v>
       </c>
       <c r="D391" t="str">
         <v/>
@@ -29370,7 +29370,7 @@
         <v>4XC - Đầu tròn - Titan xanh</v>
       </c>
       <c r="C392" t="str">
-        <v>DAU-4XCDAU-391</v>
+        <v>DAU-4XCDAUTRONVL</v>
       </c>
       <c r="D392" t="str">
         <v/>
@@ -29444,7 +29444,7 @@
         <v>Motor tay máy tím</v>
       </c>
       <c r="C393" t="str">
-        <v>DOD-MOTORT-392</v>
+        <v>DOD-MOTORTAYMALT</v>
       </c>
       <c r="D393" t="str">
         <v/>
@@ -29518,7 +29518,7 @@
         <v>Super White 250ml</v>
       </c>
       <c r="C394" t="str">
-        <v>HOA-SUPERW-393</v>
+        <v>HOA-SUPERWHITEUB</v>
       </c>
       <c r="D394" t="str">
         <v/>
@@ -29592,7 +29592,7 @@
         <v>Super Black 250ml</v>
       </c>
       <c r="C395" t="str">
-        <v>HOA-SUPERB-394</v>
+        <v>HOA-SUPERBLACKQI</v>
       </c>
       <c r="D395" t="str">
         <v/>
@@ -29666,7 +29666,7 @@
         <v>Sugar Scrub - Orange 5kg</v>
       </c>
       <c r="C396" t="str">
-        <v>PED-SUGARS-395</v>
+        <v>PED-SUGARSCRUBVX</v>
       </c>
       <c r="D396" t="str">
         <v/>
@@ -29740,7 +29740,7 @@
         <v>Gel Scrub - Mint 5KG</v>
       </c>
       <c r="C397" t="str">
-        <v>HOA-GELSCR-396</v>
+        <v>HOA-GELSCRUBMILB</v>
       </c>
       <c r="D397" t="str">
         <v/>
@@ -29814,7 +29814,7 @@
         <v>Diamond Top Coat 1L</v>
       </c>
       <c r="C398" t="str">
-        <v>TOP-DIAMON-397</v>
+        <v>TOP-DIAMONDTOPWI</v>
       </c>
       <c r="D398" t="str">
         <v/>
@@ -29888,7 +29888,7 @@
         <v>Cốc đựng bột tròn</v>
       </c>
       <c r="C399" t="str">
-        <v>TOO-COCDUN-398</v>
+        <v>TOO-COCDUNGBOTAP</v>
       </c>
       <c r="D399" t="str">
         <v/>
@@ -29962,7 +29962,7 @@
         <v>Hũ đựng gel 50ml</v>
       </c>
       <c r="C400" t="str">
-        <v>TOO-HUDUNG-399</v>
+        <v>TOO-HUDUNGGEL5QN</v>
       </c>
       <c r="D400" t="str">
         <v/>
@@ -30036,7 +30036,7 @@
         <v>Hũ đựng gel 30ml</v>
       </c>
       <c r="C401" t="str">
-        <v>TOO-HUDUNG-400</v>
+        <v>TOO-HUDUNGGEL3XN</v>
       </c>
       <c r="D401" t="str">
         <v/>
@@ -30110,7 +30110,7 @@
         <v>Chà chân vàng 400c</v>
       </c>
       <c r="C402" t="str">
-        <v>TOO-CHACHA-401</v>
+        <v>TOO-CHACHANVANOI</v>
       </c>
       <c r="D402" t="str">
         <v/>
@@ -30184,7 +30184,7 @@
         <v>Đèn sạc pin 90W</v>
       </c>
       <c r="C403" t="str">
-        <v>DOD-DENSAC-402</v>
+        <v>DOD-DENSACPIN9WJ</v>
       </c>
       <c r="D403" t="str">
         <v/>
@@ -30258,7 +30258,7 @@
         <v>Sửa chữa tay bào</v>
       </c>
       <c r="C404" t="str">
-        <v>DIC-SUACHU-403</v>
+        <v>DIC-SUACHUATAYHX</v>
       </c>
       <c r="D404" t="str">
         <v/>
@@ -30332,7 +30332,7 @@
         <v>4XC Đầu tròn v3</v>
       </c>
       <c r="C405" t="str">
-        <v>DAU-4XCDAU-404</v>
+        <v>DAU-4XCDAUTRONCT</v>
       </c>
       <c r="D405" t="str">
         <v/>
@@ -30406,7 +30406,7 @@
         <v>M vàng - to</v>
       </c>
       <c r="C406" t="str">
-        <v>DAU-MVANGT-405</v>
+        <v>DAU-MVANGTODZ</v>
       </c>
       <c r="D406" t="str">
         <v/>
@@ -30480,7 +30480,7 @@
         <v>Set Bột Neon dặm 24 màu</v>
       </c>
       <c r="C407" t="str">
-        <v>DES-SETBOT-406</v>
+        <v>DES-SETBOTNEONFV</v>
       </c>
       <c r="D407" t="str">
         <v/>
@@ -30554,7 +30554,7 @@
         <v>Set Bút Xốp dặm</v>
       </c>
       <c r="C408" t="str">
-        <v>DES-SETBUT-407</v>
+        <v>DES-SETBUTXOPDYD</v>
       </c>
       <c r="D408" t="str">
         <v/>
@@ -30628,7 +30628,7 @@
         <v>Thân máy Trắng Marathon</v>
       </c>
       <c r="C409" t="str">
-        <v>DOD-THANMA-408</v>
+        <v>DOD-THANMAYTRAAX</v>
       </c>
       <c r="D409" t="str">
         <v/>
@@ -30702,7 +30702,7 @@
         <v>Dây cắm 3 chân UP200</v>
       </c>
       <c r="C410" t="str">
-        <v>DOD-DAYCAM-409</v>
+        <v>DOD-DAYCAM3CHAMQ</v>
       </c>
       <c r="D410" t="str">
         <v/>
@@ -30776,7 +30776,7 @@
         <v>Set Sơn mắt mèo 10D 12 màu</v>
       </c>
       <c r="C411" t="str">
-        <v>SON-SETSON-410</v>
+        <v>SON-SETSONMATMAL</v>
       </c>
       <c r="D411" t="str">
         <v/>
@@ -30850,7 +30850,7 @@
         <v>Gel nặn 3D - Clear 50ml</v>
       </c>
       <c r="C412" t="str">
-        <v>DES-GELNAN-411</v>
+        <v>DES-GELNAN3DCLTQ</v>
       </c>
       <c r="D412" t="str">
         <v/>
@@ -30924,7 +30924,7 @@
         <v>Kê chân cao - đen vàng</v>
       </c>
       <c r="C413" t="str">
-        <v>TOO-KECHAN-412</v>
+        <v>TOO-KECHANCAODKW</v>
       </c>
       <c r="D413" t="str">
         <v/>
@@ -30998,7 +30998,7 @@
         <v>Kê chân cao - trắng vàng</v>
       </c>
       <c r="C414" t="str">
-        <v>TOO-KECHAN-413</v>
+        <v>TOO-KECHANCAOTZS</v>
       </c>
       <c r="D414" t="str">
         <v/>
@@ -31072,7 +31072,7 @@
         <v>Chổi quét bàn - Nhỏ</v>
       </c>
       <c r="C415" t="str">
-        <v>TOO-CHOIQU-414</v>
+        <v>TOO-CHOIQUETBARC</v>
       </c>
       <c r="D415" t="str">
         <v/>
@@ -31146,7 +31146,7 @@
         <v>Muối viên xô 4000 viên</v>
       </c>
       <c r="C416" t="str">
-        <v>PED-MUOIVI-415</v>
+        <v>PED-MUOIVIENXORB</v>
       </c>
       <c r="D416" t="str">
         <v/>
@@ -31220,7 +31220,7 @@
         <v>Moonlight Cat Eye 12 màu</v>
       </c>
       <c r="C417" t="str">
-        <v>SON-MOONLI-416</v>
+        <v>SON-MOONLIGHTCVO</v>
       </c>
       <c r="D417" t="str">
         <v/>
@@ -31294,7 +31294,7 @@
         <v>Gel thinner 30ml</v>
       </c>
       <c r="C418" t="str">
-        <v>HOA-GELTHI-417</v>
+        <v>HOA-GELTHINNERAS</v>
       </c>
       <c r="D418" t="str">
         <v/>
@@ -31368,7 +31368,7 @@
         <v>Diamond Top Coat 15ml</v>
       </c>
       <c r="C419" t="str">
-        <v>TOP-DIAMON-418</v>
+        <v>TOP-DIAMONDTOPAL</v>
       </c>
       <c r="D419" t="str">
         <v/>
@@ -31442,7 +31442,7 @@
         <v>Gel nặn 3D - trắng 15ml</v>
       </c>
       <c r="C420" t="str">
-        <v>HOA-GELNAN-419</v>
+        <v>HOA-GELNAN3DTRVK</v>
       </c>
       <c r="D420" t="str">
         <v/>
@@ -31516,7 +31516,7 @@
         <v>Sơn màu Milky White 250ml</v>
       </c>
       <c r="C421" t="str">
-        <v>SON-SONMAU-420</v>
+        <v>SON-SONMAUMILKRW</v>
       </c>
       <c r="D421" t="str">
         <v/>
@@ -31590,7 +31590,7 @@
         <v>Liquid EMA G3 C1 Blue</v>
       </c>
       <c r="C422" t="str">
-        <v>HOA-LIQUID-421</v>
+        <v>HOA-LIQUIDEMAGQT</v>
       </c>
       <c r="D422" t="str">
         <v/>
@@ -31664,7 +31664,7 @@
         <v>Xô Gel Scrub Orange - 20KG</v>
       </c>
       <c r="C423" t="str">
-        <v>PED-XOGELS-422</v>
+        <v>PED-XOGELSCRUBAI</v>
       </c>
       <c r="D423" t="str">
         <v/>
@@ -31738,7 +31738,7 @@
         <v>Vỏ nhám Mỹ ⌗150 (1000c)</v>
       </c>
       <c r="C424" t="str">
-        <v>TOO-VONHAM-423</v>
+        <v>TOO-VONHAMMY15ML</v>
       </c>
       <c r="D424" t="str">
         <v/>
@@ -31812,7 +31812,7 @@
         <v>Set 5c Bút Nặn Silicon</v>
       </c>
       <c r="C425" t="str">
-        <v>BUT-SET5CB-424</v>
+        <v>BUT-SET5CBUTNASH</v>
       </c>
       <c r="D425" t="str">
         <v/>
@@ -31886,7 +31886,7 @@
         <v>Dũa mỏng - To Vuông 80/80</v>
       </c>
       <c r="C426" t="str">
-        <v>DUA-DUAMON-425</v>
+        <v>DUA-DUAMONGTOVON</v>
       </c>
       <c r="D426" t="str">
         <v/>
@@ -31960,7 +31960,7 @@
         <v>Dũa mỏng - To Vuông 100/100</v>
       </c>
       <c r="C427" t="str">
-        <v>DUA-DUAMON-426</v>
+        <v>DUA-DUAMONGTOVHZ</v>
       </c>
       <c r="D427" t="str">
         <v/>
@@ -32034,7 +32034,7 @@
         <v>Tip Thẳng Natur Nhọn - Lẻ</v>
       </c>
       <c r="C428" t="str">
-        <v>TIP-TIPTHA-427</v>
+        <v>TIP-TIPTHANGNAHO</v>
       </c>
       <c r="D428" t="str">
         <v/>
@@ -32108,7 +32108,7 @@
         <v>Bình ngâm khử trùng dụng cụ</v>
       </c>
       <c r="C429" t="str">
-        <v>PED-BINHNG-428</v>
+        <v>PED-BINHNGAMKHBI</v>
       </c>
       <c r="D429" t="str">
         <v/>
@@ -32182,7 +32182,7 @@
         <v>Bút cán gỗ sz14</v>
       </c>
       <c r="C430" t="str">
-        <v>BUT-BUTCAN-429</v>
+        <v>BUT-BUTCANGOSZKF</v>
       </c>
       <c r="D430" t="str">
         <v/>
@@ -32256,7 +32256,7 @@
         <v>BL1 - Nhũ Đường Đen ánh trắng</v>
       </c>
       <c r="C431" t="str">
-        <v>DES-BL1NHU-430</v>
+        <v>DES-BL1NHUDUONGM</v>
       </c>
       <c r="D431" t="str">
         <v/>
@@ -32330,7 +32330,7 @@
         <v>BL2 - Nhũ Đường Đen 7 màu</v>
       </c>
       <c r="C432" t="str">
-        <v>DES-BL2NHU-431</v>
+        <v>DES-BL2NHUDUONWR</v>
       </c>
       <c r="D432" t="str">
         <v/>
@@ -32404,7 +32404,7 @@
         <v>Liquid EMA Ít mùi</v>
       </c>
       <c r="C433" t="str">
-        <v>HOA-LIQUID-432</v>
+        <v>HOA-LIQUIDEMAISP</v>
       </c>
       <c r="D433" t="str">
         <v/>
@@ -32478,7 +32478,7 @@
         <v>Bịch Dũa mini 50c - Lẻ</v>
       </c>
       <c r="C434" t="str">
-        <v>PED-BICHDU-433</v>
+        <v>PED-BICHDUAMINHK</v>
       </c>
       <c r="D434" t="str">
         <v/>
@@ -32552,7 +32552,7 @@
         <v>Xốp kẹp chân 100c - Lẻ</v>
       </c>
       <c r="C435" t="str">
-        <v>PED-XOPKEP-434</v>
+        <v>PED-XOPKEPCHANQS</v>
       </c>
       <c r="D435" t="str">
         <v/>
@@ -32626,7 +32626,7 @@
         <v>Hộp túi y tế 100c - Lẻ</v>
       </c>
       <c r="C436" t="str">
-        <v>PED-HOPTUI-435</v>
+        <v>PED-HOPTUIYTE1DB</v>
       </c>
       <c r="D436" t="str">
         <v/>
@@ -32700,7 +32700,7 @@
         <v>Muối viên - Lọ Nhỏ 250c</v>
       </c>
       <c r="C437" t="str">
-        <v>PED-MUOIVI-436</v>
+        <v>PED-MUOIVIENLOWV</v>
       </c>
       <c r="D437" t="str">
         <v/>
@@ -32774,7 +32774,7 @@
         <v>Chai Bơm Cồn 200ml</v>
       </c>
       <c r="C438" t="str">
-        <v>TOO-CHAIBO-437</v>
+        <v>TOO-CHAIBOMCONNC</v>
       </c>
       <c r="D438" t="str">
         <v/>
@@ -32848,7 +32848,7 @@
         <v>Cán dao cạo chân P05</v>
       </c>
       <c r="C439" t="str">
-        <v>PED-CANDAO-438</v>
+        <v>PED-CANDAOCAOCZT</v>
       </c>
       <c r="D439" t="str">
         <v/>
@@ -32922,7 +32922,7 @@
         <v>Kệ Acrylic đựng bút</v>
       </c>
       <c r="C440" t="str">
-        <v>TOO-KEACRY-439</v>
+        <v>TOO-KEACRYLICDAX</v>
       </c>
       <c r="D440" t="str">
         <v/>
@@ -32996,7 +32996,7 @@
         <v>Bịch que tăm 100c - Lẻ</v>
       </c>
       <c r="C441" t="str">
-        <v>TOO-BICHQU-440</v>
+        <v>TOO-BICHQUETAMBK</v>
       </c>
       <c r="D441" t="str">
         <v/>
@@ -33070,7 +33070,7 @@
         <v>Marble Ink Set 12 màu</v>
       </c>
       <c r="C442" t="str">
-        <v>DES-MARBLE-441</v>
+        <v>DES-MARBLEINKSDQ</v>
       </c>
       <c r="D442" t="str">
         <v/>
@@ -33144,7 +33144,7 @@
         <v>Gel 6in1</v>
       </c>
       <c r="C443" t="str">
-        <v>TOP-GEL6IN-442</v>
+        <v>TOP-GEL6IN1AN</v>
       </c>
       <c r="D443" t="str">
         <v/>
@@ -33218,7 +33218,7 @@
         <v>Máy bào di động 45K</v>
       </c>
       <c r="C444" t="str">
-        <v>DOD-MAYBAO-443</v>
+        <v>DOD-MAYBAODIDOGW</v>
       </c>
       <c r="D444" t="str">
         <v/>
@@ -33292,7 +33292,7 @@
         <v>Gel vẽ Đen Hũ 50ml</v>
       </c>
       <c r="C445" t="str">
-        <v>HOA-GELVED-444</v>
+        <v>HOA-GELVEDENHULD</v>
       </c>
       <c r="D445" t="str">
         <v/>
@@ -33366,7 +33366,7 @@
         <v>5in1 pedicure kit cam</v>
       </c>
       <c r="C446" t="str">
-        <v>PED-5IN1PE-445</v>
+        <v>PED-5IN1PEDICUEY</v>
       </c>
       <c r="D446" t="str">
         <v/>
@@ -33440,7 +33440,7 @@
         <v>Lẻ - Jelly Spa 1 túi</v>
       </c>
       <c r="C447" t="str">
-        <v>PED-LEJELL-446</v>
+        <v>PED-LEJELLYSPACS</v>
       </c>
       <c r="D447" t="str">
         <v/>
@@ -33514,7 +33514,7 @@
         <v>Kê tay cao - màu đen - chân bạc</v>
       </c>
       <c r="C448" t="str">
-        <v>TOO-KETAYC-447</v>
+        <v>TOO-KETAYCAOMAKR</v>
       </c>
       <c r="D448" t="str">
         <v/>
@@ -33588,7 +33588,7 @@
         <v>Kê tay cao - màu trắng - chân bạc</v>
       </c>
       <c r="C449" t="str">
-        <v>TOO-KETAYC-448</v>
+        <v>TOO-KETAYCAOMAAC</v>
       </c>
       <c r="D449" t="str">
         <v/>
@@ -33662,7 +33662,7 @@
         <v>Đèn LED làm chân</v>
       </c>
       <c r="C450" t="str">
-        <v>DOD-DENLED-449</v>
+        <v>DOD-DENLEDLAMCGX</v>
       </c>
       <c r="D450" t="str">
         <v/>
@@ -33736,7 +33736,7 @@
         <v>Máy Khử trùng nhiệt độ</v>
       </c>
       <c r="C451" t="str">
-        <v>DOD-MAYKHU-450</v>
+        <v>DOD-MAYKHUTRUNZP</v>
       </c>
       <c r="D451" t="str">
         <v/>
@@ -33810,7 +33810,7 @@
         <v>Mịn thông XF</v>
       </c>
       <c r="C452" t="str">
-        <v>DAU-MINTHO-451</v>
+        <v>DAU-MINTHONGXFDA</v>
       </c>
       <c r="D452" t="str">
         <v/>
@@ -33884,7 +33884,7 @@
         <v>Kìm Bấm Móng - Đầu Thẳng</v>
       </c>
       <c r="C453" t="str">
-        <v>TOO-KIMBAM-452</v>
+        <v>TOO-KIMBAMMONGFS</v>
       </c>
       <c r="D453" t="str">
         <v/>
@@ -33958,7 +33958,7 @@
         <v>Imperial Top Coat - 15ml - thin</v>
       </c>
       <c r="C454" t="str">
-        <v>TOP-IMPERI-453</v>
+        <v>TOP-IMPERIALTOUV</v>
       </c>
       <c r="D454" t="str">
         <v/>
@@ -34032,7 +34032,7 @@
         <v>Imperial Top Coat - 15ml - thick</v>
       </c>
       <c r="C455" t="str">
-        <v>TOP-IMPERI-454</v>
+        <v>TOP-IMPERIALTOKO</v>
       </c>
       <c r="D455" t="str">
         <v/>
@@ -34106,7 +34106,7 @@
         <v>Imperial Top Coat - 500ml - thin</v>
       </c>
       <c r="C456" t="str">
-        <v>TOP-IMPERI-455</v>
+        <v>TOP-IMPERIALTOBX</v>
       </c>
       <c r="D456" t="str">
         <v/>
@@ -34180,7 +34180,7 @@
         <v>Imperial Top Coat - 1000ml - thin</v>
       </c>
       <c r="C457" t="str">
-        <v>TOP-IMPERI-456</v>
+        <v>TOP-IMPERIALTOJS</v>
       </c>
       <c r="D457" t="str">
         <v/>
@@ -34254,7 +34254,7 @@
         <v>Imperial Top Coat - 500ml - thick</v>
       </c>
       <c r="C458" t="str">
-        <v>TOP-IMPERI-457</v>
+        <v>TOP-IMPERIALTOOA</v>
       </c>
       <c r="D458" t="str">
         <v/>
@@ -34328,7 +34328,7 @@
         <v>Imperial Top Coat - 1000ml - thick</v>
       </c>
       <c r="C459" t="str">
-        <v>TOP-IMPERI-458</v>
+        <v>TOP-IMPERIALTOND</v>
       </c>
       <c r="D459" t="str">
         <v/>
@@ -34402,7 +34402,7 @@
         <v>Glaze Gel Polish Set 12 màu</v>
       </c>
       <c r="C460" t="str">
-        <v>SON-GLAZEG-459</v>
+        <v>SON-GLAZEGELPOEQ</v>
       </c>
       <c r="D460" t="str">
         <v/>
@@ -34476,7 +34476,7 @@
         <v>BIAB 15ml</v>
       </c>
       <c r="C461" t="str">
-        <v>GEL-BIAB15-460</v>
+        <v>GEL-BIAB15MLZK</v>
       </c>
       <c r="D461" t="str">
         <v/>
@@ -34550,7 +34550,7 @@
         <v>Cuticle Oil nắp nhọn 15ml</v>
       </c>
       <c r="C462" t="str">
-        <v>HOA-CUTICL-461</v>
+        <v>HOA-CUTICLEOILDE</v>
       </c>
       <c r="D462" t="str">
         <v/>
@@ -34624,7 +34624,7 @@
         <v>Liquid Professional</v>
       </c>
       <c r="C463" t="str">
-        <v>HOA-LIQUID-462</v>
+        <v>HOA-LIQUIDPROFOV</v>
       </c>
       <c r="D463" t="str">
         <v/>
@@ -34698,7 +34698,7 @@
         <v>Liquid Winter</v>
       </c>
       <c r="C464" t="str">
-        <v>HOA-LIQUID-463</v>
+        <v>HOA-LIQUIDWINTXY</v>
       </c>
       <c r="D464" t="str">
         <v/>
@@ -34772,7 +34772,7 @@
         <v>Cốc liquid mini</v>
       </c>
       <c r="C465" t="str">
-        <v>TOO-COCLIQ-464</v>
+        <v>TOO-COCLIQUIDMAL</v>
       </c>
       <c r="D465" t="str">
         <v/>
@@ -34846,7 +34846,7 @@
         <v>Dép làm chân 24c</v>
       </c>
       <c r="C466" t="str">
-        <v>PED-DEPLAM-465</v>
+        <v>PED-DEPLAMCHANXF</v>
       </c>
       <c r="D466" t="str">
         <v/>
@@ -34920,7 +34920,7 @@
         <v>Kem đẩy da 3.8L</v>
       </c>
       <c r="C467" t="str">
-        <v>PED-KEMDAY-466</v>
+        <v>PED-KEMDAYDA38CC</v>
       </c>
       <c r="D467" t="str">
         <v/>
@@ -34994,7 +34994,7 @@
         <v>Kem đẩy da 1L</v>
       </c>
       <c r="C468" t="str">
-        <v>PED-KEMDAY-467</v>
+        <v>PED-KEMDAYDA1LVQ</v>
       </c>
       <c r="D468" t="str">
         <v/>
@@ -35068,7 +35068,7 @@
         <v>Hộp Pedicure Bath Bombs 60c</v>
       </c>
       <c r="C469" t="str">
-        <v>PED-HOPPED-468</v>
+        <v>PED-HOPPEDICURWY</v>
       </c>
       <c r="D469" t="str">
         <v/>
@@ -35142,7 +35142,7 @@
         <v>Imperial Top Coat - 250ml - thick</v>
       </c>
       <c r="C470" t="str">
-        <v>TOP-IMPERI-469</v>
+        <v>TOP-IMPERIALTORE</v>
       </c>
       <c r="D470" t="str">
         <v/>
@@ -35216,7 +35216,7 @@
         <v>Imperial Top Coat - 250ml - thin</v>
       </c>
       <c r="C471" t="str">
-        <v>TOP-IMPERI-470</v>
+        <v>TOP-IMPERIALTOSF</v>
       </c>
       <c r="D471" t="str">
         <v/>
@@ -35290,7 +35290,7 @@
         <v>Dũa Luxfile 60/60</v>
       </c>
       <c r="C472" t="str">
-        <v>DUA-DUALUX-471</v>
+        <v>DUA-DUALUXFILEMI</v>
       </c>
       <c r="D472" t="str">
         <v/>
@@ -35364,7 +35364,7 @@
         <v>Túi ni lông trong</v>
       </c>
       <c r="C473" t="str">
-        <v>PED-TUINIL-472</v>
+        <v>PED-TUINILONGTSB</v>
       </c>
       <c r="D473" t="str">
         <v/>
@@ -35438,7 +35438,7 @@
         <v>Đèn nối mi</v>
       </c>
       <c r="C474" t="str">
-        <v>DOD-DENNOI-473</v>
+        <v>DOD-DENNOIMIMU</v>
       </c>
       <c r="D474" t="str">
         <v/>
@@ -35512,7 +35512,7 @@
         <v>Đèn bàn LED siêu sáng</v>
       </c>
       <c r="C475" t="str">
-        <v>DOD-DENBAN-474</v>
+        <v>DOD-DENBANLEDSIC</v>
       </c>
       <c r="D475" t="str">
         <v/>
@@ -35586,7 +35586,7 @@
         <v>Típ làm mẫu quyển màu nhọn</v>
       </c>
       <c r="C476" t="str">
-        <v>TIP-TIPLAM-475</v>
+        <v>TIP-TIPLAMMAUQQC</v>
       </c>
       <c r="D476" t="str">
         <v/>
@@ -35660,7 +35660,7 @@
         <v>Thùng Chà chân tím 400c</v>
       </c>
       <c r="C477" t="str">
-        <v>PED-THUNGC-476</v>
+        <v>PED-THUNGCHACHZL</v>
       </c>
       <c r="D477" t="str">
         <v/>
@@ -35734,7 +35734,7 @@
         <v>Kìm bấm móng L 777 Korea</v>
       </c>
       <c r="C478" t="str">
-        <v>TOO-KIMBAM-477</v>
+        <v>TOO-KIMBAMMONGRQ</v>
       </c>
       <c r="D478" t="str">
         <v/>
@@ -35808,7 +35808,7 @@
         <v>Tip trong thẳng clear</v>
       </c>
       <c r="C479" t="str">
-        <v>TIP-TIPTRO-478</v>
+        <v>TIP-TIPTRONGTHSG</v>
       </c>
       <c r="D479" t="str">
         <v/>
@@ -35882,7 +35882,7 @@
         <v>Tip thẳng vuông đục</v>
       </c>
       <c r="C480" t="str">
-        <v>TIP-TIPTHA-479</v>
+        <v>TIP-TIPTHANGVUOG</v>
       </c>
       <c r="D480" t="str">
         <v/>
@@ -35956,7 +35956,7 @@
         <v>Tip trong nhọn</v>
       </c>
       <c r="C481" t="str">
-        <v>TIP-TIPTRO-480</v>
+        <v>TIP-TIPTRONGNHMZ</v>
       </c>
       <c r="D481" t="str">
         <v/>
@@ -36030,7 +36030,7 @@
         <v>Kìm tháo đá</v>
       </c>
       <c r="C482" t="str">
-        <v>TOO-KIMTHA-481</v>
+        <v>TOO-KIMTHAODALQ</v>
       </c>
       <c r="D482" t="str">
         <v/>
@@ -36104,7 +36104,7 @@
         <v>Bút chấm bi vôi 2 đầu</v>
       </c>
       <c r="C483" t="str">
-        <v>BUT-BUTCHA-482</v>
+        <v>BUT-BUTCHAMBIVCE</v>
       </c>
       <c r="D483" t="str">
         <v/>
@@ -36178,7 +36178,7 @@
         <v>Bào Mịn 3in1 dài - F</v>
       </c>
       <c r="C484" t="str">
-        <v>DAU-BAOMIN-483</v>
+        <v>DAU-BAOMIN3IN1QL</v>
       </c>
       <c r="D484" t="str">
         <v/>
@@ -36252,7 +36252,7 @@
         <v>Bào Mịn Dài XXL 5in1 - F</v>
       </c>
       <c r="C485" t="str">
-        <v>DAU-BAOMIN-484</v>
+        <v>DAU-BAOMINDAIXNR</v>
       </c>
       <c r="D485" t="str">
         <v/>
@@ -36326,7 +36326,7 @@
         <v>Bào Mịn Diamond - Đẩy Khoé</v>
       </c>
       <c r="C486" t="str">
-        <v>DAU-BAOMIN-485</v>
+        <v>DAU-BAOMINDIAMLB</v>
       </c>
       <c r="D486" t="str">
         <v/>
@@ -36400,7 +36400,7 @@
         <v>Đèn Hybrid SORAH</v>
       </c>
       <c r="C487" t="str">
-        <v>DOD-DENHYB-486</v>
+        <v>DOD-DENHYBRIDSSR</v>
       </c>
       <c r="D487" t="str">
         <v/>
@@ -36474,7 +36474,7 @@
         <v>Hũ đựng nhũ</v>
       </c>
       <c r="C488" t="str">
-        <v>TOO-HUDUNG-487</v>
+        <v>TOO-HUDUNGNHUFE</v>
       </c>
       <c r="D488" t="str">
         <v/>
@@ -36548,7 +36548,7 @@
         <v>Gel đắp - 500ml - Clear</v>
       </c>
       <c r="C489" t="str">
-        <v>GEL-GELDAP-488</v>
+        <v>GEL-GELDAP500MWS</v>
       </c>
       <c r="D489" t="str">
         <v/>
@@ -36622,7 +36622,7 @@
         <v>Gel đắp - 500ml - Natural Pink</v>
       </c>
       <c r="C490" t="str">
-        <v>GEL-GELDAP-489</v>
+        <v>GEL-GELDAP500MZY</v>
       </c>
       <c r="D490" t="str">
         <v/>
@@ -36696,7 +36696,7 @@
         <v>Gel đắp - 500ml - Milky Pink</v>
       </c>
       <c r="C491" t="str">
-        <v>GEL-GELDAP-490</v>
+        <v>GEL-GELDAP500MHW</v>
       </c>
       <c r="D491" t="str">
         <v/>
@@ -36770,7 +36770,7 @@
         <v>Gel đắp - 500ml - Milky White</v>
       </c>
       <c r="C492" t="str">
-        <v>GEL-GELDAP-491</v>
+        <v>GEL-GELDAP500MBN</v>
       </c>
       <c r="D492" t="str">
         <v/>
@@ -36844,7 +36844,7 @@
         <v>Gel đắp - 500ml - Makeup 1</v>
       </c>
       <c r="C493" t="str">
-        <v>GEL-GELDAP-492</v>
+        <v>GEL-GELDAP500MAC</v>
       </c>
       <c r="D493" t="str">
         <v/>
@@ -36918,7 +36918,7 @@
         <v>Gel đắp - 500ml - Makeup 2</v>
       </c>
       <c r="C494" t="str">
-        <v>GEL-GELDAP-493</v>
+        <v>GEL-GELDAP500MKP</v>
       </c>
       <c r="D494" t="str">
         <v/>
@@ -36992,7 +36992,7 @@
         <v>Gel đắp - 500ml - Makeup 3</v>
       </c>
       <c r="C495" t="str">
-        <v>GEL-GELDAP-494</v>
+        <v>GEL-GELDAP500MFO</v>
       </c>
       <c r="D495" t="str">
         <v/>
@@ -37066,7 +37066,7 @@
         <v>Gel đắp - 50ml - Clear</v>
       </c>
       <c r="C496" t="str">
-        <v>GEL-GELDAP-495</v>
+        <v>GEL-GELDAP50MLDO</v>
       </c>
       <c r="D496" t="str">
         <v/>
@@ -37140,7 +37140,7 @@
         <v>Gel đắp - 50ml - Natural Pink</v>
       </c>
       <c r="C497" t="str">
-        <v>GEL-GELDAP-496</v>
+        <v>GEL-GELDAP50MLPL</v>
       </c>
       <c r="D497" t="str">
         <v/>
@@ -37214,7 +37214,7 @@
         <v>Gel đắp - 50ml - Milky Pink</v>
       </c>
       <c r="C498" t="str">
-        <v>GEL-GELDAP-497</v>
+        <v>GEL-GELDAP50MLUG</v>
       </c>
       <c r="D498" t="str">
         <v/>
@@ -37288,7 +37288,7 @@
         <v>Gel đắp - 50ml - Milky White</v>
       </c>
       <c r="C499" t="str">
-        <v>GEL-GELDAP-498</v>
+        <v>GEL-GELDAP50MLVH</v>
       </c>
       <c r="D499" t="str">
         <v/>
@@ -37362,7 +37362,7 @@
         <v>Gel đắp - 50ml - Makeup ⌗1</v>
       </c>
       <c r="C500" t="str">
-        <v>GEL-GELDAP-499</v>
+        <v>GEL-GELDAP50MLSM</v>
       </c>
       <c r="D500" t="str">
         <v/>
@@ -37436,7 +37436,7 @@
         <v>Gel đắp - 50ml - Makeup ⌗2</v>
       </c>
       <c r="C501" t="str">
-        <v>GEL-GELDAP-500</v>
+        <v>GEL-GELDAP50MLKR</v>
       </c>
       <c r="D501" t="str">
         <v/>
@@ -37510,7 +37510,7 @@
         <v>Gel đắp - 50ml - Makeup ⌗3</v>
       </c>
       <c r="C502" t="str">
-        <v>GEL-GELDAP-501</v>
+        <v>GEL-GELDAP50MLZG</v>
       </c>
       <c r="D502" t="str">
         <v/>
@@ -37584,7 +37584,7 @@
         <v>CND Shellac Base Coat</v>
       </c>
       <c r="C503" t="str">
-        <v>TOP-CNDSHE-502</v>
+        <v>TOP-CNDSHELLACQJ</v>
       </c>
       <c r="D503" t="str">
         <v/>
@@ -37658,7 +37658,7 @@
         <v>Cồn xanh 80 độ 5L</v>
       </c>
       <c r="C504" t="str">
-        <v>HOA-CONXAN-503</v>
+        <v>HOA-CONXANH80DWV</v>
       </c>
       <c r="D504" t="str">
         <v/>
@@ -37732,7 +37732,7 @@
         <v>Thùng 5in1 pedi kit tím (200c)</v>
       </c>
       <c r="C505" t="str">
-        <v>PED-THUNG5-504</v>
+        <v>PED-THUNG5IN1PQH</v>
       </c>
       <c r="D505" t="str">
         <v/>
@@ -37806,7 +37806,7 @@
         <v>Oil vị dứa 500ml</v>
       </c>
       <c r="C506" t="str">
-        <v>HOA-OILVID-505</v>
+        <v>HOA-OILVIDUA50IN</v>
       </c>
       <c r="D506" t="str">
         <v/>
@@ -37880,7 +37880,7 @@
         <v>Hộp Cuticle oil 48c</v>
       </c>
       <c r="C507" t="str">
-        <v>NOE-HOPCUT-506</v>
+        <v>NOE-HOPCUTICLEGP</v>
       </c>
       <c r="D507" t="str">
         <v/>
@@ -37954,7 +37954,7 @@
         <v>Cuticle oil Noel</v>
       </c>
       <c r="C508" t="str">
-        <v>NOE-CUTICL-507</v>
+        <v>NOE-CUTICLEOILBB</v>
       </c>
       <c r="D508" t="str">
         <v/>
@@ -38028,7 +38028,7 @@
         <v>Kem Hộp Đỏ 50ml</v>
       </c>
       <c r="C509" t="str">
-        <v>NOE-KEMHOP-508</v>
+        <v>NOE-KEMHOPDO50PK</v>
       </c>
       <c r="D509" t="str">
         <v/>
@@ -38102,7 +38102,7 @@
         <v>Hộp kem mango vera 72c</v>
       </c>
       <c r="C510" t="str">
-        <v>NOE-HOPKEM-509</v>
+        <v>NOE-HOPKEMMANGFR</v>
       </c>
       <c r="D510" t="str">
         <v/>
@@ -38176,7 +38176,7 @@
         <v>Dầu Massage - Aloe Vera 3.8L</v>
       </c>
       <c r="C511" t="str">
-        <v>PED-DAUMAS-510</v>
+        <v>PED-DAUMASSAGEDL</v>
       </c>
       <c r="D511" t="str">
         <v/>
@@ -38250,7 +38250,7 @@
         <v>Bột Ombre Nude I</v>
       </c>
       <c r="C512" t="str">
-        <v>BOT-BOTOMB-511</v>
+        <v>BOT-BOTOMBRENUFQ</v>
       </c>
       <c r="D512" t="str">
         <v/>
@@ -38324,7 +38324,7 @@
         <v>Bột - Ombre Pink II</v>
       </c>
       <c r="C513" t="str">
-        <v>BOT-BOTOMB-512</v>
+        <v>BOT-BOTOMBREPIRC</v>
       </c>
       <c r="D513" t="str">
         <v/>
@@ -38398,7 +38398,7 @@
         <v>Bào mịn Diamond thông</v>
       </c>
       <c r="C514" t="str">
-        <v>DAU-BAOMIN-513</v>
+        <v>DAU-BAOMINDIAMAN</v>
       </c>
       <c r="D514" t="str">
         <v/>
@@ -38472,7 +38472,7 @@
         <v>Chà chân Nano Glass</v>
       </c>
       <c r="C515" t="str">
-        <v>PED-CHACHA-514</v>
+        <v>PED-CHACHANNANPK</v>
       </c>
       <c r="D515" t="str">
         <v/>
@@ -38546,7 +38546,7 @@
         <v>Vòng bi tay trắng Korea 1260</v>
       </c>
       <c r="C516" t="str">
-        <v>DOD-VONGBI-515</v>
+        <v>DOD-VONGBITAYTPW</v>
       </c>
       <c r="D516" t="str">
         <v/>
@@ -38620,7 +38620,7 @@
         <v>Vòng bi tay trắng Korea 1480</v>
       </c>
       <c r="C517" t="str">
-        <v>DOD-VONGBI-516</v>
+        <v>DOD-VONGBITAYTIM</v>
       </c>
       <c r="D517" t="str">
         <v/>
@@ -38694,7 +38694,7 @@
         <v>Vòng bi tay trắng Korea 1030</v>
       </c>
       <c r="C518" t="str">
-        <v>DOD-VONGBI-517</v>
+        <v>DOD-VONGBITAYTBA</v>
       </c>
       <c r="D518" t="str">
         <v/>
@@ -38768,7 +38768,7 @@
         <v>Chổi than Korea</v>
       </c>
       <c r="C519" t="str">
-        <v>DOD-CHOITH-518</v>
+        <v>DOD-CHOITHANKOJW</v>
       </c>
       <c r="D519" t="str">
         <v/>
@@ -38842,7 +38842,7 @@
         <v>Máy hút bụi Lugx</v>
       </c>
       <c r="C520" t="str">
-        <v>DOD-MAYHUT-519</v>
+        <v>DOD-MAYHUTBUILRS</v>
       </c>
       <c r="D520" t="str">
         <v/>
@@ -38916,7 +38916,7 @@
         <v>Metallic gel liner - Gold</v>
       </c>
       <c r="C521" t="str">
-        <v>DES-METALL-520</v>
+        <v>DES-METALLICGEDZ</v>
       </c>
       <c r="D521" t="str">
         <v/>
@@ -38990,7 +38990,7 @@
         <v>Metallic gel liner - Silver</v>
       </c>
       <c r="C522" t="str">
-        <v>DES-METALL-521</v>
+        <v>DES-METALLICGERO</v>
       </c>
       <c r="D522" t="str">
         <v/>
@@ -39064,7 +39064,7 @@
         <v>Metallic gel liner - Rose gold</v>
       </c>
       <c r="C523" t="str">
-        <v>DES-METALL-522</v>
+        <v>DES-METALLICGELY</v>
       </c>
       <c r="D523" t="str">
         <v/>
@@ -39138,7 +39138,7 @@
         <v>Metallic gel liner - Champagne gold</v>
       </c>
       <c r="C524" t="str">
-        <v>DES-METALL-523</v>
+        <v>DES-METALLICGEKN</v>
       </c>
       <c r="D524" t="str">
         <v/>
@@ -39212,7 +39212,7 @@
         <v>Chai primer trống có mác</v>
       </c>
       <c r="C525" t="str">
-        <v>HOA-CHAIPR-524</v>
+        <v>HOA-CHAIPRIMERBD</v>
       </c>
       <c r="D525" t="str">
         <v/>
@@ -39286,7 +39286,7 @@
         <v>Chai bond trống có mác</v>
       </c>
       <c r="C526" t="str">
-        <v>TOO-CHAIBO-525</v>
+        <v>TOO-CHAIBONDTRPR</v>
       </c>
       <c r="D526" t="str">
         <v/>
@@ -39360,7 +39360,7 @@
         <v>Gel dặm Ombre</v>
       </c>
       <c r="C527" t="str">
-        <v>DES-GELDAM-526</v>
+        <v>DES-GELDAMOMBRJD</v>
       </c>
       <c r="D527" t="str">
         <v/>
@@ -39434,7 +39434,7 @@
         <v>Reflective gel polish - Gold</v>
       </c>
       <c r="C528" t="str">
-        <v>DES-REFLEC-527</v>
+        <v>DES-REFLECTIVESP</v>
       </c>
       <c r="D528" t="str">
         <v/>
@@ -39508,7 +39508,7 @@
         <v>Reflective gel polish - Silver</v>
       </c>
       <c r="C529" t="str">
-        <v>DES-REFLEC-528</v>
+        <v>DES-REFLECTIVEEL</v>
       </c>
       <c r="D529" t="str">
         <v/>
@@ -39582,7 +39582,7 @@
         <v>Reflective gel polish - Red</v>
       </c>
       <c r="C530" t="str">
-        <v>DES-REFLEC-529</v>
+        <v>DES-REFLECTIVEOQ</v>
       </c>
       <c r="D530" t="str">
         <v/>
@@ -39656,7 +39656,7 @@
         <v>Reflective gel polish - Black</v>
       </c>
       <c r="C531" t="str">
-        <v>DES-REFLEC-530</v>
+        <v>DES-REFLECTIVEZS</v>
       </c>
       <c r="D531" t="str">
         <v/>
@@ -39730,7 +39730,7 @@
         <v>Quyển mẫu sơn SORAH 300</v>
       </c>
       <c r="C532" t="str">
-        <v>SON-QUYENM-531</v>
+        <v>SON-QUYENMAUSOGW</v>
       </c>
       <c r="D532" t="str">
         <v/>

</xml_diff>

<commit_message>
Update SKU generation to use product names and improve import file format
Refactor generateSKU function in storage.ts to use product name text for SKU suffix, and regenerate products-import-final.xlsx.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 8436b268-12fd-450e-b517-e55adeb71af1
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 9c4333da-ab00-4136-9bd0-032545970e36
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/6e81966b-af7d-438d-b68d-89d915c5170b/8436b268-12fd-450e-b517-e55adeb71af1/pCPGKM5
</commit_message>
<xml_diff>
--- a/attached_assets/products-import-final.xlsx
+++ b/attached_assets/products-import-final.xlsx
@@ -404,7 +404,7 @@
   <cols>
     <col min="1" max="1" width="40.83203125" customWidth="1"/>
     <col min="2" max="2" width="40.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="45.83203125" customWidth="1"/>
@@ -510,7 +510,7 @@
         <v>4XC - 5in1</v>
       </c>
       <c r="C2" t="str">
-        <v>DAU-4XC5IN1FH</v>
+        <v>DAU-4XC5IN1</v>
       </c>
       <c r="D2" t="str">
         <v/>
@@ -584,7 +584,7 @@
         <v>M - nhỏ tròn</v>
       </c>
       <c r="C3" t="str">
-        <v>DAU-MNHOTRONTP</v>
+        <v>DAU-MNHOTRON</v>
       </c>
       <c r="D3" t="str">
         <v/>
@@ -658,7 +658,7 @@
         <v>XF - nhỏ</v>
       </c>
       <c r="C4" t="str">
-        <v>DAU-XFNHORH</v>
+        <v>DAU-XFNHO</v>
       </c>
       <c r="D4" t="str">
         <v/>
@@ -732,7 +732,7 @@
         <v>Sticker - 5D</v>
       </c>
       <c r="C5" t="str">
-        <v>DES-STICKER5DQG</v>
+        <v>DES-STICKER5D</v>
       </c>
       <c r="D5" t="str">
         <v/>
@@ -806,7 +806,7 @@
         <v>Sticker - 3D</v>
       </c>
       <c r="C6" t="str">
-        <v>DES-STICKER3DNW</v>
+        <v>DES-STICKER3D</v>
       </c>
       <c r="D6" t="str">
         <v/>
@@ -880,7 +880,7 @@
         <v>Sticker - 2D</v>
       </c>
       <c r="C7" t="str">
-        <v>DES-STICKER2DHH</v>
+        <v>DES-STICKER2D</v>
       </c>
       <c r="D7" t="str">
         <v/>
@@ -954,7 +954,7 @@
         <v>Foil sticker</v>
       </c>
       <c r="C8" t="str">
-        <v>DES-FOILSTICKEQA</v>
+        <v>DES-FOILSTICKER</v>
       </c>
       <c r="D8" t="str">
         <v/>
@@ -1028,7 +1028,7 @@
         <v>Tips natur nhọn ngắn</v>
       </c>
       <c r="C9" t="str">
-        <v>TIP-TIPSNATURNKB</v>
+        <v>TIP-TIPSNATURNHO</v>
       </c>
       <c r="D9" t="str">
         <v/>
@@ -1102,7 +1102,7 @@
         <v>Tips natur thẳng ngắn</v>
       </c>
       <c r="C10" t="str">
-        <v>TIP-TIPSNATURTNM</v>
+        <v>TIP-TIPSNATURTHA</v>
       </c>
       <c r="D10" t="str">
         <v/>
@@ -1176,7 +1176,7 @@
         <v>Tips natur nhọn dài</v>
       </c>
       <c r="C11" t="str">
-        <v>TIP-TIPSNATURNQK</v>
+        <v>TIP-TIPSNATURNHO2</v>
       </c>
       <c r="D11" t="str">
         <v/>
@@ -1250,7 +1250,7 @@
         <v>Tips trong nhọn ngắn</v>
       </c>
       <c r="C12" t="str">
-        <v>TIP-TIPSTRONGNBM</v>
+        <v>TIP-TIPSTRONGNHO</v>
       </c>
       <c r="D12" t="str">
         <v/>
@@ -1324,7 +1324,7 @@
         <v>Đá nhỏ 7mầu</v>
       </c>
       <c r="C13" t="str">
-        <v>DES-DANHO7MAUPR</v>
+        <v>DES-DANHO7MAU</v>
       </c>
       <c r="D13" t="str">
         <v/>
@@ -1398,7 +1398,7 @@
         <v>Bút vẽ (1set=3c)</v>
       </c>
       <c r="C14" t="str">
-        <v>BUT-BUTVE1SET3UK</v>
+        <v>BUT-BUTVE1SET3C</v>
       </c>
       <c r="D14" t="str">
         <v/>
@@ -1472,7 +1472,7 @@
         <v>Hộp đựng móng (0-9)</v>
       </c>
       <c r="C15" t="str">
-        <v>TOO-HOPDUNGMONLU</v>
+        <v>TOO-HOPDUNGMONG0</v>
       </c>
       <c r="D15" t="str">
         <v/>
@@ -1546,7 +1546,7 @@
         <v>Cây fen - V shape</v>
       </c>
       <c r="C16" t="str">
-        <v>TOO-CAYFENVSHAEW</v>
+        <v>TOO-CAYFENVSHAPE</v>
       </c>
       <c r="D16" t="str">
         <v/>
@@ -1620,7 +1620,7 @@
         <v>Cây fen - U shape</v>
       </c>
       <c r="C17" t="str">
-        <v>TOO-CAYFENUSHACF</v>
+        <v>TOO-CAYFENUSHAPE</v>
       </c>
       <c r="D17" t="str">
         <v/>
@@ -1694,7 +1694,7 @@
         <v>Mịn Fusion</v>
       </c>
       <c r="C18" t="str">
-        <v>DAU-MINFUSIONBC</v>
+        <v>DAU-MINFUSION</v>
       </c>
       <c r="D18" t="str">
         <v/>
@@ -1768,7 +1768,7 @@
         <v>French A</v>
       </c>
       <c r="C19" t="str">
-        <v>TOO-FRENCHAKI</v>
+        <v>TOO-FRENCHA</v>
       </c>
       <c r="D19" t="str">
         <v/>
@@ -1842,7 +1842,7 @@
         <v>French B</v>
       </c>
       <c r="C20" t="str">
-        <v>TOO-FRENCHBZG</v>
+        <v>TOO-FRENCHB</v>
       </c>
       <c r="D20" t="str">
         <v/>
@@ -1916,7 +1916,7 @@
         <v>Sticker lửa</v>
       </c>
       <c r="C21" t="str">
-        <v>DES-STICKERLUATD</v>
+        <v>DES-STICKERLUA</v>
       </c>
       <c r="D21" t="str">
         <v/>
@@ -1990,7 +1990,7 @@
         <v>Bút vẽ 2 đầu - 7/11mm</v>
       </c>
       <c r="C22" t="str">
-        <v>BUT-BUTVE2DAU7PA</v>
+        <v>BUT-BUTVE2DAU711</v>
       </c>
       <c r="D22" t="str">
         <v/>
@@ -2064,7 +2064,7 @@
         <v>Chrome Red</v>
       </c>
       <c r="C23" t="str">
-        <v>DES-CHROMEREDJL</v>
+        <v>DES-CHROMERED</v>
       </c>
       <c r="D23" t="str">
         <v/>
@@ -2138,7 +2138,7 @@
         <v>Sơn Ultra Black</v>
       </c>
       <c r="C24" t="str">
-        <v>HOA-SONULTRABLFG</v>
+        <v>HOA-SONULTRABLAC</v>
       </c>
       <c r="D24" t="str">
         <v/>
@@ -2212,7 +2212,7 @@
         <v>Sơn Ultra White</v>
       </c>
       <c r="C25" t="str">
-        <v>HOA-SONULTRAWHRT</v>
+        <v>HOA-SONULTRAWHIT</v>
       </c>
       <c r="D25" t="str">
         <v/>
@@ -2286,7 +2286,7 @@
         <v>Vỏ nhám tím ⌗60 - C</v>
       </c>
       <c r="C26" t="str">
-        <v>TOO-VONHAMTIM6BJ</v>
+        <v>TOO-VONHAMTIM60C</v>
       </c>
       <c r="D26" t="str">
         <v/>
@@ -2360,7 +2360,7 @@
         <v>Bút fen</v>
       </c>
       <c r="C27" t="str">
-        <v>BUT-BUTFENEL</v>
+        <v>BUT-BUTFEN</v>
       </c>
       <c r="D27" t="str">
         <v/>
@@ -2434,7 +2434,7 @@
         <v>Bút ombre</v>
       </c>
       <c r="C28" t="str">
-        <v>BUT-BUTOMBRESA</v>
+        <v>BUT-BUTOMBRE</v>
       </c>
       <c r="D28" t="str">
         <v/>
@@ -2508,7 +2508,7 @@
         <v>Vỏ nhám trắng ⌗60 - C</v>
       </c>
       <c r="C29" t="str">
-        <v>TOO-VONHAMTRANFI</v>
+        <v>TOO-VONHAMTRANG6</v>
       </c>
       <c r="D29" t="str">
         <v/>
@@ -2582,7 +2582,7 @@
         <v>Set sơn mầu vẽ 12 lọ</v>
       </c>
       <c r="C30" t="str">
-        <v>HOA-SETSONMAUVEF</v>
+        <v>HOA-SETSONMAUVE1</v>
       </c>
       <c r="D30" t="str">
         <v/>
@@ -2656,7 +2656,7 @@
         <v>Đá kê sơn</v>
       </c>
       <c r="C31" t="str">
-        <v>TOO-DAKESONPI</v>
+        <v>TOO-DAKESON</v>
       </c>
       <c r="D31" t="str">
         <v/>
@@ -2730,7 +2730,7 @@
         <v>Sticker Bướm</v>
       </c>
       <c r="C32" t="str">
-        <v>DES-STICKERBUOEF</v>
+        <v>DES-STICKERBUOM</v>
       </c>
       <c r="D32" t="str">
         <v/>
@@ -2804,7 +2804,7 @@
         <v>Đá rắc 28g</v>
       </c>
       <c r="C33" t="str">
-        <v>DES-DARAC28GWB</v>
+        <v>DES-DARAC28G</v>
       </c>
       <c r="D33" t="str">
         <v/>
@@ -2878,7 +2878,7 @@
         <v>Kê tay Silicon</v>
       </c>
       <c r="C34" t="str">
-        <v>TOO-KETAYSILICMZ</v>
+        <v>TOO-KETAYSILICON</v>
       </c>
       <c r="D34" t="str">
         <v/>
@@ -2952,7 +2952,7 @@
         <v>Bút mực vẽ</v>
       </c>
       <c r="C35" t="str">
-        <v>DES-BUTMUCVEOJ</v>
+        <v>DES-BUTMUCVE</v>
       </c>
       <c r="D35" t="str">
         <v/>
@@ -3026,7 +3026,7 @@
         <v>5in1 Phá 2XC</v>
       </c>
       <c r="C36" t="str">
-        <v>DAU-5IN1PHA2XCVB</v>
+        <v>DAU-5IN1PHA2XC</v>
       </c>
       <c r="D36" t="str">
         <v/>
@@ -3100,7 +3100,7 @@
         <v>Bút đắp gel sz14</v>
       </c>
       <c r="C37" t="str">
-        <v>BUT-BUTDAPGELSEF</v>
+        <v>BUT-BUTDAPGELSZ1</v>
       </c>
       <c r="D37" t="str">
         <v/>
@@ -3174,7 +3174,7 @@
         <v>Tips thường gói 50c</v>
       </c>
       <c r="C38" t="str">
-        <v>TIP-TIPSTHUONGJG</v>
+        <v>TIP-TIPSTHUONGGO</v>
       </c>
       <c r="D38" t="str">
         <v/>
@@ -3248,7 +3248,7 @@
         <v>Bút gel đỏ sz8</v>
       </c>
       <c r="C39" t="str">
-        <v>BUT-BUTGELDOSZZF</v>
+        <v>BUT-BUTGELDOSZ8</v>
       </c>
       <c r="D39" t="str">
         <v/>
@@ -3322,7 +3322,7 @@
         <v>In French</v>
       </c>
       <c r="C40" t="str">
-        <v>DES-INFRENCHSZ</v>
+        <v>DES-INFRENCH</v>
       </c>
       <c r="D40" t="str">
         <v/>
@@ -3396,7 +3396,7 @@
         <v>Dao cắt fen</v>
       </c>
       <c r="C41" t="str">
-        <v>TOO-DAOCATFENRY</v>
+        <v>TOO-DAOCATFEN</v>
       </c>
       <c r="D41" t="str">
         <v/>
@@ -3470,7 +3470,7 @@
         <v>Sticker playboy</v>
       </c>
       <c r="C42" t="str">
-        <v>DES-STICKERPLARY</v>
+        <v>DES-STICKERPLAYB</v>
       </c>
       <c r="D42" t="str">
         <v/>
@@ -3544,7 +3544,7 @@
         <v>Gold foil</v>
       </c>
       <c r="C43" t="str">
-        <v>DES-GOLDFOILBT</v>
+        <v>DES-GOLDFOIL</v>
       </c>
       <c r="D43" t="str">
         <v/>
@@ -3618,7 +3618,7 @@
         <v>Bút gel - tròn 10</v>
       </c>
       <c r="C44" t="str">
-        <v>BUT-BUTGELTRONLW</v>
+        <v>BUT-BUTGELTRON10</v>
       </c>
       <c r="D44" t="str">
         <v/>
@@ -3692,7 +3692,7 @@
         <v>Bút gel quét mầu - tròn 8</v>
       </c>
       <c r="C45" t="str">
-        <v>BUT-BUTGELQUETYP</v>
+        <v>BUT-BUTGELQUETMA</v>
       </c>
       <c r="D45" t="str">
         <v/>
@@ -3766,7 +3766,7 @@
         <v>Set bào &amp; vỏ mịn da chân</v>
       </c>
       <c r="C46" t="str">
-        <v>DAU-SETBAOVOMIVA</v>
+        <v>DAU-SETBAOVOMIND</v>
       </c>
       <c r="D46" t="str">
         <v/>
@@ -3840,7 +3840,7 @@
         <v>Tips Vuông trong XXL</v>
       </c>
       <c r="C47" t="str">
-        <v>TIP-TIPSVUONGTRK</v>
+        <v>TIP-TIPSVUONGTRO</v>
       </c>
       <c r="D47" t="str">
         <v/>
@@ -3914,7 +3914,7 @@
         <v>Bấm móng 777 Korea</v>
       </c>
       <c r="C48" t="str">
-        <v>TOO-BAMMONG777EE</v>
+        <v>TOO-BAMMONG777KO</v>
       </c>
       <c r="D48" t="str">
         <v/>
@@ -3988,7 +3988,7 @@
         <v>Sticker Halloween Phát sáng</v>
       </c>
       <c r="C49" t="str">
-        <v>DES-STICKERHALYL</v>
+        <v>DES-STICKERHALLO</v>
       </c>
       <c r="D49" t="str">
         <v/>
@@ -4062,7 +4062,7 @@
         <v>Top matte 15ml</v>
       </c>
       <c r="C50" t="str">
-        <v>HOA-TOPMATTE15LM</v>
+        <v>HOA-TOPMATTE15ML</v>
       </c>
       <c r="D50" t="str">
         <v/>
@@ -4136,7 +4136,7 @@
         <v>Foil gel</v>
       </c>
       <c r="C51" t="str">
-        <v>HOA-FOILGELPT</v>
+        <v>HOA-FOILGEL</v>
       </c>
       <c r="D51" t="str">
         <v/>
@@ -4210,7 +4210,7 @@
         <v>Sticker Playboy</v>
       </c>
       <c r="C52" t="str">
-        <v>DES-STICKERPLADA</v>
+        <v>DES-STICKERPLAYB2</v>
       </c>
       <c r="D52" t="str">
         <v/>
@@ -4284,7 +4284,7 @@
         <v>Bình xịt ombre bột</v>
       </c>
       <c r="C53" t="str">
-        <v>TOO-BINHXITOMBNK</v>
+        <v>TOO-BINHXITOMBRE</v>
       </c>
       <c r="D53" t="str">
         <v/>
@@ -4358,7 +4358,7 @@
         <v>Tay giả mềm</v>
       </c>
       <c r="C54" t="str">
-        <v>TOO-TAYGIAMEMYL</v>
+        <v>TOO-TAYGIAMEM</v>
       </c>
       <c r="D54" t="str">
         <v/>
@@ -4432,7 +4432,7 @@
         <v>Tay giả khớp</v>
       </c>
       <c r="C55" t="str">
-        <v>TOO-TAYGIAKHOPOJ</v>
+        <v>TOO-TAYGIAKHOP</v>
       </c>
       <c r="D55" t="str">
         <v/>
@@ -4506,7 +4506,7 @@
         <v>Bút Gradient</v>
       </c>
       <c r="C56" t="str">
-        <v>BUT-BUTGRADIENVR</v>
+        <v>BUT-BUTGRADIENT</v>
       </c>
       <c r="D56" t="str">
         <v/>
@@ -4580,7 +4580,7 @@
         <v>Đầu Chổi sắt</v>
       </c>
       <c r="C57" t="str">
-        <v>DAU-DAUCHOISATYH</v>
+        <v>DAU-DAUCHOISAT</v>
       </c>
       <c r="D57" t="str">
         <v/>
@@ -4654,7 +4654,7 @@
         <v>3in1 Mịn C - ngắn</v>
       </c>
       <c r="C58" t="str">
-        <v>DAU-3IN1MINCNGGD</v>
+        <v>DAU-3IN1MINCNGAN</v>
       </c>
       <c r="D58" t="str">
         <v/>
@@ -4728,7 +4728,7 @@
         <v>3XC ULTRA</v>
       </c>
       <c r="C59" t="str">
-        <v>DAU-3XCULTRABP</v>
+        <v>DAU-3XCULTRA</v>
       </c>
       <c r="D59" t="str">
         <v/>
@@ -4802,7 +4802,7 @@
         <v>5XC - Titan</v>
       </c>
       <c r="C60" t="str">
-        <v>DAU-5XCTITANLX</v>
+        <v>DAU-5XCTITAN</v>
       </c>
       <c r="D60" t="str">
         <v/>
@@ -4876,7 +4876,7 @@
         <v>Bào nhám Diamond nhỏ - M</v>
       </c>
       <c r="C61" t="str">
-        <v>DAU-BAONHAMDIAIH</v>
+        <v>DAU-BAONHAMDIAMO</v>
       </c>
       <c r="D61" t="str">
         <v/>
@@ -4950,7 +4950,7 @@
         <v>Bào nhám Diamond to - C</v>
       </c>
       <c r="C62" t="str">
-        <v>DAU-BAONHAMDIAHI</v>
+        <v>DAU-BAONHAMDIAMO2</v>
       </c>
       <c r="D62" t="str">
         <v/>
@@ -5024,7 +5024,7 @@
         <v>Hoa 3D Design</v>
       </c>
       <c r="C63" t="str">
-        <v>DES-HOA3DDESIGKO</v>
+        <v>DES-HOA3DDESIGN</v>
       </c>
       <c r="D63" t="str">
         <v/>
@@ -5098,7 +5098,7 @@
         <v>Sticker chữ</v>
       </c>
       <c r="C64" t="str">
-        <v>DES-STICKERCHUJP</v>
+        <v>DES-STICKERCHU</v>
       </c>
       <c r="D64" t="str">
         <v/>
@@ -5172,7 +5172,7 @@
         <v>Tips Ballerina trong XXL</v>
       </c>
       <c r="C65" t="str">
-        <v>TIP-TIPSBALLERKQ</v>
+        <v>TIP-TIPSBALLERIN</v>
       </c>
       <c r="D65" t="str">
         <v/>
@@ -5246,7 +5246,7 @@
         <v>Tip ballerina ngắn 4/5/5/6</v>
       </c>
       <c r="C66" t="str">
-        <v>TOO-TIPBALLERIUQ</v>
+        <v>TOO-TIPBALLERINA</v>
       </c>
       <c r="D66" t="str">
         <v/>
@@ -5320,7 +5320,7 @@
         <v>Tip trong nhọn 4/5/5/6</v>
       </c>
       <c r="C67" t="str">
-        <v>TOO-TIPTRONGNHFG</v>
+        <v>TOO-TIPTRONGNHON</v>
       </c>
       <c r="D67" t="str">
         <v/>
@@ -5394,7 +5394,7 @@
         <v>Lá Trái tim set</v>
       </c>
       <c r="C68" t="str">
-        <v>DES-LATRAITIMSDJ</v>
+        <v>DES-LATRAITIMSET</v>
       </c>
       <c r="D68" t="str">
         <v/>
@@ -5468,7 +5468,7 @@
         <v>Bột màu 56g</v>
       </c>
       <c r="C69" t="str">
-        <v>HOA-BOTMAU56GOU</v>
+        <v>HOA-BOTMAU56G</v>
       </c>
       <c r="D69" t="str">
         <v/>
@@ -5542,7 +5542,7 @@
         <v>Máy xịt ombre gel</v>
       </c>
       <c r="C70" t="str">
-        <v>DOD-MAYXITOMBRDY</v>
+        <v>DOD-MAYXITOMBREG</v>
       </c>
       <c r="D70" t="str">
         <v/>
@@ -5616,7 +5616,7 @@
         <v>Sơn vẽ hũ Metallic 5g</v>
       </c>
       <c r="C71" t="str">
-        <v>DES-SONVEHUMETEM</v>
+        <v>DES-SONVEHUMETAL</v>
       </c>
       <c r="D71" t="str">
         <v/>
@@ -5690,7 +5690,7 @@
         <v>Sơn vẽ hũ 5g</v>
       </c>
       <c r="C72" t="str">
-        <v>DES-SONVEHU5GUN</v>
+        <v>DES-SONVEHU5G</v>
       </c>
       <c r="D72" t="str">
         <v/>
@@ -5764,7 +5764,7 @@
         <v>Cuticle oil 15ml</v>
       </c>
       <c r="C73" t="str">
-        <v>HOA-CUTICLEOILHX</v>
+        <v>HOA-CUTICLEOIL15</v>
       </c>
       <c r="D73" t="str">
         <v/>
@@ -5838,7 +5838,7 @@
         <v>Gel vẽ màng nhện 5g</v>
       </c>
       <c r="C74" t="str">
-        <v>DES-GELVEMANGNVY</v>
+        <v>DES-GELVEMANGNHE</v>
       </c>
       <c r="D74" t="str">
         <v/>
@@ -5912,7 +5912,7 @@
         <v>Nhám trắng M ⌗240 (1000c)</v>
       </c>
       <c r="C75" t="str">
-        <v>TOO-NHAMTRANGMLR</v>
+        <v>TOO-NHAMTRANGM24</v>
       </c>
       <c r="D75" t="str">
         <v/>
@@ -5986,7 +5986,7 @@
         <v>Tips trong nhọn dài</v>
       </c>
       <c r="C76" t="str">
-        <v>TIP-TIPSTRONGNIY</v>
+        <v>TIP-TIPSTRONGNHO2</v>
       </c>
       <c r="D76" t="str">
         <v/>
@@ -6060,7 +6060,7 @@
         <v>Lẻ - Tip Trong nhọn</v>
       </c>
       <c r="C77" t="str">
-        <v>TIP-LETIPTRONGKP</v>
+        <v>TIP-LETIPTRONGNH</v>
       </c>
       <c r="D77" t="str">
         <v/>
@@ -6134,7 +6134,7 @@
         <v>Bào Diamond Cuticle 2.5mm</v>
       </c>
       <c r="C78" t="str">
-        <v>DAU-BAODIAMONDOJ</v>
+        <v>DAU-BAODIAMONDCU</v>
       </c>
       <c r="D78" t="str">
         <v/>
@@ -6208,7 +6208,7 @@
         <v>Sticker F Noel - 3D</v>
       </c>
       <c r="C79" t="str">
-        <v>DES-STICKERFNORT</v>
+        <v>DES-STICKERFNOEL</v>
       </c>
       <c r="D79" t="str">
         <v/>
@@ -6282,7 +6282,7 @@
         <v>Sticker STZ Noel - 5D</v>
       </c>
       <c r="C80" t="str">
-        <v>DES-STICKERSTZGZ</v>
+        <v>DES-STICKERSTZNO</v>
       </c>
       <c r="D80" t="str">
         <v/>
@@ -6356,7 +6356,7 @@
         <v>Kéo</v>
       </c>
       <c r="C81" t="str">
-        <v>TOO-KEOZQ</v>
+        <v>TOO-KEO</v>
       </c>
       <c r="D81" t="str">
         <v/>
@@ -6430,7 +6430,7 @@
         <v>Máy Bào Btmarathon 3</v>
       </c>
       <c r="C82" t="str">
-        <v>DOD-MAYBAOBTMADA</v>
+        <v>DOD-MAYBAOBTMARA</v>
       </c>
       <c r="D82" t="str">
         <v/>
@@ -6504,7 +6504,7 @@
         <v>Bút chấm bi set 5c</v>
       </c>
       <c r="C83" t="str">
-        <v>TOO-BUTCHAMBISXF</v>
+        <v>TOO-BUTCHAMBISET</v>
       </c>
       <c r="D83" t="str">
         <v/>
@@ -6578,7 +6578,7 @@
         <v>Cán dao cạo chân - hồng</v>
       </c>
       <c r="C84" t="str">
-        <v>TOO-CANDAOCAOCOF</v>
+        <v>TOO-CANDAOCAOCHA</v>
       </c>
       <c r="D84" t="str">
         <v/>
@@ -6652,7 +6652,7 @@
         <v>Đèn LED pin cầm tay</v>
       </c>
       <c r="C85" t="str">
-        <v>DOD-DENLEDPINCZR</v>
+        <v>DOD-DENLEDPINCAM</v>
       </c>
       <c r="D85" t="str">
         <v/>
@@ -6726,7 +6726,7 @@
         <v>Khay inox</v>
       </c>
       <c r="C86" t="str">
-        <v>TOO-KHAYINOXHS</v>
+        <v>TOO-KHAYINOX</v>
       </c>
       <c r="D86" t="str">
         <v/>
@@ -6800,7 +6800,7 @@
         <v>Tay thay máy bào di động</v>
       </c>
       <c r="C87" t="str">
-        <v>DOD-TAYTHAYMAYAJ</v>
+        <v>DOD-TAYTHAYMAYBA</v>
       </c>
       <c r="D87" t="str">
         <v/>
@@ -6874,7 +6874,7 @@
         <v>Cây đẩy da inox japan</v>
       </c>
       <c r="C88" t="str">
-        <v>TOO-CAYDAYDAINKX</v>
+        <v>TOO-CAYDAYDAINOX</v>
       </c>
       <c r="D88" t="str">
         <v/>
@@ -6948,7 +6948,7 @@
         <v>3XC Hoa cúc ULTRA</v>
       </c>
       <c r="C89" t="str">
-        <v>DAU-3XCHOACUCUBC</v>
+        <v>DAU-3XCHOACUCULT</v>
       </c>
       <c r="D89" t="str">
         <v/>
@@ -7022,7 +7022,7 @@
         <v>Bút quan tài</v>
       </c>
       <c r="C90" t="str">
-        <v>BUT-BUTQUANTAIYM</v>
+        <v>BUT-BUTQUANTAI</v>
       </c>
       <c r="D90" t="str">
         <v/>
@@ -7096,7 +7096,7 @@
         <v>Bút vẽ 2 đầu - 10/20mm</v>
       </c>
       <c r="C91" t="str">
-        <v>BUT-BUTVE2DAU1ZI</v>
+        <v>BUT-BUTVE2DAU102</v>
       </c>
       <c r="D91" t="str">
         <v/>
@@ -7170,7 +7170,7 @@
         <v>Kéo - dài</v>
       </c>
       <c r="C92" t="str">
-        <v>TOO-KEODAIAV</v>
+        <v>TOO-KEODAI</v>
       </c>
       <c r="D92" t="str">
         <v/>
@@ -7244,7 +7244,7 @@
         <v>4XC - Titan</v>
       </c>
       <c r="C93" t="str">
-        <v>DAU-4XCTITANUC</v>
+        <v>DAU-4XCTITAN</v>
       </c>
       <c r="D93" t="str">
         <v/>
@@ -7318,7 +7318,7 @@
         <v>4XC trục nhỏ</v>
       </c>
       <c r="C94" t="str">
-        <v>DAU-4XCTRUCNHOYE</v>
+        <v>DAU-4XCTRUCNHO</v>
       </c>
       <c r="D94" t="str">
         <v/>
@@ -7392,7 +7392,7 @@
         <v>Vỏ nhám trắng M ⌗240 (100c)</v>
       </c>
       <c r="C95" t="str">
-        <v>TOO-VONHAMTRANBO</v>
+        <v>TOO-VONHAMTRANGM</v>
       </c>
       <c r="D95" t="str">
         <v/>
@@ -7466,7 +7466,7 @@
         <v>Găng tay Latex trắng - S</v>
       </c>
       <c r="C96" t="str">
-        <v>TOO-GANGTAYLATQD</v>
+        <v>TOO-GANGTAYLATEX</v>
       </c>
       <c r="D96" t="str">
         <v/>
@@ -7540,7 +7540,7 @@
         <v>Găng tay Latex trắng - M</v>
       </c>
       <c r="C97" t="str">
-        <v>TOO-GANGTAYLATXC</v>
+        <v>TOO-GANGTAYLATEX2</v>
       </c>
       <c r="D97" t="str">
         <v/>
@@ -7614,7 +7614,7 @@
         <v>Chà chân 2 mặt</v>
       </c>
       <c r="C98" t="str">
-        <v>TOO-CHACHAN2MAHP</v>
+        <v>TOO-CHACHAN2MAT</v>
       </c>
       <c r="D98" t="str">
         <v/>
@@ -7688,7 +7688,7 @@
         <v>Nước rửa cọ 120ml</v>
       </c>
       <c r="C99" t="str">
-        <v>HOA-NUOCRUACO1FN</v>
+        <v>HOA-NUOCRUACO120</v>
       </c>
       <c r="D99" t="str">
         <v/>
@@ -7762,7 +7762,7 @@
         <v>Bào gầm</v>
       </c>
       <c r="C100" t="str">
-        <v>DAU-BAOGAMQK</v>
+        <v>DAU-BAOGAM</v>
       </c>
       <c r="D100" t="str">
         <v/>
@@ -7836,7 +7836,7 @@
         <v>Gel đính đá</v>
       </c>
       <c r="C101" t="str">
-        <v>HOA-GELDINHDAVQ</v>
+        <v>HOA-GELDINHDA</v>
       </c>
       <c r="D101" t="str">
         <v/>
@@ -7910,7 +7910,7 @@
         <v>BNS keo</v>
       </c>
       <c r="C102" t="str">
-        <v>HOA-BNSKEOQK</v>
+        <v>HOA-BNSKEO</v>
       </c>
       <c r="D102" t="str">
         <v/>
@@ -7984,7 +7984,7 @@
         <v>15ml top coat tím loãng</v>
       </c>
       <c r="C103" t="str">
-        <v>TOP-15MLTOPCOAYI</v>
+        <v>TOP-15MLTOPCOATT</v>
       </c>
       <c r="D103" t="str">
         <v/>
@@ -8058,7 +8058,7 @@
         <v>Tip Trong Vuông XXL - Lẻ</v>
       </c>
       <c r="C104" t="str">
-        <v>TIP-TIPTRONGVUFU</v>
+        <v>TIP-TIPTRONGVUON</v>
       </c>
       <c r="D104" t="str">
         <v/>
@@ -8132,7 +8132,7 @@
         <v>Chổi phủi bàn</v>
       </c>
       <c r="C105" t="str">
-        <v>TOO-CHOIPHUIBADO</v>
+        <v>TOO-CHOIPHUIBAN</v>
       </c>
       <c r="D105" t="str">
         <v/>
@@ -8206,7 +8206,7 @@
         <v>Spa tablets 2gal 4000 viên</v>
       </c>
       <c r="C106" t="str">
-        <v>HOA-SPATABLETSOY</v>
+        <v>HOA-SPATABLETS2G</v>
       </c>
       <c r="D106" t="str">
         <v/>
@@ -8280,7 +8280,7 @@
         <v>Nhũ đường</v>
       </c>
       <c r="C107" t="str">
-        <v>DES-NHUDUONGHY</v>
+        <v>DES-NHUDUONG</v>
       </c>
       <c r="D107" t="str">
         <v/>
@@ -8354,7 +8354,7 @@
         <v>Bút quan tài sz18</v>
       </c>
       <c r="C108" t="str">
-        <v>BUT-BUTQUANTAIBL</v>
+        <v>BUT-BUTQUANTAISZ</v>
       </c>
       <c r="D108" t="str">
         <v/>
@@ -8428,7 +8428,7 @@
         <v>Bút gel - vuông 10</v>
       </c>
       <c r="C109" t="str">
-        <v>BUT-BUTGELVUONXO</v>
+        <v>BUT-BUTGELVUONG1</v>
       </c>
       <c r="D109" t="str">
         <v/>
@@ -8502,7 +8502,7 @@
         <v>Súng bào korea</v>
       </c>
       <c r="C110" t="str">
-        <v>DOD-SUNGBAOKORES</v>
+        <v>DOD-SUNGBAOKOREA</v>
       </c>
       <c r="D110" t="str">
         <v/>
@@ -8576,7 +8576,7 @@
         <v>XC</v>
       </c>
       <c r="C111" t="str">
-        <v>DAU-XCNE</v>
+        <v>DAU-XC</v>
       </c>
       <c r="D111" t="str">
         <v/>
@@ -8650,7 +8650,7 @@
         <v>Bao ngón cái 500c</v>
       </c>
       <c r="C112" t="str">
-        <v>TOO-BAONGONCAIVT</v>
+        <v>TOO-BAONGONCAI50</v>
       </c>
       <c r="D112" t="str">
         <v/>
@@ -8724,7 +8724,7 @@
         <v>Top coat 500ml</v>
       </c>
       <c r="C113" t="str">
-        <v>TOP-TOPCOAT500ZG</v>
+        <v>TOP-TOPCOAT500ML</v>
       </c>
       <c r="D113" t="str">
         <v/>
@@ -8798,7 +8798,7 @@
         <v>Chrome trắng gương 1g</v>
       </c>
       <c r="C114" t="str">
-        <v>DES-CHROMETRANWE</v>
+        <v>DES-CHROMETRANGG</v>
       </c>
       <c r="D114" t="str">
         <v/>
@@ -8872,7 +8872,7 @@
         <v>Top matte 250ml</v>
       </c>
       <c r="C115" t="str">
-        <v>HOA-TOPMATTE25HB</v>
+        <v>HOA-TOPMATTE250M</v>
       </c>
       <c r="D115" t="str">
         <v/>
@@ -8946,7 +8946,7 @@
         <v>Chà chân 1 lần 400c</v>
       </c>
       <c r="C116" t="str">
-        <v>TOO-CHACHAN1LAHS</v>
+        <v>TOO-CHACHAN1LAN4</v>
       </c>
       <c r="D116" t="str">
         <v/>
@@ -9020,7 +9020,7 @@
         <v>Bào mịn Diamond - M</v>
       </c>
       <c r="C117" t="str">
-        <v>DAU-BAOMINDIAMWD</v>
+        <v>DAU-BAOMINDIAMON</v>
       </c>
       <c r="D117" t="str">
         <v/>
@@ -9094,7 +9094,7 @@
         <v>Mịn Fusion - C</v>
       </c>
       <c r="C118" t="str">
-        <v>DAU-MINFUSIONCXM</v>
+        <v>DAU-MINFUSIONC</v>
       </c>
       <c r="D118" t="str">
         <v/>
@@ -9168,7 +9168,7 @@
         <v>Mịn Fusion - F</v>
       </c>
       <c r="C119" t="str">
-        <v>DAU-MINFUSIONFCG</v>
+        <v>DAU-MINFUSIONF</v>
       </c>
       <c r="D119" t="str">
         <v/>
@@ -9242,7 +9242,7 @@
         <v>3XC răng thẳng</v>
       </c>
       <c r="C120" t="str">
-        <v>DAU-3XCRANGTHAWO</v>
+        <v>DAU-3XCRANGTHANG</v>
       </c>
       <c r="D120" t="str">
         <v/>
@@ -9316,7 +9316,7 @@
         <v>4XC răng thẳng</v>
       </c>
       <c r="C121" t="str">
-        <v>DAU-4XCRANGTHACX</v>
+        <v>DAU-4XCRANGTHANG</v>
       </c>
       <c r="D121" t="str">
         <v/>
@@ -9390,7 +9390,7 @@
         <v>Trục nhám rẻ</v>
       </c>
       <c r="C122" t="str">
-        <v>DAU-TRUCNHAMREOB</v>
+        <v>DAU-TRUCNHAMRE</v>
       </c>
       <c r="D122" t="str">
         <v/>
@@ -9464,7 +9464,7 @@
         <v>Bút cán gỗ sz18</v>
       </c>
       <c r="C123" t="str">
-        <v>BUT-BUTCANGOSZFO</v>
+        <v>BUT-BUTCANGOSZ18</v>
       </c>
       <c r="D123" t="str">
         <v/>
@@ -9538,7 +9538,7 @@
         <v>Chrome liquid - ngọc trai</v>
       </c>
       <c r="C124" t="str">
-        <v>DES-CHROMELIQUUW</v>
+        <v>DES-CHROMELIQUID</v>
       </c>
       <c r="D124" t="str">
         <v/>
@@ -9612,7 +9612,7 @@
         <v>Base coat 250ml</v>
       </c>
       <c r="C125" t="str">
-        <v>HOA-BASECOAT25XF</v>
+        <v>HOA-BASECOAT250M</v>
       </c>
       <c r="D125" t="str">
         <v/>
@@ -9686,7 +9686,7 @@
         <v>Top loang - Blooming gel 15ml</v>
       </c>
       <c r="C126" t="str">
-        <v>HOA-TOPLOANGBLZC</v>
+        <v>HOA-TOPLOANGBLOO</v>
       </c>
       <c r="D126" t="str">
         <v/>
@@ -9760,7 +9760,7 @@
         <v>5in1 Pedicure kit xanh</v>
       </c>
       <c r="C127" t="str">
-        <v>TOO-5IN1PEDICULJ</v>
+        <v>TOO-5IN1PEDICURE</v>
       </c>
       <c r="D127" t="str">
         <v/>
@@ -9834,7 +9834,7 @@
         <v>Buffer đen cam 3 mặt</v>
       </c>
       <c r="C128" t="str">
-        <v>TOO-BUFFERDENCPY</v>
+        <v>TOO-BUFFERDENCAM</v>
       </c>
       <c r="D128" t="str">
         <v/>
@@ -9908,7 +9908,7 @@
         <v>Tip ballerina - lẻ</v>
       </c>
       <c r="C129" t="str">
-        <v>TIP-TIPBALLERIZY</v>
+        <v>TIP-TIPBALLERINA</v>
       </c>
       <c r="D129" t="str">
         <v/>
@@ -9982,7 +9982,7 @@
         <v>Kim tuyến DL10-18</v>
       </c>
       <c r="C130" t="str">
-        <v>DES-KIMTUYENDLHR</v>
+        <v>DES-KIMTUYENDL10</v>
       </c>
       <c r="D130" t="str">
         <v/>
@@ -10056,7 +10056,7 @@
         <v>Kim tuyến DL01-09</v>
       </c>
       <c r="C131" t="str">
-        <v>DES-KIMTUYENDLGT</v>
+        <v>DES-KIMTUYENDL01</v>
       </c>
       <c r="D131" t="str">
         <v/>
@@ -10130,7 +10130,7 @@
         <v>Kim tuyến sáng 23g DL01-09</v>
       </c>
       <c r="C132" t="str">
-        <v>DES-KIMTUYENSASC</v>
+        <v>DES-KIMTUYENSANG</v>
       </c>
       <c r="D132" t="str">
         <v/>
@@ -10204,7 +10204,7 @@
         <v>Cốc liquid</v>
       </c>
       <c r="C133" t="str">
-        <v>TOO-COCLIQUIDOV</v>
+        <v>TOO-COCLIQUID</v>
       </c>
       <c r="D133" t="str">
         <v/>
@@ -10278,7 +10278,7 @@
         <v>XXS - Đầu tròn ULTRA</v>
       </c>
       <c r="C134" t="str">
-        <v>DAU-XXSDAUTRONTF</v>
+        <v>DAU-XXSDAUTRONUL</v>
       </c>
       <c r="D134" t="str">
         <v/>
@@ -10352,7 +10352,7 @@
         <v>Bào viên đạn</v>
       </c>
       <c r="C135" t="str">
-        <v>DAU-BAOVIENDANWH</v>
+        <v>DAU-BAOVIENDAN</v>
       </c>
       <c r="D135" t="str">
         <v/>
@@ -10426,7 +10426,7 @@
         <v>4XC Đầu tròn ULTRA</v>
       </c>
       <c r="C136" t="str">
-        <v>DAU-4XCDAUTRONXM</v>
+        <v>DAU-4XCDAUTRONUL</v>
       </c>
       <c r="D136" t="str">
         <v/>
@@ -10500,7 +10500,7 @@
         <v>Cán dao cạo chân - đen</v>
       </c>
       <c r="C137" t="str">
-        <v>TOO-CANDAOCAOCII</v>
+        <v>TOO-CANDAOCAOCHA2</v>
       </c>
       <c r="D137" t="str">
         <v/>
@@ -10574,7 +10574,7 @@
         <v>Nhũ đường - T</v>
       </c>
       <c r="C138" t="str">
-        <v>DES-NHUDUONGTAX</v>
+        <v>DES-NHUDUONGT</v>
       </c>
       <c r="D138" t="str">
         <v/>
@@ -10648,7 +10648,7 @@
         <v>Kem mềm da</v>
       </c>
       <c r="C139" t="str">
-        <v>HOA-KEMMEMDACC</v>
+        <v>HOA-KEMMEMDA</v>
       </c>
       <c r="D139" t="str">
         <v/>
@@ -10722,7 +10722,7 @@
         <v>Liquid mango</v>
       </c>
       <c r="C140" t="str">
-        <v>HOA-LIQUIDMANGZH</v>
+        <v>HOA-LIQUIDMANGO</v>
       </c>
       <c r="D140" t="str">
         <v/>
@@ -10796,7 +10796,7 @@
         <v>Vỏ nhám Mini - 100c</v>
       </c>
       <c r="C141" t="str">
-        <v>TOO-VONHAMMINIQJ</v>
+        <v>TOO-VONHAMMINI10</v>
       </c>
       <c r="D141" t="str">
         <v/>
@@ -10870,7 +10870,7 @@
         <v>Vỏ nhám Mini - 1000c</v>
       </c>
       <c r="C142" t="str">
-        <v>TOO-VONHAMMINIZU</v>
+        <v>TOO-VONHAMMINI102</v>
       </c>
       <c r="D142" t="str">
         <v/>
@@ -10944,7 +10944,7 @@
         <v>Vỏ nhám trắng ⌗150 - M</v>
       </c>
       <c r="C143" t="str">
-        <v>TOO-VONHAMTRANBY</v>
+        <v>TOO-VONHAMTRANG1</v>
       </c>
       <c r="D143" t="str">
         <v/>
@@ -11018,7 +11018,7 @@
         <v>Súng bào máy tím</v>
       </c>
       <c r="C144" t="str">
-        <v>DOD-SUNGBAOMAYJA</v>
+        <v>DOD-SUNGBAOMAYTI</v>
       </c>
       <c r="D144" t="str">
         <v/>
@@ -11092,7 +11092,7 @@
         <v>Vòng bi dưới máy tím - to</v>
       </c>
       <c r="C145" t="str">
-        <v>DOD-VONGBIDUOIMF</v>
+        <v>DOD-VONGBIDUOIMA</v>
       </c>
       <c r="D145" t="str">
         <v/>
@@ -11166,7 +11166,7 @@
         <v>Vòng bi dưới máy tím - nhỏ</v>
       </c>
       <c r="C146" t="str">
-        <v>DOD-VONGBIDUOIIP</v>
+        <v>DOD-VONGBIDUOIMA2</v>
       </c>
       <c r="D146" t="str">
         <v/>
@@ -11240,7 +11240,7 @@
         <v>Bột - Natural white</v>
       </c>
       <c r="C147" t="str">
-        <v>BOT-BOTNATURALIB</v>
+        <v>BOT-BOTNATURALWH</v>
       </c>
       <c r="D147" t="str">
         <v/>
@@ -11314,7 +11314,7 @@
         <v>Xô Gel Scrub - Mint 23KG</v>
       </c>
       <c r="C148" t="str">
-        <v>HOA-XOGELSCRUBMD</v>
+        <v>HOA-XOGELSCRUBMI</v>
       </c>
       <c r="D148" t="str">
         <v/>
@@ -11388,7 +11388,7 @@
         <v>Cuticle Oil - Pineapple 1gal</v>
       </c>
       <c r="C149" t="str">
-        <v>HOA-CUTICLEOILGS</v>
+        <v>HOA-CUTICLEOILPI</v>
       </c>
       <c r="D149" t="str">
         <v/>
@@ -11462,7 +11462,7 @@
         <v>Top coat tím Medium 500ml</v>
       </c>
       <c r="C150" t="str">
-        <v>TOP-TOPCOATTIMDK</v>
+        <v>TOP-TOPCOATTIMME</v>
       </c>
       <c r="D150" t="str">
         <v/>
@@ -11536,7 +11536,7 @@
         <v>Top coat tím Medium 15ml</v>
       </c>
       <c r="C151" t="str">
-        <v>TOP-TOPCOATTIMZO</v>
+        <v>TOP-TOPCOATTIMME2</v>
       </c>
       <c r="D151" t="str">
         <v/>
@@ -11610,7 +11610,7 @@
         <v>Color Acrylic powder 2oz</v>
       </c>
       <c r="C152" t="str">
-        <v>BOT-COLORACRYLPO</v>
+        <v>BOT-COLORACRYLIC</v>
       </c>
       <c r="D152" t="str">
         <v/>
@@ -11684,7 +11684,7 @@
         <v>Tay bào Trắng Korea</v>
       </c>
       <c r="C153" t="str">
-        <v>DOD-TAYBAOTRANVA</v>
+        <v>DOD-TAYBAOTRANGK</v>
       </c>
       <c r="D153" t="str">
         <v/>
@@ -11758,7 +11758,7 @@
         <v>Súng tay bào Trắng Korea</v>
       </c>
       <c r="C154" t="str">
-        <v>DOD-SUNGTAYBAOGI</v>
+        <v>DOD-SUNGTAYBAOTR</v>
       </c>
       <c r="D154" t="str">
         <v/>
@@ -11832,7 +11832,7 @@
         <v>Máy bào Korea Trắng</v>
       </c>
       <c r="C155" t="str">
-        <v>DOD-MAYBAOKOREQX</v>
+        <v>DOD-MAYBAOKOREAT</v>
       </c>
       <c r="D155" t="str">
         <v/>
@@ -11906,7 +11906,7 @@
         <v>Típ làm mẫu 20 màu 10 bảng/set</v>
       </c>
       <c r="C156" t="str">
-        <v>TOO-TIPLAMMAU2YW</v>
+        <v>TOO-TIPLAMMAU20M</v>
       </c>
       <c r="D156" t="str">
         <v/>
@@ -11980,7 +11980,7 @@
         <v>Tay cầm bấm móng inox</v>
       </c>
       <c r="C157" t="str">
-        <v>TOO-TAYCAMBAMMCI</v>
+        <v>TOO-TAYCAMBAMMON</v>
       </c>
       <c r="D157" t="str">
         <v/>
@@ -12054,7 +12054,7 @@
         <v>Dũa nhỏ Precision 100/100</v>
       </c>
       <c r="C158" t="str">
-        <v>DUA-DUANHOPRECRY</v>
+        <v>DUA-DUANHOPRECIS</v>
       </c>
       <c r="D158" t="str">
         <v/>
@@ -12128,7 +12128,7 @@
         <v>Tips natur ballerina ngắn</v>
       </c>
       <c r="C159" t="str">
-        <v>TIP-TIPSNATURBPA</v>
+        <v>TIP-TIPSNATURBAL</v>
       </c>
       <c r="D159" t="str">
         <v/>
@@ -12202,7 +12202,7 @@
         <v>Lõi súng G5</v>
       </c>
       <c r="C160" t="str">
-        <v>DOD-LOISUNGG5EQ</v>
+        <v>DOD-LOISUNGG5</v>
       </c>
       <c r="D160" t="str">
         <v/>
@@ -12276,7 +12276,7 @@
         <v>Dây tay máy tím 3 chân</v>
       </c>
       <c r="C161" t="str">
-        <v>DOD-DAYTAYMAYTSY</v>
+        <v>DOD-DAYTAYMAYTIM</v>
       </c>
       <c r="D161" t="str">
         <v/>
@@ -12350,7 +12350,7 @@
         <v>Bột - Intense Pink</v>
       </c>
       <c r="C162" t="str">
-        <v>BOT-BOTINTENSECQ</v>
+        <v>BOT-BOTINTENSEPI</v>
       </c>
       <c r="D162" t="str">
         <v/>
@@ -12424,7 +12424,7 @@
         <v>Bút đắp hoa 3D 2 đầu</v>
       </c>
       <c r="C163" t="str">
-        <v>BUT-BUTDAPHOA3DF</v>
+        <v>BUT-BUTDAPHOA3D2</v>
       </c>
       <c r="D163" t="str">
         <v/>
@@ -12498,7 +12498,7 @@
         <v>Bút đắp bột Davie sz16</v>
       </c>
       <c r="C164" t="str">
-        <v>BUT-BUTDAPBOTDUA</v>
+        <v>BUT-BUTDAPBOTDAV</v>
       </c>
       <c r="D164" t="str">
         <v/>
@@ -12572,7 +12572,7 @@
         <v>Chổi rắc nhũ</v>
       </c>
       <c r="C165" t="str">
-        <v>BUT-CHOIRACNHUEA</v>
+        <v>BUT-CHOIRACNHU</v>
       </c>
       <c r="D165" t="str">
         <v/>
@@ -12646,7 +12646,7 @@
         <v>Bút vẽ cọ</v>
       </c>
       <c r="C166" t="str">
-        <v>BUT-BUTVECOIJ</v>
+        <v>BUT-BUTVECO</v>
       </c>
       <c r="D166" t="str">
         <v/>
@@ -12720,7 +12720,7 @@
         <v>Bút vẽ hoa cúc</v>
       </c>
       <c r="C167" t="str">
-        <v>BUT-BUTVEHOACUUC</v>
+        <v>BUT-BUTVEHOACUC</v>
       </c>
       <c r="D167" t="str">
         <v/>
@@ -12794,7 +12794,7 @@
         <v>Dây cắm O japan</v>
       </c>
       <c r="C168" t="str">
-        <v>DOD-DAYCAMOJAPUB</v>
+        <v>DOD-DAYCAMOJAPAN</v>
       </c>
       <c r="D168" t="str">
         <v/>
@@ -12868,7 +12868,7 @@
         <v>Mịn thông XF</v>
       </c>
       <c r="C169" t="str">
-        <v>DAU-MINTHONGXFCV</v>
+        <v>DAU-MINTHONGXF</v>
       </c>
       <c r="D169" t="str">
         <v/>
@@ -12942,7 +12942,7 @@
         <v>5in1 Phá volcano 4XC</v>
       </c>
       <c r="C170" t="str">
-        <v>DAU-5IN1PHAVOLHJ</v>
+        <v>DAU-5IN1PHAVOLCA</v>
       </c>
       <c r="D170" t="str">
         <v/>
@@ -13016,7 +13016,7 @@
         <v>5XC</v>
       </c>
       <c r="C171" t="str">
-        <v>DAU-5XCVQ</v>
+        <v>DAU-5XC</v>
       </c>
       <c r="D171" t="str">
         <v/>
@@ -13090,7 +13090,7 @@
         <v>XXS đầu vác</v>
       </c>
       <c r="C172" t="str">
-        <v>DAU-XXSDAUVACRL</v>
+        <v>DAU-XXSDAUVAC</v>
       </c>
       <c r="D172" t="str">
         <v/>
@@ -13164,7 +13164,7 @@
         <v>Biển google review</v>
       </c>
       <c r="C173" t="str">
-        <v>TOO-BIENGOOGLEEL</v>
+        <v>TOO-BIENGOOGLERE</v>
       </c>
       <c r="D173" t="str">
         <v/>
@@ -13238,7 +13238,7 @@
         <v>Trục nhám Mini</v>
       </c>
       <c r="C174" t="str">
-        <v>TOO-TRUCNHAMMIDJ</v>
+        <v>TOO-TRUCNHAMMINI</v>
       </c>
       <c r="D174" t="str">
         <v/>
@@ -13312,7 +13312,7 @@
         <v>Bút gel - vuông 6</v>
       </c>
       <c r="C175" t="str">
-        <v>BUT-BUTGELVUONZV</v>
+        <v>BUT-BUTGELVUONG6</v>
       </c>
       <c r="D175" t="str">
         <v/>
@@ -13386,7 +13386,7 @@
         <v>Bút gel quét mầu - vuông 8</v>
       </c>
       <c r="C176" t="str">
-        <v>BUT-BUTGELQUETMT</v>
+        <v>BUT-BUTGELQUETMA2</v>
       </c>
       <c r="D176" t="str">
         <v/>
@@ -13460,7 +13460,7 @@
         <v>Keo DNS Pro 1s</v>
       </c>
       <c r="C177" t="str">
-        <v>HOA-KEODNSPRO1IH</v>
+        <v>HOA-KEODNSPRO1S</v>
       </c>
       <c r="D177" t="str">
         <v/>
@@ -13534,7 +13534,7 @@
         <v>Ultraschall reiniger 5L</v>
       </c>
       <c r="C178" t="str">
-        <v>HOA-ULTRASCHALOH</v>
+        <v>HOA-ULTRASCHALLR</v>
       </c>
       <c r="D178" t="str">
         <v/>
@@ -13608,7 +13608,7 @@
         <v>Kìm Nghĩa D555</v>
       </c>
       <c r="C179" t="str">
-        <v>TOO-KIMNGHIAD5UL</v>
+        <v>TOO-KIMNGHIAD555</v>
       </c>
       <c r="D179" t="str">
         <v/>
@@ -13682,7 +13682,7 @@
         <v>50ml - Gel đắp IBD PINK</v>
       </c>
       <c r="C180" t="str">
-        <v>GEL-50MLGELDAPZX</v>
+        <v>GEL-50MLGELDAPIB</v>
       </c>
       <c r="D180" t="str">
         <v/>
@@ -13756,7 +13756,7 @@
         <v>Chrome base coat 15ml</v>
       </c>
       <c r="C181" t="str">
-        <v>TOP-CHROMEBASERM</v>
+        <v>TOP-CHROMEBASECO</v>
       </c>
       <c r="D181" t="str">
         <v/>
@@ -13830,7 +13830,7 @@
         <v>Nam châm Mắt mèo thường</v>
       </c>
       <c r="C182" t="str">
-        <v>TOO-NAMCHAMMATNV</v>
+        <v>TOO-NAMCHAMMATME</v>
       </c>
       <c r="D182" t="str">
         <v/>
@@ -13904,7 +13904,7 @@
         <v>Chrome ngọc trai 1g</v>
       </c>
       <c r="C183" t="str">
-        <v>DES-CHROMENGOCYV</v>
+        <v>DES-CHROMENGOCTR</v>
       </c>
       <c r="D183" t="str">
         <v/>
@@ -13978,7 +13978,7 @@
         <v>Nhũ đường D hũ 50gram</v>
       </c>
       <c r="C184" t="str">
-        <v>DES-NHUDUONGDHPO</v>
+        <v>DES-NHUDUONGDHU5</v>
       </c>
       <c r="D184" t="str">
         <v/>
@@ -14052,7 +14052,7 @@
         <v>15ml top coat tím đặc</v>
       </c>
       <c r="C185" t="str">
-        <v>TOP-15MLTOPCOADM</v>
+        <v>TOP-15MLTOPCOATT2</v>
       </c>
       <c r="D185" t="str">
         <v/>
@@ -14126,7 +14126,7 @@
         <v>Khẩu trang y tế</v>
       </c>
       <c r="C186" t="str">
-        <v>TOO-KHAUTRANGYZH</v>
+        <v>TOO-KHAUTRANGYTE</v>
       </c>
       <c r="D186" t="str">
         <v/>
@@ -14200,7 +14200,7 @@
         <v>Bào nâng gầm</v>
       </c>
       <c r="C187" t="str">
-        <v>DAU-BAONANGGAMRV</v>
+        <v>DAU-BAONANGGAM</v>
       </c>
       <c r="D187" t="str">
         <v/>
@@ -14274,7 +14274,7 @@
         <v>4XC - Đầu tròn v2</v>
       </c>
       <c r="C188" t="str">
-        <v>DAU-4XCDAUTRONGO</v>
+        <v>DAU-4XCDAUTRONV2</v>
       </c>
       <c r="D188" t="str">
         <v/>
@@ -14348,7 +14348,7 @@
         <v>3in1 Mịn C - dài</v>
       </c>
       <c r="C189" t="str">
-        <v>DAU-3IN1MINCDAYW</v>
+        <v>DAU-3IN1MINCDAI</v>
       </c>
       <c r="D189" t="str">
         <v/>
@@ -14422,7 +14422,7 @@
         <v>Bút đắp bột - kim cương - sz18</v>
       </c>
       <c r="C190" t="str">
-        <v>BUT-BUTDAPBOTKQM</v>
+        <v>BUT-BUTDAPBOTKIM</v>
       </c>
       <c r="D190" t="str">
         <v/>
@@ -14496,7 +14496,7 @@
         <v>Nhám đỏ manicure</v>
       </c>
       <c r="C191" t="str">
-        <v>TOO-NHAMDOMANIUR</v>
+        <v>TOO-NHAMDOMANICU</v>
       </c>
       <c r="D191" t="str">
         <v/>
@@ -14570,7 +14570,7 @@
         <v>Máy bào Marathon 3 bạc</v>
       </c>
       <c r="C192" t="str">
-        <v>DOD-MAYBAOMARAPX</v>
+        <v>DOD-MAYBAOMARATH</v>
       </c>
       <c r="D192" t="str">
         <v/>
@@ -14644,7 +14644,7 @@
         <v>Dây cắm 3 châm Korea</v>
       </c>
       <c r="C193" t="str">
-        <v>DOD-DAYCAM3CHAYM</v>
+        <v>DOD-DAYCAM3CHAMK</v>
       </c>
       <c r="D193" t="str">
         <v/>
@@ -14718,7 +14718,7 @@
         <v>Đèn bàn LED đen</v>
       </c>
       <c r="C194" t="str">
-        <v>DOD-DENBANLEDDPX</v>
+        <v>DOD-DENBANLEDDEN</v>
       </c>
       <c r="D194" t="str">
         <v/>
@@ -14792,7 +14792,7 @@
         <v>Cốc nắp vặn liquid</v>
       </c>
       <c r="C195" t="str">
-        <v>TOO-COCNAPVANLPK</v>
+        <v>TOO-COCNAPVANLIQ</v>
       </c>
       <c r="D195" t="str">
         <v/>
@@ -14866,7 +14866,7 @@
         <v>Set lọ inox đựng bột liquid</v>
       </c>
       <c r="C196" t="str">
-        <v>TOO-SETLOINOXDXP</v>
+        <v>TOO-SETLOINOXDUN</v>
       </c>
       <c r="D196" t="str">
         <v/>
@@ -14940,7 +14940,7 @@
         <v>Kê bàn trưng bày</v>
       </c>
       <c r="C197" t="str">
-        <v>TOO-KEBANTRUNGYT</v>
+        <v>TOO-KEBANTRUNGBA</v>
       </c>
       <c r="D197" t="str">
         <v/>
@@ -15014,7 +15014,7 @@
         <v>Cốc đựng bột trái tim</v>
       </c>
       <c r="C198" t="str">
-        <v>TOO-COCDUNGBOTCG</v>
+        <v>TOO-COCDUNGBOTTR</v>
       </c>
       <c r="D198" t="str">
         <v/>
@@ -15088,7 +15088,7 @@
         <v>Hộp đựng dụng cụ</v>
       </c>
       <c r="C199" t="str">
-        <v>TOO-HOPDUNGDUNWT</v>
+        <v>TOO-HOPDUNGDUNGC</v>
       </c>
       <c r="D199" t="str">
         <v/>
@@ -15162,7 +15162,7 @@
         <v>Túi Đá nhỏ - bạc</v>
       </c>
       <c r="C200" t="str">
-        <v>DES-TUIDANHOBAXB</v>
+        <v>DES-TUIDANHOBAC</v>
       </c>
       <c r="D200" t="str">
         <v/>
@@ -15236,7 +15236,7 @@
         <v>Túi Đá nhỏ - 7 màu</v>
       </c>
       <c r="C201" t="str">
-        <v>DES-TUIDANHO7MKM</v>
+        <v>DES-TUIDANHO7MAU</v>
       </c>
       <c r="D201" t="str">
         <v/>
@@ -15310,7 +15310,7 @@
         <v>Biển mẫu 50 NailArt</v>
       </c>
       <c r="C202" t="str">
-        <v>TOO-BIENMAU50NWR</v>
+        <v>TOO-BIENMAU50NAI</v>
       </c>
       <c r="D202" t="str">
         <v/>
@@ -15384,7 +15384,7 @@
         <v>Típ cho bảng tip display</v>
       </c>
       <c r="C203" t="str">
-        <v>TOO-TIPCHOBANGHG</v>
+        <v>TOO-TIPCHOBANGTI</v>
       </c>
       <c r="D203" t="str">
         <v/>
@@ -15458,7 +15458,7 @@
         <v>Quyển bảng màu marble 160</v>
       </c>
       <c r="C204" t="str">
-        <v>TOO-QUYENBANGMOB</v>
+        <v>TOO-QUYENBANGMAU</v>
       </c>
       <c r="D204" t="str">
         <v/>
@@ -15532,7 +15532,7 @@
         <v>Quyển bảng màu gold 120</v>
       </c>
       <c r="C205" t="str">
-        <v>TOO-QUYENBANGMPV</v>
+        <v>TOO-QUYENBANGMAU2</v>
       </c>
       <c r="D205" t="str">
         <v/>
@@ -15606,7 +15606,7 @@
         <v>Quyển bảng màu gold 216</v>
       </c>
       <c r="C206" t="str">
-        <v>TOO-QUYENBANGMKU</v>
+        <v>TOO-QUYENBANGMAU3</v>
       </c>
       <c r="D206" t="str">
         <v/>
@@ -15680,7 +15680,7 @@
         <v>Quyển bảng màu to 300</v>
       </c>
       <c r="C207" t="str">
-        <v>TOO-QUYENBANGMRN</v>
+        <v>TOO-QUYENBANGMAU4</v>
       </c>
       <c r="D207" t="str">
         <v/>
@@ -15754,7 +15754,7 @@
         <v>Dũa nhỏ Precision 80/80</v>
       </c>
       <c r="C208" t="str">
-        <v>DUA-DUANHOPRECZP</v>
+        <v>DUA-DUANHOPRECIS2</v>
       </c>
       <c r="D208" t="str">
         <v/>
@@ -15828,7 +15828,7 @@
         <v>Đèn vòng bàn - trắng</v>
       </c>
       <c r="C209" t="str">
-        <v>DOD-DENVONGBANFW</v>
+        <v>DOD-DENVONGBANTR</v>
       </c>
       <c r="D209" t="str">
         <v/>
@@ -15902,7 +15902,7 @@
         <v>Thùng Túi y tế 4000c</v>
       </c>
       <c r="C210" t="str">
-        <v>PED-THUNGTUIYTPK</v>
+        <v>PED-THUNGTUIYTE4</v>
       </c>
       <c r="D210" t="str">
         <v/>
@@ -15976,7 +15976,7 @@
         <v>Thùng Mini buffer 1500c</v>
       </c>
       <c r="C211" t="str">
-        <v>PED-THUNGMINIBWK</v>
+        <v>PED-THUNGMINIBUF</v>
       </c>
       <c r="D211" t="str">
         <v/>
@@ -16050,7 +16050,7 @@
         <v>Thùng Dũa mini 5000c</v>
       </c>
       <c r="C212" t="str">
-        <v>PED-THUNGDUAMIJL</v>
+        <v>PED-THUNGDUAMINI</v>
       </c>
       <c r="D212" t="str">
         <v/>
@@ -16124,7 +16124,7 @@
         <v>5XC - Titan Xanh</v>
       </c>
       <c r="C213" t="str">
-        <v>DAU-5XCTITANXALD</v>
+        <v>DAU-5XCTITANXANH</v>
       </c>
       <c r="D213" t="str">
         <v/>
@@ -16198,7 +16198,7 @@
         <v>4XC - tròn nhỏ</v>
       </c>
       <c r="C214" t="str">
-        <v>DAU-4XCTRONNHOND</v>
+        <v>DAU-4XCTRONNHO</v>
       </c>
       <c r="D214" t="str">
         <v/>
@@ -16272,7 +16272,7 @@
         <v>Bút quan tài sz16</v>
       </c>
       <c r="C215" t="str">
-        <v>BUT-BUTQUANTAIRH</v>
+        <v>BUT-BUTQUANTAISZ2</v>
       </c>
       <c r="D215" t="str">
         <v/>
@@ -16346,7 +16346,7 @@
         <v>Tay bào Korea bạc</v>
       </c>
       <c r="C216" t="str">
-        <v>DOD-TAYBAOKORESA</v>
+        <v>DOD-TAYBAOKOREAB</v>
       </c>
       <c r="D216" t="str">
         <v/>
@@ -16420,7 +16420,7 @@
         <v>Chổi than japan</v>
       </c>
       <c r="C217" t="str">
-        <v>DOD-CHOITHANJABQ</v>
+        <v>DOD-CHOITHANJAPA</v>
       </c>
       <c r="D217" t="str">
         <v/>
@@ -16494,7 +16494,7 @@
         <v>Mài da khoé</v>
       </c>
       <c r="C218" t="str">
-        <v>DAU-MAIDAKHOEOT</v>
+        <v>DAU-MAIDAKHOE</v>
       </c>
       <c r="D218" t="str">
         <v/>
@@ -16568,7 +16568,7 @@
         <v>Bào mịn 3in1 - F</v>
       </c>
       <c r="C219" t="str">
-        <v>DAU-BAOMIN3IN1JE</v>
+        <v>DAU-BAOMIN3IN1F</v>
       </c>
       <c r="D219" t="str">
         <v/>
@@ -16642,7 +16642,7 @@
         <v>Đèn cầu vòng đính đá</v>
       </c>
       <c r="C220" t="str">
-        <v>DOD-DENCAUVONGMI</v>
+        <v>DOD-DENCAUVONGDI</v>
       </c>
       <c r="D220" t="str">
         <v/>
@@ -16716,7 +16716,7 @@
         <v>Chrome ngọc trai 7 màu</v>
       </c>
       <c r="C221" t="str">
-        <v>DES-CHROMENGOCWT</v>
+        <v>DES-CHROMENGOCTR2</v>
       </c>
       <c r="D221" t="str">
         <v/>
@@ -16790,7 +16790,7 @@
         <v>Chả gọt chân Inox</v>
       </c>
       <c r="C222" t="str">
-        <v>TOO-CHAGOTCHANKD</v>
+        <v>TOO-CHAGOTCHANIN</v>
       </c>
       <c r="D222" t="str">
         <v/>
@@ -16864,7 +16864,7 @@
         <v>Xốp kẹp chân 1000c</v>
       </c>
       <c r="C223" t="str">
-        <v>TOO-XOPKEPCHANBR</v>
+        <v>TOO-XOPKEPCHAN10</v>
       </c>
       <c r="D223" t="str">
         <v/>
@@ -16938,7 +16938,7 @@
         <v>Kê tay da - ghi</v>
       </c>
       <c r="C224" t="str">
-        <v>TOO-KETAYDAGHIIY</v>
+        <v>TOO-KETAYDAGHI</v>
       </c>
       <c r="D224" t="str">
         <v/>
@@ -17012,7 +17012,7 @@
         <v>Bào gầm khoé nhọn</v>
       </c>
       <c r="C225" t="str">
-        <v>DAU-BAOGAMKHOENC</v>
+        <v>DAU-BAOGAMKHOENH</v>
       </c>
       <c r="D225" t="str">
         <v/>
@@ -17086,7 +17086,7 @@
         <v>Bào gầm mỏng</v>
       </c>
       <c r="C226" t="str">
-        <v>DAU-BAOGAMMONGQV</v>
+        <v>DAU-BAOGAMMONG</v>
       </c>
       <c r="D226" t="str">
         <v/>
@@ -17160,7 +17160,7 @@
         <v>Chổi đánh bóng</v>
       </c>
       <c r="C227" t="str">
-        <v>DAU-CHOIDANHBOZV</v>
+        <v>DAU-CHOIDANHBONG</v>
       </c>
       <c r="D227" t="str">
         <v/>
@@ -17234,7 +17234,7 @@
         <v>Bào gầm răng thẳng</v>
       </c>
       <c r="C228" t="str">
-        <v>DAU-BAOGAMRANGOV</v>
+        <v>DAU-BAOGAMRANGTH</v>
       </c>
       <c r="D228" t="str">
         <v/>
@@ -17308,7 +17308,7 @@
         <v>5XC - đầu tròn</v>
       </c>
       <c r="C229" t="str">
-        <v>DAU-5XCDAUTRONLD</v>
+        <v>DAU-5XCDAUTRON</v>
       </c>
       <c r="D229" t="str">
         <v/>
@@ -17382,7 +17382,7 @@
         <v>M - to tròn</v>
       </c>
       <c r="C230" t="str">
-        <v>DAU-MTOTRONFL</v>
+        <v>DAU-MTOTRON</v>
       </c>
       <c r="D230" t="str">
         <v/>
@@ -17456,7 +17456,7 @@
         <v>M - nhỏ</v>
       </c>
       <c r="C231" t="str">
-        <v>DAU-MNHOAS</v>
+        <v>DAU-MNHO</v>
       </c>
       <c r="D231" t="str">
         <v/>
@@ -17530,7 +17530,7 @@
         <v>Bào mịn 3in1 - M</v>
       </c>
       <c r="C232" t="str">
-        <v>DAU-BAOMIN3IN1MU</v>
+        <v>DAU-BAOMIN3IN1M</v>
       </c>
       <c r="D232" t="str">
         <v/>
@@ -17604,7 +17604,7 @@
         <v>2XC Đầu vát</v>
       </c>
       <c r="C233" t="str">
-        <v>DAU-2XCDAUVATJP</v>
+        <v>DAU-2XCDAUVAT</v>
       </c>
       <c r="D233" t="str">
         <v/>
@@ -17678,7 +17678,7 @@
         <v>Bột màu 56g Nude collection</v>
       </c>
       <c r="C234" t="str">
-        <v>BOT-BOTMAU56GNNL</v>
+        <v>BOT-BOTMAU56GNUD</v>
       </c>
       <c r="D234" t="str">
         <v/>
@@ -17752,7 +17752,7 @@
         <v>Bột - VIP Natural Pink</v>
       </c>
       <c r="C235" t="str">
-        <v>BOT-BOTVIPNATUDN</v>
+        <v>BOT-BOTVIPNATURA</v>
       </c>
       <c r="D235" t="str">
         <v/>
@@ -17826,7 +17826,7 @@
         <v>Muối ngâm chân 5kg</v>
       </c>
       <c r="C236" t="str">
-        <v>PED-MUOINGAMCHRW</v>
+        <v>PED-MUOINGAMCHAN</v>
       </c>
       <c r="D236" t="str">
         <v/>
@@ -17900,7 +17900,7 @@
         <v>Sugar Scrub - Orange 20kg</v>
       </c>
       <c r="C237" t="str">
-        <v>PED-SUGARSCRUBHA</v>
+        <v>PED-SUGARSCRUBOR</v>
       </c>
       <c r="D237" t="str">
         <v/>
@@ -17974,7 +17974,7 @@
         <v>Kem Mango Vera 600ml</v>
       </c>
       <c r="C238" t="str">
-        <v>HOA-KEMMANGOVEHQ</v>
+        <v>HOA-KEMMANGOVERA</v>
       </c>
       <c r="D238" t="str">
         <v/>
@@ -18048,7 +18048,7 @@
         <v>Sơn Enjoy super trắng</v>
       </c>
       <c r="C239" t="str">
-        <v>HOA-SONENJOYSURV</v>
+        <v>HOA-SONENJOYSUPE</v>
       </c>
       <c r="D239" t="str">
         <v/>
@@ -18122,7 +18122,7 @@
         <v>Sơn Enjoy super đen</v>
       </c>
       <c r="C240" t="str">
-        <v>HOA-SONENJOYSUEZ</v>
+        <v>HOA-SONENJOYSUPE2</v>
       </c>
       <c r="D240" t="str">
         <v/>
@@ -18196,7 +18196,7 @@
         <v>Máy Ultraschall 2L</v>
       </c>
       <c r="C241" t="str">
-        <v>DOD-MAYULTRASCEN</v>
+        <v>DOD-MAYULTRASCHA</v>
       </c>
       <c r="D241" t="str">
         <v/>
@@ -18270,7 +18270,7 @@
         <v>Nhũ đường A 50g</v>
       </c>
       <c r="C242" t="str">
-        <v>DES-NHUDUONGA5ST</v>
+        <v>DES-NHUDUONGA50G</v>
       </c>
       <c r="D242" t="str">
         <v/>
@@ -18344,7 +18344,7 @@
         <v>Nhũ đường B 50g</v>
       </c>
       <c r="C243" t="str">
-        <v>DES-NHUDUONGB5VJ</v>
+        <v>DES-NHUDUONGB50G</v>
       </c>
       <c r="D243" t="str">
         <v/>
@@ -18418,7 +18418,7 @@
         <v>Nhũ đường C 50g</v>
       </c>
       <c r="C244" t="str">
-        <v>DES-NHUDUONGC5ZP</v>
+        <v>DES-NHUDUONGC50G</v>
       </c>
       <c r="D244" t="str">
         <v/>
@@ -18492,7 +18492,7 @@
         <v>Nhũ bạc phản quang mịn R1 50g</v>
       </c>
       <c r="C245" t="str">
-        <v>DES-NHUBACPHANKW</v>
+        <v>DES-NHUBACPHANQU</v>
       </c>
       <c r="D245" t="str">
         <v/>
@@ -18566,7 +18566,7 @@
         <v>Bát nhựa ngâm tay</v>
       </c>
       <c r="C246" t="str">
-        <v>TOO-BATNHUANGAWW</v>
+        <v>TOO-BATNHUANGAMT</v>
       </c>
       <c r="D246" t="str">
         <v/>
@@ -18640,7 +18640,7 @@
         <v>Bạc Foil 3g</v>
       </c>
       <c r="C247" t="str">
-        <v>DES-BACFOIL3GQC</v>
+        <v>DES-BACFOIL3G</v>
       </c>
       <c r="D247" t="str">
         <v/>
@@ -18714,7 +18714,7 @@
         <v>Típ làm mẫu trong tròn 50c set</v>
       </c>
       <c r="C248" t="str">
-        <v>TOO-TIPLAMMAUTXJ</v>
+        <v>TOO-TIPLAMMAUTRO</v>
       </c>
       <c r="D248" t="str">
         <v/>
@@ -18788,7 +18788,7 @@
         <v>Nam châm mắt mèo - 5in1</v>
       </c>
       <c r="C249" t="str">
-        <v>TOO-NAMCHAMMATQE</v>
+        <v>TOO-NAMCHAMMATME2</v>
       </c>
       <c r="D249" t="str">
         <v/>
@@ -18862,7 +18862,7 @@
         <v>Chổi vệ sinh đầu mài</v>
       </c>
       <c r="C250" t="str">
-        <v>TOO-CHOIVESINHHE</v>
+        <v>TOO-CHOIVESINHDA</v>
       </c>
       <c r="D250" t="str">
         <v/>
@@ -18936,7 +18936,7 @@
         <v>Chai sơn không 15ml</v>
       </c>
       <c r="C251" t="str">
-        <v>TOO-CHAISONKHOLF</v>
+        <v>TOO-CHAISONKHONG</v>
       </c>
       <c r="D251" t="str">
         <v/>
@@ -19010,7 +19010,7 @@
         <v>Chai primer không 15ml</v>
       </c>
       <c r="C252" t="str">
-        <v>TOO-CHAIPRIMERSH</v>
+        <v>TOO-CHAIPRIMERKH</v>
       </c>
       <c r="D252" t="str">
         <v/>
@@ -19084,7 +19084,7 @@
         <v>Chai bond không 15ml</v>
       </c>
       <c r="C253" t="str">
-        <v>TOO-CHAIBONDKHWS</v>
+        <v>TOO-CHAIBONDKHON</v>
       </c>
       <c r="D253" t="str">
         <v/>
@@ -19158,7 +19158,7 @@
         <v>Hộp đựng phá tròn trắng</v>
       </c>
       <c r="C254" t="str">
-        <v>TOO-HOPDUNGPHAFQ</v>
+        <v>TOO-HOPDUNGPHATR</v>
       </c>
       <c r="D254" t="str">
         <v/>
@@ -19232,7 +19232,7 @@
         <v>Bút cán gỗ sz16</v>
       </c>
       <c r="C255" t="str">
-        <v>BUT-BUTCANGOSZCG</v>
+        <v>BUT-BUTCANGOSZ16</v>
       </c>
       <c r="D255" t="str">
         <v/>
@@ -19306,7 +19306,7 @@
         <v>Bút đắp bột - kim cương - sz16</v>
       </c>
       <c r="C256" t="str">
-        <v>BUT-BUTDAPBOTKBW</v>
+        <v>BUT-BUTDAPBOTKIM2</v>
       </c>
       <c r="D256" t="str">
         <v/>
@@ -19380,7 +19380,7 @@
         <v>Tay bào trắng Korea SH20N</v>
       </c>
       <c r="C257" t="str">
-        <v>DOD-TAYBAOTRANMV</v>
+        <v>DOD-TAYBAOTRANGK2</v>
       </c>
       <c r="D257" t="str">
         <v/>
@@ -19454,7 +19454,7 @@
         <v>Vòng bi to Japan</v>
       </c>
       <c r="C258" t="str">
-        <v>TOO-VONGBITOJAOT</v>
+        <v>TOO-VONGBITOJAPA</v>
       </c>
       <c r="D258" t="str">
         <v/>
@@ -19528,7 +19528,7 @@
         <v>Vòng bi nhỏ Japan</v>
       </c>
       <c r="C259" t="str">
-        <v>TOO-VONGBINHOJUN</v>
+        <v>TOO-VONGBINHOJAP</v>
       </c>
       <c r="D259" t="str">
         <v/>
@@ -19602,7 +19602,7 @@
         <v>1KG - Gel đắp CLEAR</v>
       </c>
       <c r="C260" t="str">
-        <v>GEL-1KGGELDAPCTU</v>
+        <v>GEL-1KGGELDAPCLE</v>
       </c>
       <c r="D260" t="str">
         <v/>
@@ -19676,7 +19676,7 @@
         <v>1KG - Gel đắp NATURAL PINK</v>
       </c>
       <c r="C261" t="str">
-        <v>GEL-1KGGELDAPNJI</v>
+        <v>GEL-1KGGELDAPNAT</v>
       </c>
       <c r="D261" t="str">
         <v/>
@@ -19750,7 +19750,7 @@
         <v>1KG - Gel đắp MAKEUP ⌗1</v>
       </c>
       <c r="C262" t="str">
-        <v>GEL-1KGGELDAPMHL</v>
+        <v>GEL-1KGGELDAPMAK</v>
       </c>
       <c r="D262" t="str">
         <v/>
@@ -19824,7 +19824,7 @@
         <v>1KG - Gel đắp MAKEUP ⌗2</v>
       </c>
       <c r="C263" t="str">
-        <v>GEL-1KGGELDAPMZQ</v>
+        <v>GEL-1KGGELDAPMAK2</v>
       </c>
       <c r="D263" t="str">
         <v/>
@@ -19898,7 +19898,7 @@
         <v>1KG - Gel đắp MAKEUP ⌗3</v>
       </c>
       <c r="C264" t="str">
-        <v>GEL-1KGGELDAPMGO</v>
+        <v>GEL-1KGGELDAPMAK3</v>
       </c>
       <c r="D264" t="str">
         <v/>
@@ -19972,7 +19972,7 @@
         <v>Cắt fen thường</v>
       </c>
       <c r="C265" t="str">
-        <v>TOO-CATFENTHUOVP</v>
+        <v>TOO-CATFENTHUONG</v>
       </c>
       <c r="D265" t="str">
         <v/>
@@ -20046,7 +20046,7 @@
         <v>Cắt fen sâu - E</v>
       </c>
       <c r="C266" t="str">
-        <v>TOO-CATFENSAUEJH</v>
+        <v>TOO-CATFENSAUE</v>
       </c>
       <c r="D266" t="str">
         <v/>
@@ -20120,7 +20120,7 @@
         <v>XXS ULTRA</v>
       </c>
       <c r="C267" t="str">
-        <v>DAU-XXSULTRAEL</v>
+        <v>DAU-XXSULTRA</v>
       </c>
       <c r="D267" t="str">
         <v/>
@@ -20194,7 +20194,7 @@
         <v>XC - tròn</v>
       </c>
       <c r="C268" t="str">
-        <v>DAU-XCTRONEM</v>
+        <v>DAU-XCTRON</v>
       </c>
       <c r="D268" t="str">
         <v/>
@@ -20268,7 +20268,7 @@
         <v>Bào Mịn SM</v>
       </c>
       <c r="C269" t="str">
-        <v>DAU-BAOMINSMID</v>
+        <v>DAU-BAOMINSM</v>
       </c>
       <c r="D269" t="str">
         <v/>
@@ -20342,7 +20342,7 @@
         <v>C - bào lửa</v>
       </c>
       <c r="C270" t="str">
-        <v>DAU-CBAOLUAEQ</v>
+        <v>DAU-CBAOLUA</v>
       </c>
       <c r="D270" t="str">
         <v/>
@@ -20416,7 +20416,7 @@
         <v>Bào khoé tròn</v>
       </c>
       <c r="C271" t="str">
-        <v>DAU-BAOKHOETROEL</v>
+        <v>DAU-BAOKHOETRON</v>
       </c>
       <c r="D271" t="str">
         <v/>
@@ -20490,7 +20490,7 @@
         <v>XXS Hoa cúc ULTRA</v>
       </c>
       <c r="C272" t="str">
-        <v>DAU-XXSHOACUCUPL</v>
+        <v>DAU-XXSHOACUCULT</v>
       </c>
       <c r="D272" t="str">
         <v/>
@@ -20564,7 +20564,7 @@
         <v>Base coat 15ml</v>
       </c>
       <c r="C273" t="str">
-        <v>HOA-BASECOAT15LS</v>
+        <v>HOA-BASECOAT15ML</v>
       </c>
       <c r="D273" t="str">
         <v/>
@@ -20638,7 +20638,7 @@
         <v>Sơn màu SORAH 15ml</v>
       </c>
       <c r="C274" t="str">
-        <v>SON-SONMAUSORABU</v>
+        <v>SON-SONMAUSORAH1</v>
       </c>
       <c r="D274" t="str">
         <v/>
@@ -20712,7 +20712,7 @@
         <v>SORAH 144 quyển màu</v>
       </c>
       <c r="C275" t="str">
-        <v>SON-SORAH144QUST</v>
+        <v>SON-SORAH144QUYE</v>
       </c>
       <c r="D275" t="str">
         <v/>
@@ -20786,7 +20786,7 @@
         <v>Máy hút bụi bàn di dộng</v>
       </c>
       <c r="C276" t="str">
-        <v>DOD-MAYHUTBUIBFS</v>
+        <v>DOD-MAYHUTBUIBAN</v>
       </c>
       <c r="D276" t="str">
         <v/>
@@ -20860,7 +20860,7 @@
         <v>Dũa Bông hoa đen 80/80</v>
       </c>
       <c r="C277" t="str">
-        <v>DUA-DUABONGHOABE</v>
+        <v>DUA-DUABONGHOADE</v>
       </c>
       <c r="D277" t="str">
         <v/>
@@ -20934,7 +20934,7 @@
         <v>Tip Thẳng Straight jet - Lẻ (50c)</v>
       </c>
       <c r="C278" t="str">
-        <v>TIP-TIPTHANGSTNX</v>
+        <v>TIP-TIPTHANGSTRA</v>
       </c>
       <c r="D278" t="str">
         <v/>
@@ -21008,7 +21008,7 @@
         <v>Vỏ nhám trắng ⌗150 (1000c)</v>
       </c>
       <c r="C279" t="str">
-        <v>TOO-VONHAMTRANRM</v>
+        <v>TOO-VONHAMTRANG12</v>
       </c>
       <c r="D279" t="str">
         <v/>
@@ -21082,7 +21082,7 @@
         <v>Vỏ nhám trắng ⌗120 - C (1000c)</v>
       </c>
       <c r="C280" t="str">
-        <v>TOO-VONHAMTRANYR</v>
+        <v>TOO-VONHAMTRANG13</v>
       </c>
       <c r="D280" t="str">
         <v/>
@@ -21156,7 +21156,7 @@
         <v>Vỏ nhám trắng ⌗180 - F (1000c)</v>
       </c>
       <c r="C281" t="str">
-        <v>TOO-VONHAMTRANBC</v>
+        <v>TOO-VONHAMTRANG14</v>
       </c>
       <c r="D281" t="str">
         <v/>
@@ -21230,7 +21230,7 @@
         <v>Set Hộp đá - 7 màu</v>
       </c>
       <c r="C282" t="str">
-        <v>DES-SETHOPDA7MEH</v>
+        <v>DES-SETHOPDA7MAU</v>
       </c>
       <c r="D282" t="str">
         <v/>
@@ -21304,7 +21304,7 @@
         <v>Set Hộp đá - bạc</v>
       </c>
       <c r="C283" t="str">
-        <v>DES-SETHOPDABAMS</v>
+        <v>DES-SETHOPDABAC</v>
       </c>
       <c r="D283" t="str">
         <v/>
@@ -21378,7 +21378,7 @@
         <v>Set Hộp đá - vàng</v>
       </c>
       <c r="C284" t="str">
-        <v>DOD-SETHOPDAVAIF</v>
+        <v>DOD-SETHOPDAVANG</v>
       </c>
       <c r="D284" t="str">
         <v/>
@@ -21452,7 +21452,7 @@
         <v>Set Hộp đá - chữ vàng</v>
       </c>
       <c r="C285" t="str">
-        <v>DES-SETHOPDACHZT</v>
+        <v>DES-SETHOPDACHUV</v>
       </c>
       <c r="D285" t="str">
         <v/>
@@ -21526,7 +21526,7 @@
         <v>Kem Mango Vera 5kg</v>
       </c>
       <c r="C286" t="str">
-        <v>HOA-KEMMANGOVEWU</v>
+        <v>HOA-KEMMANGOVERA2</v>
       </c>
       <c r="D286" t="str">
         <v/>
@@ -21600,7 +21600,7 @@
         <v>Callus Remover 5kg</v>
       </c>
       <c r="C287" t="str">
-        <v>PED-CALLUSREMOME</v>
+        <v>PED-CALLUSREMOVE</v>
       </c>
       <c r="D287" t="str">
         <v/>
@@ -21674,7 +21674,7 @@
         <v>Xô Muối ngâm chân - mịn 23kg</v>
       </c>
       <c r="C288" t="str">
-        <v>HOA-XOMUOINGAMQE</v>
+        <v>HOA-XOMUOINGAMCH</v>
       </c>
       <c r="D288" t="str">
         <v/>
@@ -21748,7 +21748,7 @@
         <v>Chổi quét bàn to</v>
       </c>
       <c r="C289" t="str">
-        <v>TOO-CHOIQUETBARI</v>
+        <v>TOO-CHOIQUETBANT</v>
       </c>
       <c r="D289" t="str">
         <v/>
@@ -21822,7 +21822,7 @@
         <v>4XC đầu vát</v>
       </c>
       <c r="C290" t="str">
-        <v>DAU-4XCDAUVATTZ</v>
+        <v>DAU-4XCDAUVAT</v>
       </c>
       <c r="D290" t="str">
         <v/>
@@ -21896,7 +21896,7 @@
         <v>Kìm Nghĩa D01 Mũi 16</v>
       </c>
       <c r="C291" t="str">
-        <v>TOO-KIMNGHIAD0HS</v>
+        <v>TOO-KIMNGHIAD01M</v>
       </c>
       <c r="D291" t="str">
         <v/>
@@ -21970,7 +21970,7 @@
         <v>Cây đẩy da</v>
       </c>
       <c r="C292" t="str">
-        <v>TOO-CAYDAYDAUT</v>
+        <v>TOO-CAYDAYDA</v>
       </c>
       <c r="D292" t="str">
         <v/>
@@ -22044,7 +22044,7 @@
         <v>Aceton 5L</v>
       </c>
       <c r="C293" t="str">
-        <v>HOA-ACETON5LVY</v>
+        <v>HOA-ACETON5L</v>
       </c>
       <c r="D293" t="str">
         <v/>
@@ -22118,7 +22118,7 @@
         <v>Cồn IPA70 5L</v>
       </c>
       <c r="C294" t="str">
-        <v>HOA-CONIPA705LWG</v>
+        <v>HOA-CONIPA705L</v>
       </c>
       <c r="D294" t="str">
         <v/>
@@ -22192,7 +22192,7 @@
         <v>Aceton 1L</v>
       </c>
       <c r="C295" t="str">
-        <v>HOA-ACETON1LZP</v>
+        <v>HOA-ACETON1L</v>
       </c>
       <c r="D295" t="str">
         <v/>
@@ -22266,7 +22266,7 @@
         <v>Típ thường 50c</v>
       </c>
       <c r="C296" t="str">
-        <v>TOO-TIPTHUONG5VH</v>
+        <v>TOO-TIPTHUONG50C</v>
       </c>
       <c r="D296" t="str">
         <v/>
@@ -22340,7 +22340,7 @@
         <v>Gel vẽ trắng French 50ml</v>
       </c>
       <c r="C297" t="str">
-        <v>DES-GELVETRANGJG</v>
+        <v>DES-GELVETRANGFR</v>
       </c>
       <c r="D297" t="str">
         <v/>
@@ -22414,7 +22414,7 @@
         <v>Sơn màu Milky White 15ml</v>
       </c>
       <c r="C298" t="str">
-        <v>SON-SONMAUMILKIQ</v>
+        <v>SON-SONMAUMILKYW</v>
       </c>
       <c r="D298" t="str">
         <v/>
@@ -22488,7 +22488,7 @@
         <v>Flash Disco Cat Eye 12 màu</v>
       </c>
       <c r="C299" t="str">
-        <v>SON-FLASHDISCOTX</v>
+        <v>SON-FLASHDISCOCA</v>
       </c>
       <c r="D299" t="str">
         <v/>
@@ -22562,7 +22562,7 @@
         <v>Set Phấn nén làm ombre</v>
       </c>
       <c r="C300" t="str">
-        <v>DES-SETPHANNENWH</v>
+        <v>DES-SETPHANNENLA</v>
       </c>
       <c r="D300" t="str">
         <v/>
@@ -22636,7 +22636,7 @@
         <v>1KG - Gel đắp MILKY WHITE</v>
       </c>
       <c r="C301" t="str">
-        <v>GEL-1KGGELDAPMCI</v>
+        <v>GEL-1KGGELDAPMIL</v>
       </c>
       <c r="D301" t="str">
         <v/>
@@ -22710,7 +22710,7 @@
         <v>1KG - Gel đắp MILKY PINK</v>
       </c>
       <c r="C302" t="str">
-        <v>GEL-1KGGELDAPMZV</v>
+        <v>GEL-1KGGELDAPMIL2</v>
       </c>
       <c r="D302" t="str">
         <v/>
@@ -22784,7 +22784,7 @@
         <v>M - to</v>
       </c>
       <c r="C303" t="str">
-        <v>DAU-MTODE</v>
+        <v>DAU-MTO</v>
       </c>
       <c r="D303" t="str">
         <v/>
@@ -22858,7 +22858,7 @@
         <v>Bào gầm 2.0</v>
       </c>
       <c r="C304" t="str">
-        <v>DAU-BAOGAM20WL</v>
+        <v>DAU-BAOGAM20</v>
       </c>
       <c r="D304" t="str">
         <v/>
@@ -22932,7 +22932,7 @@
         <v>Phá Shellac</v>
       </c>
       <c r="C305" t="str">
-        <v>DAU-PHASHELLACVD</v>
+        <v>DAU-PHASHELLAC</v>
       </c>
       <c r="D305" t="str">
         <v/>
@@ -23006,7 +23006,7 @@
         <v>Mịn thông M</v>
       </c>
       <c r="C306" t="str">
-        <v>DAU-MINTHONGMHO</v>
+        <v>DAU-MINTHONGM</v>
       </c>
       <c r="D306" t="str">
         <v/>
@@ -23080,7 +23080,7 @@
         <v>Top coat tím đặc 500ml</v>
       </c>
       <c r="C307" t="str">
-        <v>TOP-TOPCOATTIMMF</v>
+        <v>TOP-TOPCOATTIMDA</v>
       </c>
       <c r="D307" t="str">
         <v/>
@@ -23154,7 +23154,7 @@
         <v>Liner gel vẽ Platinum</v>
       </c>
       <c r="C308" t="str">
-        <v>DES-LINERGELVEDL</v>
+        <v>DES-LINERGELVEPL</v>
       </c>
       <c r="D308" t="str">
         <v/>
@@ -23228,7 +23228,7 @@
         <v>Đèn bàn trắng 18W</v>
       </c>
       <c r="C309" t="str">
-        <v>DOD-DENBANTRANGL</v>
+        <v>DOD-DENBANTRANG1</v>
       </c>
       <c r="D309" t="str">
         <v/>
@@ -23302,7 +23302,7 @@
         <v>Dũa mỏng nhỏ tròn 100/100</v>
       </c>
       <c r="C310" t="str">
-        <v>DUA-DUAMONGNHOWG</v>
+        <v>DUA-DUAMONGNHOTR</v>
       </c>
       <c r="D310" t="str">
         <v/>
@@ -23376,7 +23376,7 @@
         <v>Dũa mỏng nhỏ tròn 80/80</v>
       </c>
       <c r="C311" t="str">
-        <v>DUA-DUAMONGNHODK</v>
+        <v>DUA-DUAMONGNHOTR2</v>
       </c>
       <c r="D311" t="str">
         <v/>
@@ -23450,7 +23450,7 @@
         <v>Bột - Clear Nhanh khô</v>
       </c>
       <c r="C312" t="str">
-        <v>BOT-BOTCLEARNHUL</v>
+        <v>BOT-BOTCLEARNHAN</v>
       </c>
       <c r="D312" t="str">
         <v/>
@@ -23524,7 +23524,7 @@
         <v>Bột - Natural Dark Pink</v>
       </c>
       <c r="C313" t="str">
-        <v>BOT-BOTNATURALSP</v>
+        <v>BOT-BOTNATURALDA</v>
       </c>
       <c r="D313" t="str">
         <v/>
@@ -23598,7 +23598,7 @@
         <v>Chrome base coat 250ml</v>
       </c>
       <c r="C314" t="str">
-        <v>HOA-CHROMEBASEAK</v>
+        <v>HOA-CHROMEBASECO</v>
       </c>
       <c r="D314" t="str">
         <v/>
@@ -23672,7 +23672,7 @@
         <v>Giấy làm chân 50x70cm</v>
       </c>
       <c r="C315" t="str">
-        <v>TOO-GIAYLAMCHAVJ</v>
+        <v>TOO-GIAYLAMCHAN5</v>
       </c>
       <c r="D315" t="str">
         <v/>
@@ -23746,7 +23746,7 @@
         <v>Găng tay Nitril đen - S</v>
       </c>
       <c r="C316" t="str">
-        <v>TOO-GANGTAYNITNX</v>
+        <v>TOO-GANGTAYNITRI</v>
       </c>
       <c r="D316" t="str">
         <v/>
@@ -23820,7 +23820,7 @@
         <v>Găng tay Nitril đen - M</v>
       </c>
       <c r="C317" t="str">
-        <v>TOO-GANGTAYNITDO</v>
+        <v>TOO-GANGTAYNITRI2</v>
       </c>
       <c r="D317" t="str">
         <v/>
@@ -23894,7 +23894,7 @@
         <v>Vỏ nhám tím ⌗150 - M</v>
       </c>
       <c r="C318" t="str">
-        <v>TOO-VONHAMTIM1NP</v>
+        <v>TOO-VONHAMTIM150</v>
       </c>
       <c r="D318" t="str">
         <v/>
@@ -23968,7 +23968,7 @@
         <v>Cốc đựng bột nhỏ</v>
       </c>
       <c r="C319" t="str">
-        <v>TOO-COCDUNGBOTMU</v>
+        <v>TOO-COCDUNGBOTNH</v>
       </c>
       <c r="D319" t="str">
         <v/>
@@ -24042,7 +24042,7 @@
         <v>Hộp đựng tip 0-10</v>
       </c>
       <c r="C320" t="str">
-        <v>TOO-HOPDUNGTIPIH</v>
+        <v>TOO-HOPDUNGTIP01</v>
       </c>
       <c r="D320" t="str">
         <v/>
@@ -24116,7 +24116,7 @@
         <v>Típ làm mẫu 36 màu</v>
       </c>
       <c r="C321" t="str">
-        <v>TOO-TIPLAMMAU3HQ</v>
+        <v>TOO-TIPLAMMAU36M</v>
       </c>
       <c r="D321" t="str">
         <v/>
@@ -24190,7 +24190,7 @@
         <v>Kê tay cao - hồng</v>
       </c>
       <c r="C322" t="str">
-        <v>TOO-KETAYCAOHODP</v>
+        <v>TOO-KETAYCAOHONG</v>
       </c>
       <c r="D322" t="str">
         <v/>
@@ -24264,7 +24264,7 @@
         <v>Kê tay cao - be</v>
       </c>
       <c r="C323" t="str">
-        <v>TOO-KETAYCAOBEUH</v>
+        <v>TOO-KETAYCAOBE</v>
       </c>
       <c r="D323" t="str">
         <v/>
@@ -24338,7 +24338,7 @@
         <v>Kê tay cao - vàng</v>
       </c>
       <c r="C324" t="str">
-        <v>TOO-KETAYCAOVAEY</v>
+        <v>TOO-KETAYCAOVANG</v>
       </c>
       <c r="D324" t="str">
         <v/>
@@ -24412,7 +24412,7 @@
         <v>Máy bào di động - đen</v>
       </c>
       <c r="C325" t="str">
-        <v>DOD-MAYBAODIDOIK</v>
+        <v>DOD-MAYBAODIDONG</v>
       </c>
       <c r="D325" t="str">
         <v/>
@@ -24486,7 +24486,7 @@
         <v>Đèn pin cầm tay v2</v>
       </c>
       <c r="C326" t="str">
-        <v>DOD-DENPINCAMTKW</v>
+        <v>DOD-DENPINCAMTAY</v>
       </c>
       <c r="D326" t="str">
         <v/>
@@ -24560,7 +24560,7 @@
         <v>Pin thay đèn sạc</v>
       </c>
       <c r="C327" t="str">
-        <v>DOD-PINTHAYDENHS</v>
+        <v>DOD-PINTHAYDENSA</v>
       </c>
       <c r="D327" t="str">
         <v/>
@@ -24634,7 +24634,7 @@
         <v>Tinh dầu trị nấm 15ml</v>
       </c>
       <c r="C328" t="str">
-        <v>HOA-TINHDAUTRIOV</v>
+        <v>HOA-TINHDAUTRINA</v>
       </c>
       <c r="D328" t="str">
         <v/>
@@ -24708,7 +24708,7 @@
         <v>Nước cầm máu</v>
       </c>
       <c r="C329" t="str">
-        <v>HOA-NUOCCAMMAUSZ</v>
+        <v>HOA-NUOCCAMMAU</v>
       </c>
       <c r="D329" t="str">
         <v/>
@@ -24782,7 +24782,7 @@
         <v>Bột - Natural pink</v>
       </c>
       <c r="C330" t="str">
-        <v>BOT-BOTNATURALQF</v>
+        <v>BOT-BOTNATURALPI</v>
       </c>
       <c r="D330" t="str">
         <v/>
@@ -24856,7 +24856,7 @@
         <v>Bột - Crystal clear</v>
       </c>
       <c r="C331" t="str">
-        <v>BOT-BOTCRYSTALJX</v>
+        <v>BOT-BOTCRYSTALCL</v>
       </c>
       <c r="D331" t="str">
         <v/>
@@ -24930,7 +24930,7 @@
         <v>Liquid Mango J2000M C2</v>
       </c>
       <c r="C332" t="str">
-        <v>HOA-LIQUIDMANGOP</v>
+        <v>HOA-LIQUIDMANGOJ</v>
       </c>
       <c r="D332" t="str">
         <v/>
@@ -25004,7 +25004,7 @@
         <v>Liquid J-2000 C2</v>
       </c>
       <c r="C333" t="str">
-        <v>HOA-LIQUIDJ200BT</v>
+        <v>HOA-LIQUIDJ2000C</v>
       </c>
       <c r="D333" t="str">
         <v/>
@@ -25078,7 +25078,7 @@
         <v>Liquid J2000 C0</v>
       </c>
       <c r="C334" t="str">
-        <v>HOA-LIQUIDJ200BJ</v>
+        <v>HOA-LIQUIDJ2000C2</v>
       </c>
       <c r="D334" t="str">
         <v/>
@@ -25152,7 +25152,7 @@
         <v>Bột - Super white</v>
       </c>
       <c r="C335" t="str">
-        <v>BOT-BOTSUPERWHGA</v>
+        <v>BOT-BOTSUPERWHIT</v>
       </c>
       <c r="D335" t="str">
         <v/>
@@ -25226,7 +25226,7 @@
         <v>Bột - Ombre white</v>
       </c>
       <c r="C336" t="str">
-        <v>BOT-BOTOMBREWHCG</v>
+        <v>BOT-BOTOMBREWHIT</v>
       </c>
       <c r="D336" t="str">
         <v/>
@@ -25300,7 +25300,7 @@
         <v>Bột - Milky white</v>
       </c>
       <c r="C337" t="str">
-        <v>BOT-BOTMILKYWHEM</v>
+        <v>BOT-BOTMILKYWHIT</v>
       </c>
       <c r="D337" t="str">
         <v/>
@@ -25374,7 +25374,7 @@
         <v>Bột - Makeup nude</v>
       </c>
       <c r="C338" t="str">
-        <v>BOT-BOTMAKEUPNCD</v>
+        <v>BOT-BOTMAKEUPNUD</v>
       </c>
       <c r="D338" t="str">
         <v/>
@@ -25448,7 +25448,7 @@
         <v>Bột - Makeup peach</v>
       </c>
       <c r="C339" t="str">
-        <v>BOT-BOTMAKEUPPRS</v>
+        <v>BOT-BOTMAKEUPPEA</v>
       </c>
       <c r="D339" t="str">
         <v/>
@@ -25522,7 +25522,7 @@
         <v>Bột - Makeup pink</v>
       </c>
       <c r="C340" t="str">
-        <v>BOT-BOTMAKEUPPZN</v>
+        <v>BOT-BOTMAKEUPPIN</v>
       </c>
       <c r="D340" t="str">
         <v/>
@@ -25596,7 +25596,7 @@
         <v>Bột - Clear</v>
       </c>
       <c r="C341" t="str">
-        <v>BOT-BOTCLEARTL</v>
+        <v>BOT-BOTCLEAR</v>
       </c>
       <c r="D341" t="str">
         <v/>
@@ -25670,7 +25670,7 @@
         <v>Primer 500ml</v>
       </c>
       <c r="C342" t="str">
-        <v>HOA-PRIMER500MYX</v>
+        <v>HOA-PRIMER500ML</v>
       </c>
       <c r="D342" t="str">
         <v/>
@@ -25744,7 +25744,7 @@
         <v>Bond dry 500ml</v>
       </c>
       <c r="C343" t="str">
-        <v>HOA-BONDDRY500BP</v>
+        <v>HOA-BONDDRY500ML</v>
       </c>
       <c r="D343" t="str">
         <v/>
@@ -25818,7 +25818,7 @@
         <v>Tay bào Marathon bạc</v>
       </c>
       <c r="C344" t="str">
-        <v>DOD-TAYBAOMARARO</v>
+        <v>DOD-TAYBAOMARATH</v>
       </c>
       <c r="D344" t="str">
         <v/>
@@ -25892,7 +25892,7 @@
         <v>Cắt fen thường USA</v>
       </c>
       <c r="C345" t="str">
-        <v>TOO-CATFENTHUOID</v>
+        <v>TOO-CATFENTHUONG2</v>
       </c>
       <c r="D345" t="str">
         <v/>
@@ -25966,7 +25966,7 @@
         <v>Cắt fen sâu USA</v>
       </c>
       <c r="C346" t="str">
-        <v>TOO-CATFENSAUUQJ</v>
+        <v>TOO-CATFENSAUUSA</v>
       </c>
       <c r="D346" t="str">
         <v/>
@@ -26040,7 +26040,7 @@
         <v>Diamond Top Coat 500ml</v>
       </c>
       <c r="C347" t="str">
-        <v>TOP-DIAMONDTOPRZ</v>
+        <v>TOP-DIAMONDTOPCO</v>
       </c>
       <c r="D347" t="str">
         <v/>
@@ -26114,7 +26114,7 @@
         <v>Top coat tím Medium 1KG</v>
       </c>
       <c r="C348" t="str">
-        <v>TOP-TOPCOATTIMMX</v>
+        <v>TOP-TOPCOATTIMME3</v>
       </c>
       <c r="D348" t="str">
         <v/>
@@ -26188,7 +26188,7 @@
         <v>1KG top coat tím loãng</v>
       </c>
       <c r="C349" t="str">
-        <v>TOP-1KGTOPCOATUR</v>
+        <v>TOP-1KGTOPCOATTI</v>
       </c>
       <c r="D349" t="str">
         <v/>
@@ -26262,7 +26262,7 @@
         <v>Top coat tím loãng 500ml</v>
       </c>
       <c r="C350" t="str">
-        <v>TOP-TOPCOATTIMBP</v>
+        <v>TOP-TOPCOATTIMLO</v>
       </c>
       <c r="D350" t="str">
         <v/>
@@ -26336,7 +26336,7 @@
         <v>Chà chân xanh 400c</v>
       </c>
       <c r="C351" t="str">
-        <v>TOO-CHACHANXANDL</v>
+        <v>TOO-CHACHANXANH4</v>
       </c>
       <c r="D351" t="str">
         <v/>
@@ -26410,7 +26410,7 @@
         <v>Buffer cam 3 mặt</v>
       </c>
       <c r="C352" t="str">
-        <v>TOO-BUFFERCAM3YF</v>
+        <v>TOO-BUFFERCAM3MA</v>
       </c>
       <c r="D352" t="str">
         <v/>
@@ -26484,7 +26484,7 @@
         <v>Buffer trắng 4 mặt</v>
       </c>
       <c r="C353" t="str">
-        <v>PED-BUFFERTRANSO</v>
+        <v>PED-BUFFERTRANG4</v>
       </c>
       <c r="D353" t="str">
         <v/>
@@ -26558,7 +26558,7 @@
         <v>Tay bào máy tím</v>
       </c>
       <c r="C354" t="str">
-        <v>DOD-TAYBAOMAYTLJ</v>
+        <v>DOD-TAYBAOMAYTIM</v>
       </c>
       <c r="D354" t="str">
         <v/>
@@ -26632,7 +26632,7 @@
         <v>Tay bào máy G5</v>
       </c>
       <c r="C355" t="str">
-        <v>DOD-TAYBAOMAYGGT</v>
+        <v>DOD-TAYBAOMAYG5</v>
       </c>
       <c r="D355" t="str">
         <v/>
@@ -26706,7 +26706,7 @@
         <v>Đèn LED 96W</v>
       </c>
       <c r="C356" t="str">
-        <v>DOD-DENLED96WRH</v>
+        <v>DOD-DENLED96W</v>
       </c>
       <c r="D356" t="str">
         <v/>
@@ -26780,7 +26780,7 @@
         <v>Đèn LED 48W</v>
       </c>
       <c r="C357" t="str">
-        <v>DOD-DENLED48WYF</v>
+        <v>DOD-DENLED48W</v>
       </c>
       <c r="D357" t="str">
         <v/>
@@ -26854,7 +26854,7 @@
         <v>Tip làm chân set</v>
       </c>
       <c r="C358" t="str">
-        <v>PED-TIPLAMCHANVL</v>
+        <v>PED-TIPLAMCHANSE</v>
       </c>
       <c r="D358" t="str">
         <v/>
@@ -26928,7 +26928,7 @@
         <v>Chai sơn trống 15ml</v>
       </c>
       <c r="C359" t="str">
-        <v>TOO-CHAISONTROTL</v>
+        <v>TOO-CHAISONTRONG</v>
       </c>
       <c r="D359" t="str">
         <v/>
@@ -27002,7 +27002,7 @@
         <v>Túi ni lông xanh 800c</v>
       </c>
       <c r="C360" t="str">
-        <v>TOO-TUINILONGXGV</v>
+        <v>TOO-TUINILONGXAN</v>
       </c>
       <c r="D360" t="str">
         <v/>
@@ -27076,7 +27076,7 @@
         <v>5in1 Pedicure kit - 200c</v>
       </c>
       <c r="C361" t="str">
-        <v>TOO-5IN1PEDICUHE</v>
+        <v>TOO-5IN1PEDICURE2</v>
       </c>
       <c r="D361" t="str">
         <v/>
@@ -27150,7 +27150,7 @@
         <v>Thùng Dũa mini 5000c</v>
       </c>
       <c r="C362" t="str">
-        <v>PED-THUNGDUAMINR</v>
+        <v>PED-THUNGDUAMINI2</v>
       </c>
       <c r="D362" t="str">
         <v/>
@@ -27224,7 +27224,7 @@
         <v>Thùng Slim buffer 500c</v>
       </c>
       <c r="C363" t="str">
-        <v>PED-THUNGSLIMBPI</v>
+        <v>PED-THUNGSLIMBUF</v>
       </c>
       <c r="D363" t="str">
         <v/>
@@ -27298,7 +27298,7 @@
         <v>Thùng que tăm 800c</v>
       </c>
       <c r="C364" t="str">
-        <v>PED-THUNGQUETAGD</v>
+        <v>PED-THUNGQUETAM8</v>
       </c>
       <c r="D364" t="str">
         <v/>
@@ -27372,7 +27372,7 @@
         <v>Đèn cầu vòng đính đá v2</v>
       </c>
       <c r="C365" t="str">
-        <v>DOD-DENCAUVONGSH</v>
+        <v>DOD-DENCAUVONGDI2</v>
       </c>
       <c r="D365" t="str">
         <v/>
@@ -27446,7 +27446,7 @@
         <v>Đèn cầu vòng trắng v2</v>
       </c>
       <c r="C366" t="str">
-        <v>DOD-DENCAUVONGQO</v>
+        <v>DOD-DENCAUVONGTR</v>
       </c>
       <c r="D366" t="str">
         <v/>
@@ -27520,7 +27520,7 @@
         <v>4XC - Titan Xanh</v>
       </c>
       <c r="C367" t="str">
-        <v>DAU-4XCTITANXAFA</v>
+        <v>DAU-4XCTITANXANH</v>
       </c>
       <c r="D367" t="str">
         <v/>
@@ -27594,7 +27594,7 @@
         <v>2XC Titan xanh</v>
       </c>
       <c r="C368" t="str">
-        <v>DAU-2XCTITANXAHC</v>
+        <v>DAU-2XCTITANXANH</v>
       </c>
       <c r="D368" t="str">
         <v/>
@@ -27668,7 +27668,7 @@
         <v>Lọ không 500ml</v>
       </c>
       <c r="C369" t="str">
-        <v>TOO-LOKHONG500RE</v>
+        <v>TOO-LOKHONG500ML</v>
       </c>
       <c r="D369" t="str">
         <v/>
@@ -27742,7 +27742,7 @@
         <v>Cán dao cạo chân Inox</v>
       </c>
       <c r="C370" t="str">
-        <v>PED-CANDAOCAOCJQ</v>
+        <v>PED-CANDAOCAOCHA</v>
       </c>
       <c r="D370" t="str">
         <v/>
@@ -27816,7 +27816,7 @@
         <v>Dao lam Micra</v>
       </c>
       <c r="C371" t="str">
-        <v>PED-DAOLAMMICRTZ</v>
+        <v>PED-DAOLAMMICRA</v>
       </c>
       <c r="D371" t="str">
         <v/>
@@ -27890,7 +27890,7 @@
         <v>Dũa 80/80 Luxfile</v>
       </c>
       <c r="C372" t="str">
-        <v>DUA-DUA8080LUXPI</v>
+        <v>DUA-DUA8080LUXFI</v>
       </c>
       <c r="D372" t="str">
         <v/>
@@ -27964,7 +27964,7 @@
         <v>Dũa 100/100 Luxfile</v>
       </c>
       <c r="C373" t="str">
-        <v>DUA-DUA100100LMY</v>
+        <v>DUA-DUA100100LUX</v>
       </c>
       <c r="D373" t="str">
         <v/>
@@ -28038,7 +28038,7 @@
         <v>Máy sấy khô</v>
       </c>
       <c r="C374" t="str">
-        <v>DOD-MAYSAYKHOOJ</v>
+        <v>DOD-MAYSAYKHO</v>
       </c>
       <c r="D374" t="str">
         <v/>
@@ -28112,7 +28112,7 @@
         <v>Tip fan 120 màu - tip nhọn trong</v>
       </c>
       <c r="C375" t="str">
-        <v>TOO-TIPFAN120MCU</v>
+        <v>TOO-TIPFAN120MAU</v>
       </c>
       <c r="D375" t="str">
         <v/>
@@ -28186,7 +28186,7 @@
         <v>Tip fan 120 màu - tip nhọn đục</v>
       </c>
       <c r="C376" t="str">
-        <v>TOO-TIPFAN120MCV</v>
+        <v>TOO-TIPFAN120MAU2</v>
       </c>
       <c r="D376" t="str">
         <v/>
@@ -28260,7 +28260,7 @@
         <v>Tip fan 120 màu - tip natur trong</v>
       </c>
       <c r="C377" t="str">
-        <v>TOO-TIPFAN120MZQ</v>
+        <v>TOO-TIPFAN120MAU3</v>
       </c>
       <c r="D377" t="str">
         <v/>
@@ -28334,7 +28334,7 @@
         <v>Tip fan 120 màu - tip natur đục</v>
       </c>
       <c r="C378" t="str">
-        <v>TOO-TIPFAN120MKA</v>
+        <v>TOO-TIPFAN120MAU4</v>
       </c>
       <c r="D378" t="str">
         <v/>
@@ -28408,7 +28408,7 @@
         <v>Barbicide Concentrate 500ml</v>
       </c>
       <c r="C379" t="str">
-        <v>HOA-BARBICIDECML</v>
+        <v>HOA-BARBICIDECON</v>
       </c>
       <c r="D379" t="str">
         <v/>
@@ -28482,7 +28482,7 @@
         <v>liner gel vẽ 12ml - trắng</v>
       </c>
       <c r="C380" t="str">
-        <v>HOA-LINERGELVETR</v>
+        <v>HOA-LINERGELVE12</v>
       </c>
       <c r="D380" t="str">
         <v/>
@@ -28556,7 +28556,7 @@
         <v>liner gel vẽ 12ml - đen</v>
       </c>
       <c r="C381" t="str">
-        <v>HOA-LINERGELVEVJ</v>
+        <v>HOA-LINERGELVE122</v>
       </c>
       <c r="D381" t="str">
         <v/>
@@ -28630,7 +28630,7 @@
         <v>4XC - Hoa cúc 2.0</v>
       </c>
       <c r="C382" t="str">
-        <v>DAU-4XCHOACUC2VD</v>
+        <v>DAU-4XCHOACUC20</v>
       </c>
       <c r="D382" t="str">
         <v/>
@@ -28704,7 +28704,7 @@
         <v>Liner gel vẽ metallic - vàng 15ml</v>
       </c>
       <c r="C383" t="str">
-        <v>DES-LINERGELVEPS</v>
+        <v>DES-LINERGELVEME</v>
       </c>
       <c r="D383" t="str">
         <v/>
@@ -28778,7 +28778,7 @@
         <v>Liner gel vẽ metallic - bạc 15ml</v>
       </c>
       <c r="C384" t="str">
-        <v>DES-LINERGELVEOG</v>
+        <v>DES-LINERGELVEME2</v>
       </c>
       <c r="D384" t="str">
         <v/>
@@ -28852,7 +28852,7 @@
         <v>1KG top coat tím đặc</v>
       </c>
       <c r="C385" t="str">
-        <v>TOP-1KGTOPCOATSF</v>
+        <v>TOP-1KGTOPCOATTI2</v>
       </c>
       <c r="D385" t="str">
         <v/>
@@ -28926,7 +28926,7 @@
         <v>4XC</v>
       </c>
       <c r="C386" t="str">
-        <v>DAU-4XCXR</v>
+        <v>DAU-4XC</v>
       </c>
       <c r="D386" t="str">
         <v/>
@@ -29000,7 +29000,7 @@
         <v>Trục nhám sắt v2</v>
       </c>
       <c r="C387" t="str">
-        <v>DAU-TRUCNHAMSARG</v>
+        <v>DAU-TRUCNHAMSATV</v>
       </c>
       <c r="D387" t="str">
         <v/>
@@ -29074,7 +29074,7 @@
         <v>Trục nhám chắc chắn v2</v>
       </c>
       <c r="C388" t="str">
-        <v>DAU-TRUCNHAMCHMJ</v>
+        <v>DAU-TRUCNHAMCHAC</v>
       </c>
       <c r="D388" t="str">
         <v/>
@@ -29148,7 +29148,7 @@
         <v>Liquid J-2000 C7</v>
       </c>
       <c r="C389" t="str">
-        <v>HOA-LIQUIDJ200QO</v>
+        <v>HOA-LIQUIDJ2000C3</v>
       </c>
       <c r="D389" t="str">
         <v/>
@@ -29222,7 +29222,7 @@
         <v>Bột - Ombre Pink I</v>
       </c>
       <c r="C390" t="str">
-        <v>BOT-BOTOMBREPIMU</v>
+        <v>BOT-BOTOMBREPINK</v>
       </c>
       <c r="D390" t="str">
         <v/>
@@ -29296,7 +29296,7 @@
         <v>Liquid EMA J-2 C7</v>
       </c>
       <c r="C391" t="str">
-        <v>HOA-LIQUIDEMAJFM</v>
+        <v>HOA-LIQUIDEMAJ2C</v>
       </c>
       <c r="D391" t="str">
         <v/>
@@ -29370,7 +29370,7 @@
         <v>4XC - Đầu tròn - Titan xanh</v>
       </c>
       <c r="C392" t="str">
-        <v>DAU-4XCDAUTRONVL</v>
+        <v>DAU-4XCDAUTRONTI</v>
       </c>
       <c r="D392" t="str">
         <v/>
@@ -29444,7 +29444,7 @@
         <v>Motor tay máy tím</v>
       </c>
       <c r="C393" t="str">
-        <v>DOD-MOTORTAYMALT</v>
+        <v>DOD-MOTORTAYMAYT</v>
       </c>
       <c r="D393" t="str">
         <v/>
@@ -29518,7 +29518,7 @@
         <v>Super White 250ml</v>
       </c>
       <c r="C394" t="str">
-        <v>HOA-SUPERWHITEUB</v>
+        <v>HOA-SUPERWHITE25</v>
       </c>
       <c r="D394" t="str">
         <v/>
@@ -29592,7 +29592,7 @@
         <v>Super Black 250ml</v>
       </c>
       <c r="C395" t="str">
-        <v>HOA-SUPERBLACKQI</v>
+        <v>HOA-SUPERBLACK25</v>
       </c>
       <c r="D395" t="str">
         <v/>
@@ -29666,7 +29666,7 @@
         <v>Sugar Scrub - Orange 5kg</v>
       </c>
       <c r="C396" t="str">
-        <v>PED-SUGARSCRUBVX</v>
+        <v>PED-SUGARSCRUBOR2</v>
       </c>
       <c r="D396" t="str">
         <v/>
@@ -29740,7 +29740,7 @@
         <v>Gel Scrub - Mint 5KG</v>
       </c>
       <c r="C397" t="str">
-        <v>HOA-GELSCRUBMILB</v>
+        <v>HOA-GELSCRUBMINT</v>
       </c>
       <c r="D397" t="str">
         <v/>
@@ -29814,7 +29814,7 @@
         <v>Diamond Top Coat 1L</v>
       </c>
       <c r="C398" t="str">
-        <v>TOP-DIAMONDTOPWI</v>
+        <v>TOP-DIAMONDTOPCO2</v>
       </c>
       <c r="D398" t="str">
         <v/>
@@ -29888,7 +29888,7 @@
         <v>Cốc đựng bột tròn</v>
       </c>
       <c r="C399" t="str">
-        <v>TOO-COCDUNGBOTAP</v>
+        <v>TOO-COCDUNGBOTTR2</v>
       </c>
       <c r="D399" t="str">
         <v/>
@@ -29962,7 +29962,7 @@
         <v>Hũ đựng gel 50ml</v>
       </c>
       <c r="C400" t="str">
-        <v>TOO-HUDUNGGEL5QN</v>
+        <v>TOO-HUDUNGGEL50M</v>
       </c>
       <c r="D400" t="str">
         <v/>
@@ -30036,7 +30036,7 @@
         <v>Hũ đựng gel 30ml</v>
       </c>
       <c r="C401" t="str">
-        <v>TOO-HUDUNGGEL3XN</v>
+        <v>TOO-HUDUNGGEL30M</v>
       </c>
       <c r="D401" t="str">
         <v/>
@@ -30110,7 +30110,7 @@
         <v>Chà chân vàng 400c</v>
       </c>
       <c r="C402" t="str">
-        <v>TOO-CHACHANVANOI</v>
+        <v>TOO-CHACHANVANG4</v>
       </c>
       <c r="D402" t="str">
         <v/>
@@ -30184,7 +30184,7 @@
         <v>Đèn sạc pin 90W</v>
       </c>
       <c r="C403" t="str">
-        <v>DOD-DENSACPIN9WJ</v>
+        <v>DOD-DENSACPIN90W</v>
       </c>
       <c r="D403" t="str">
         <v/>
@@ -30258,7 +30258,7 @@
         <v>Sửa chữa tay bào</v>
       </c>
       <c r="C404" t="str">
-        <v>DIC-SUACHUATAYHX</v>
+        <v>DIC-SUACHUATAYBA</v>
       </c>
       <c r="D404" t="str">
         <v/>
@@ -30332,7 +30332,7 @@
         <v>4XC Đầu tròn v3</v>
       </c>
       <c r="C405" t="str">
-        <v>DAU-4XCDAUTRONCT</v>
+        <v>DAU-4XCDAUTRONV3</v>
       </c>
       <c r="D405" t="str">
         <v/>
@@ -30406,7 +30406,7 @@
         <v>M vàng - to</v>
       </c>
       <c r="C406" t="str">
-        <v>DAU-MVANGTODZ</v>
+        <v>DAU-MVANGTO</v>
       </c>
       <c r="D406" t="str">
         <v/>
@@ -30480,7 +30480,7 @@
         <v>Set Bột Neon dặm 24 màu</v>
       </c>
       <c r="C407" t="str">
-        <v>DES-SETBOTNEONFV</v>
+        <v>DES-SETBOTNEONDA</v>
       </c>
       <c r="D407" t="str">
         <v/>
@@ -30554,7 +30554,7 @@
         <v>Set Bút Xốp dặm</v>
       </c>
       <c r="C408" t="str">
-        <v>DES-SETBUTXOPDYD</v>
+        <v>DES-SETBUTXOPDAM</v>
       </c>
       <c r="D408" t="str">
         <v/>
@@ -30628,7 +30628,7 @@
         <v>Thân máy Trắng Marathon</v>
       </c>
       <c r="C409" t="str">
-        <v>DOD-THANMAYTRAAX</v>
+        <v>DOD-THANMAYTRANG</v>
       </c>
       <c r="D409" t="str">
         <v/>
@@ -30702,7 +30702,7 @@
         <v>Dây cắm 3 chân UP200</v>
       </c>
       <c r="C410" t="str">
-        <v>DOD-DAYCAM3CHAMQ</v>
+        <v>DOD-DAYCAM3CHANU</v>
       </c>
       <c r="D410" t="str">
         <v/>
@@ -30776,7 +30776,7 @@
         <v>Set Sơn mắt mèo 10D 12 màu</v>
       </c>
       <c r="C411" t="str">
-        <v>SON-SETSONMATMAL</v>
+        <v>SON-SETSONMATMEO</v>
       </c>
       <c r="D411" t="str">
         <v/>
@@ -30850,7 +30850,7 @@
         <v>Gel nặn 3D - Clear 50ml</v>
       </c>
       <c r="C412" t="str">
-        <v>DES-GELNAN3DCLTQ</v>
+        <v>DES-GELNAN3DCLEA</v>
       </c>
       <c r="D412" t="str">
         <v/>
@@ -30924,7 +30924,7 @@
         <v>Kê chân cao - đen vàng</v>
       </c>
       <c r="C413" t="str">
-        <v>TOO-KECHANCAODKW</v>
+        <v>TOO-KECHANCAODEN</v>
       </c>
       <c r="D413" t="str">
         <v/>
@@ -30998,7 +30998,7 @@
         <v>Kê chân cao - trắng vàng</v>
       </c>
       <c r="C414" t="str">
-        <v>TOO-KECHANCAOTZS</v>
+        <v>TOO-KECHANCAOTRA</v>
       </c>
       <c r="D414" t="str">
         <v/>
@@ -31072,7 +31072,7 @@
         <v>Chổi quét bàn - Nhỏ</v>
       </c>
       <c r="C415" t="str">
-        <v>TOO-CHOIQUETBARC</v>
+        <v>TOO-CHOIQUETBANN</v>
       </c>
       <c r="D415" t="str">
         <v/>
@@ -31146,7 +31146,7 @@
         <v>Muối viên xô 4000 viên</v>
       </c>
       <c r="C416" t="str">
-        <v>PED-MUOIVIENXORB</v>
+        <v>PED-MUOIVIENXO40</v>
       </c>
       <c r="D416" t="str">
         <v/>
@@ -31220,7 +31220,7 @@
         <v>Moonlight Cat Eye 12 màu</v>
       </c>
       <c r="C417" t="str">
-        <v>SON-MOONLIGHTCVO</v>
+        <v>SON-MOONLIGHTCAT</v>
       </c>
       <c r="D417" t="str">
         <v/>
@@ -31294,7 +31294,7 @@
         <v>Gel thinner 30ml</v>
       </c>
       <c r="C418" t="str">
-        <v>HOA-GELTHINNERAS</v>
+        <v>HOA-GELTHINNER30</v>
       </c>
       <c r="D418" t="str">
         <v/>
@@ -31368,7 +31368,7 @@
         <v>Diamond Top Coat 15ml</v>
       </c>
       <c r="C419" t="str">
-        <v>TOP-DIAMONDTOPAL</v>
+        <v>TOP-DIAMONDTOPCO3</v>
       </c>
       <c r="D419" t="str">
         <v/>
@@ -31442,7 +31442,7 @@
         <v>Gel nặn 3D - trắng 15ml</v>
       </c>
       <c r="C420" t="str">
-        <v>HOA-GELNAN3DTRVK</v>
+        <v>HOA-GELNAN3DTRAN</v>
       </c>
       <c r="D420" t="str">
         <v/>
@@ -31516,7 +31516,7 @@
         <v>Sơn màu Milky White 250ml</v>
       </c>
       <c r="C421" t="str">
-        <v>SON-SONMAUMILKRW</v>
+        <v>SON-SONMAUMILKYW2</v>
       </c>
       <c r="D421" t="str">
         <v/>
@@ -31590,7 +31590,7 @@
         <v>Liquid EMA G3 C1 Blue</v>
       </c>
       <c r="C422" t="str">
-        <v>HOA-LIQUIDEMAGQT</v>
+        <v>HOA-LIQUIDEMAG3C</v>
       </c>
       <c r="D422" t="str">
         <v/>
@@ -31664,7 +31664,7 @@
         <v>Xô Gel Scrub Orange - 20KG</v>
       </c>
       <c r="C423" t="str">
-        <v>PED-XOGELSCRUBAI</v>
+        <v>PED-XOGELSCRUBOR</v>
       </c>
       <c r="D423" t="str">
         <v/>
@@ -31738,7 +31738,7 @@
         <v>Vỏ nhám Mỹ ⌗150 (1000c)</v>
       </c>
       <c r="C424" t="str">
-        <v>TOO-VONHAMMY15ML</v>
+        <v>TOO-VONHAMMY1501</v>
       </c>
       <c r="D424" t="str">
         <v/>
@@ -31812,7 +31812,7 @@
         <v>Set 5c Bút Nặn Silicon</v>
       </c>
       <c r="C425" t="str">
-        <v>BUT-SET5CBUTNASH</v>
+        <v>BUT-SET5CBUTNANS</v>
       </c>
       <c r="D425" t="str">
         <v/>
@@ -31886,7 +31886,7 @@
         <v>Dũa mỏng - To Vuông 80/80</v>
       </c>
       <c r="C426" t="str">
-        <v>DUA-DUAMONGTOVON</v>
+        <v>DUA-DUAMONGTOVUO</v>
       </c>
       <c r="D426" t="str">
         <v/>
@@ -31960,7 +31960,7 @@
         <v>Dũa mỏng - To Vuông 100/100</v>
       </c>
       <c r="C427" t="str">
-        <v>DUA-DUAMONGTOVHZ</v>
+        <v>DUA-DUAMONGTOVUO2</v>
       </c>
       <c r="D427" t="str">
         <v/>
@@ -32034,7 +32034,7 @@
         <v>Tip Thẳng Natur Nhọn - Lẻ</v>
       </c>
       <c r="C428" t="str">
-        <v>TIP-TIPTHANGNAHO</v>
+        <v>TIP-TIPTHANGNATU</v>
       </c>
       <c r="D428" t="str">
         <v/>
@@ -32108,7 +32108,7 @@
         <v>Bình ngâm khử trùng dụng cụ</v>
       </c>
       <c r="C429" t="str">
-        <v>PED-BINHNGAMKHBI</v>
+        <v>PED-BINHNGAMKHUT</v>
       </c>
       <c r="D429" t="str">
         <v/>
@@ -32182,7 +32182,7 @@
         <v>Bút cán gỗ sz14</v>
       </c>
       <c r="C430" t="str">
-        <v>BUT-BUTCANGOSZKF</v>
+        <v>BUT-BUTCANGOSZ14</v>
       </c>
       <c r="D430" t="str">
         <v/>
@@ -32256,7 +32256,7 @@
         <v>BL1 - Nhũ Đường Đen ánh trắng</v>
       </c>
       <c r="C431" t="str">
-        <v>DES-BL1NHUDUONGM</v>
+        <v>DES-BL1NHUDUONGD</v>
       </c>
       <c r="D431" t="str">
         <v/>
@@ -32330,7 +32330,7 @@
         <v>BL2 - Nhũ Đường Đen 7 màu</v>
       </c>
       <c r="C432" t="str">
-        <v>DES-BL2NHUDUONWR</v>
+        <v>DES-BL2NHUDUONGD</v>
       </c>
       <c r="D432" t="str">
         <v/>
@@ -32404,7 +32404,7 @@
         <v>Liquid EMA Ít mùi</v>
       </c>
       <c r="C433" t="str">
-        <v>HOA-LIQUIDEMAISP</v>
+        <v>HOA-LIQUIDEMAITM</v>
       </c>
       <c r="D433" t="str">
         <v/>
@@ -32478,7 +32478,7 @@
         <v>Bịch Dũa mini 50c - Lẻ</v>
       </c>
       <c r="C434" t="str">
-        <v>PED-BICHDUAMINHK</v>
+        <v>PED-BICHDUAMINI5</v>
       </c>
       <c r="D434" t="str">
         <v/>
@@ -32552,7 +32552,7 @@
         <v>Xốp kẹp chân 100c - Lẻ</v>
       </c>
       <c r="C435" t="str">
-        <v>PED-XOPKEPCHANQS</v>
+        <v>PED-XOPKEPCHAN10</v>
       </c>
       <c r="D435" t="str">
         <v/>
@@ -32626,7 +32626,7 @@
         <v>Hộp túi y tế 100c - Lẻ</v>
       </c>
       <c r="C436" t="str">
-        <v>PED-HOPTUIYTE1DB</v>
+        <v>PED-HOPTUIYTE100</v>
       </c>
       <c r="D436" t="str">
         <v/>
@@ -32700,7 +32700,7 @@
         <v>Muối viên - Lọ Nhỏ 250c</v>
       </c>
       <c r="C437" t="str">
-        <v>PED-MUOIVIENLOWV</v>
+        <v>PED-MUOIVIENLONH</v>
       </c>
       <c r="D437" t="str">
         <v/>
@@ -32774,7 +32774,7 @@
         <v>Chai Bơm Cồn 200ml</v>
       </c>
       <c r="C438" t="str">
-        <v>TOO-CHAIBOMCONNC</v>
+        <v>TOO-CHAIBOMCON20</v>
       </c>
       <c r="D438" t="str">
         <v/>
@@ -32848,7 +32848,7 @@
         <v>Cán dao cạo chân P05</v>
       </c>
       <c r="C439" t="str">
-        <v>PED-CANDAOCAOCZT</v>
+        <v>PED-CANDAOCAOCHA2</v>
       </c>
       <c r="D439" t="str">
         <v/>
@@ -32922,7 +32922,7 @@
         <v>Kệ Acrylic đựng bút</v>
       </c>
       <c r="C440" t="str">
-        <v>TOO-KEACRYLICDAX</v>
+        <v>TOO-KEACRYLICDUN</v>
       </c>
       <c r="D440" t="str">
         <v/>
@@ -32996,7 +32996,7 @@
         <v>Bịch que tăm 100c - Lẻ</v>
       </c>
       <c r="C441" t="str">
-        <v>TOO-BICHQUETAMBK</v>
+        <v>TOO-BICHQUETAM10</v>
       </c>
       <c r="D441" t="str">
         <v/>
@@ -33070,7 +33070,7 @@
         <v>Marble Ink Set 12 màu</v>
       </c>
       <c r="C442" t="str">
-        <v>DES-MARBLEINKSDQ</v>
+        <v>DES-MARBLEINKSET</v>
       </c>
       <c r="D442" t="str">
         <v/>
@@ -33144,7 +33144,7 @@
         <v>Gel 6in1</v>
       </c>
       <c r="C443" t="str">
-        <v>TOP-GEL6IN1AN</v>
+        <v>TOP-GEL6IN1</v>
       </c>
       <c r="D443" t="str">
         <v/>
@@ -33218,7 +33218,7 @@
         <v>Máy bào di động 45K</v>
       </c>
       <c r="C444" t="str">
-        <v>DOD-MAYBAODIDOGW</v>
+        <v>DOD-MAYBAODIDONG2</v>
       </c>
       <c r="D444" t="str">
         <v/>
@@ -33292,7 +33292,7 @@
         <v>Gel vẽ Đen Hũ 50ml</v>
       </c>
       <c r="C445" t="str">
-        <v>HOA-GELVEDENHULD</v>
+        <v>HOA-GELVEDENHU50</v>
       </c>
       <c r="D445" t="str">
         <v/>
@@ -33366,7 +33366,7 @@
         <v>5in1 pedicure kit cam</v>
       </c>
       <c r="C446" t="str">
-        <v>PED-5IN1PEDICUEY</v>
+        <v>PED-5IN1PEDICURE</v>
       </c>
       <c r="D446" t="str">
         <v/>
@@ -33440,7 +33440,7 @@
         <v>Lẻ - Jelly Spa 1 túi</v>
       </c>
       <c r="C447" t="str">
-        <v>PED-LEJELLYSPACS</v>
+        <v>PED-LEJELLYSPA1T</v>
       </c>
       <c r="D447" t="str">
         <v/>
@@ -33514,7 +33514,7 @@
         <v>Kê tay cao - màu đen - chân bạc</v>
       </c>
       <c r="C448" t="str">
-        <v>TOO-KETAYCAOMAKR</v>
+        <v>TOO-KETAYCAOMAUD</v>
       </c>
       <c r="D448" t="str">
         <v/>
@@ -33588,7 +33588,7 @@
         <v>Kê tay cao - màu trắng - chân bạc</v>
       </c>
       <c r="C449" t="str">
-        <v>TOO-KETAYCAOMAAC</v>
+        <v>TOO-KETAYCAOMAUT</v>
       </c>
       <c r="D449" t="str">
         <v/>
@@ -33662,7 +33662,7 @@
         <v>Đèn LED làm chân</v>
       </c>
       <c r="C450" t="str">
-        <v>DOD-DENLEDLAMCGX</v>
+        <v>DOD-DENLEDLAMCHA</v>
       </c>
       <c r="D450" t="str">
         <v/>
@@ -33736,7 +33736,7 @@
         <v>Máy Khử trùng nhiệt độ</v>
       </c>
       <c r="C451" t="str">
-        <v>DOD-MAYKHUTRUNZP</v>
+        <v>DOD-MAYKHUTRUNGN</v>
       </c>
       <c r="D451" t="str">
         <v/>
@@ -33810,7 +33810,7 @@
         <v>Mịn thông XF</v>
       </c>
       <c r="C452" t="str">
-        <v>DAU-MINTHONGXFDA</v>
+        <v>DAU-MINTHONGXF2</v>
       </c>
       <c r="D452" t="str">
         <v/>
@@ -33884,7 +33884,7 @@
         <v>Kìm Bấm Móng - Đầu Thẳng</v>
       </c>
       <c r="C453" t="str">
-        <v>TOO-KIMBAMMONGFS</v>
+        <v>TOO-KIMBAMMONGDA</v>
       </c>
       <c r="D453" t="str">
         <v/>
@@ -33958,7 +33958,7 @@
         <v>Imperial Top Coat - 15ml - thin</v>
       </c>
       <c r="C454" t="str">
-        <v>TOP-IMPERIALTOUV</v>
+        <v>TOP-IMPERIALTOPC</v>
       </c>
       <c r="D454" t="str">
         <v/>
@@ -34032,7 +34032,7 @@
         <v>Imperial Top Coat - 15ml - thick</v>
       </c>
       <c r="C455" t="str">
-        <v>TOP-IMPERIALTOKO</v>
+        <v>TOP-IMPERIALTOPC2</v>
       </c>
       <c r="D455" t="str">
         <v/>
@@ -34106,7 +34106,7 @@
         <v>Imperial Top Coat - 500ml - thin</v>
       </c>
       <c r="C456" t="str">
-        <v>TOP-IMPERIALTOBX</v>
+        <v>TOP-IMPERIALTOPC3</v>
       </c>
       <c r="D456" t="str">
         <v/>
@@ -34180,7 +34180,7 @@
         <v>Imperial Top Coat - 1000ml - thin</v>
       </c>
       <c r="C457" t="str">
-        <v>TOP-IMPERIALTOJS</v>
+        <v>TOP-IMPERIALTOPC4</v>
       </c>
       <c r="D457" t="str">
         <v/>
@@ -34254,7 +34254,7 @@
         <v>Imperial Top Coat - 500ml - thick</v>
       </c>
       <c r="C458" t="str">
-        <v>TOP-IMPERIALTOOA</v>
+        <v>TOP-IMPERIALTOPC5</v>
       </c>
       <c r="D458" t="str">
         <v/>
@@ -34328,7 +34328,7 @@
         <v>Imperial Top Coat - 1000ml - thick</v>
       </c>
       <c r="C459" t="str">
-        <v>TOP-IMPERIALTOND</v>
+        <v>TOP-IMPERIALTOPC6</v>
       </c>
       <c r="D459" t="str">
         <v/>
@@ -34402,7 +34402,7 @@
         <v>Glaze Gel Polish Set 12 màu</v>
       </c>
       <c r="C460" t="str">
-        <v>SON-GLAZEGELPOEQ</v>
+        <v>SON-GLAZEGELPOLI</v>
       </c>
       <c r="D460" t="str">
         <v/>
@@ -34476,7 +34476,7 @@
         <v>BIAB 15ml</v>
       </c>
       <c r="C461" t="str">
-        <v>GEL-BIAB15MLZK</v>
+        <v>GEL-BIAB15ML</v>
       </c>
       <c r="D461" t="str">
         <v/>
@@ -34550,7 +34550,7 @@
         <v>Cuticle Oil nắp nhọn 15ml</v>
       </c>
       <c r="C462" t="str">
-        <v>HOA-CUTICLEOILDE</v>
+        <v>HOA-CUTICLEOILNA</v>
       </c>
       <c r="D462" t="str">
         <v/>
@@ -34624,7 +34624,7 @@
         <v>Liquid Professional</v>
       </c>
       <c r="C463" t="str">
-        <v>HOA-LIQUIDPROFOV</v>
+        <v>HOA-LIQUIDPROFES</v>
       </c>
       <c r="D463" t="str">
         <v/>
@@ -34698,7 +34698,7 @@
         <v>Liquid Winter</v>
       </c>
       <c r="C464" t="str">
-        <v>HOA-LIQUIDWINTXY</v>
+        <v>HOA-LIQUIDWINTER</v>
       </c>
       <c r="D464" t="str">
         <v/>
@@ -34772,7 +34772,7 @@
         <v>Cốc liquid mini</v>
       </c>
       <c r="C465" t="str">
-        <v>TOO-COCLIQUIDMAL</v>
+        <v>TOO-COCLIQUIDMIN</v>
       </c>
       <c r="D465" t="str">
         <v/>
@@ -34846,7 +34846,7 @@
         <v>Dép làm chân 24c</v>
       </c>
       <c r="C466" t="str">
-        <v>PED-DEPLAMCHANXF</v>
+        <v>PED-DEPLAMCHAN24</v>
       </c>
       <c r="D466" t="str">
         <v/>
@@ -34920,7 +34920,7 @@
         <v>Kem đẩy da 3.8L</v>
       </c>
       <c r="C467" t="str">
-        <v>PED-KEMDAYDA38CC</v>
+        <v>PED-KEMDAYDA38L</v>
       </c>
       <c r="D467" t="str">
         <v/>
@@ -34994,7 +34994,7 @@
         <v>Kem đẩy da 1L</v>
       </c>
       <c r="C468" t="str">
-        <v>PED-KEMDAYDA1LVQ</v>
+        <v>PED-KEMDAYDA1L</v>
       </c>
       <c r="D468" t="str">
         <v/>
@@ -35068,7 +35068,7 @@
         <v>Hộp Pedicure Bath Bombs 60c</v>
       </c>
       <c r="C469" t="str">
-        <v>PED-HOPPEDICURWY</v>
+        <v>PED-HOPPEDICUREB</v>
       </c>
       <c r="D469" t="str">
         <v/>
@@ -35142,7 +35142,7 @@
         <v>Imperial Top Coat - 250ml - thick</v>
       </c>
       <c r="C470" t="str">
-        <v>TOP-IMPERIALTORE</v>
+        <v>TOP-IMPERIALTOPC7</v>
       </c>
       <c r="D470" t="str">
         <v/>
@@ -35216,7 +35216,7 @@
         <v>Imperial Top Coat - 250ml - thin</v>
       </c>
       <c r="C471" t="str">
-        <v>TOP-IMPERIALTOSF</v>
+        <v>TOP-IMPERIALTOPC8</v>
       </c>
       <c r="D471" t="str">
         <v/>
@@ -35290,7 +35290,7 @@
         <v>Dũa Luxfile 60/60</v>
       </c>
       <c r="C472" t="str">
-        <v>DUA-DUALUXFILEMI</v>
+        <v>DUA-DUALUXFILE60</v>
       </c>
       <c r="D472" t="str">
         <v/>
@@ -35364,7 +35364,7 @@
         <v>Túi ni lông trong</v>
       </c>
       <c r="C473" t="str">
-        <v>PED-TUINILONGTSB</v>
+        <v>PED-TUINILONGTRO</v>
       </c>
       <c r="D473" t="str">
         <v/>
@@ -35438,7 +35438,7 @@
         <v>Đèn nối mi</v>
       </c>
       <c r="C474" t="str">
-        <v>DOD-DENNOIMIMU</v>
+        <v>DOD-DENNOIMI</v>
       </c>
       <c r="D474" t="str">
         <v/>
@@ -35512,7 +35512,7 @@
         <v>Đèn bàn LED siêu sáng</v>
       </c>
       <c r="C475" t="str">
-        <v>DOD-DENBANLEDSIC</v>
+        <v>DOD-DENBANLEDSIE</v>
       </c>
       <c r="D475" t="str">
         <v/>
@@ -35586,7 +35586,7 @@
         <v>Típ làm mẫu quyển màu nhọn</v>
       </c>
       <c r="C476" t="str">
-        <v>TIP-TIPLAMMAUQQC</v>
+        <v>TIP-TIPLAMMAUQUY</v>
       </c>
       <c r="D476" t="str">
         <v/>
@@ -35660,7 +35660,7 @@
         <v>Thùng Chà chân tím 400c</v>
       </c>
       <c r="C477" t="str">
-        <v>PED-THUNGCHACHZL</v>
+        <v>PED-THUNGCHACHAN</v>
       </c>
       <c r="D477" t="str">
         <v/>
@@ -35734,7 +35734,7 @@
         <v>Kìm bấm móng L 777 Korea</v>
       </c>
       <c r="C478" t="str">
-        <v>TOO-KIMBAMMONGRQ</v>
+        <v>TOO-KIMBAMMONGL7</v>
       </c>
       <c r="D478" t="str">
         <v/>
@@ -35808,7 +35808,7 @@
         <v>Tip trong thẳng clear</v>
       </c>
       <c r="C479" t="str">
-        <v>TIP-TIPTRONGTHSG</v>
+        <v>TIP-TIPTRONGTHAN</v>
       </c>
       <c r="D479" t="str">
         <v/>
@@ -35882,7 +35882,7 @@
         <v>Tip thẳng vuông đục</v>
       </c>
       <c r="C480" t="str">
-        <v>TIP-TIPTHANGVUOG</v>
+        <v>TIP-TIPTHANGVUON</v>
       </c>
       <c r="D480" t="str">
         <v/>
@@ -35956,7 +35956,7 @@
         <v>Tip trong nhọn</v>
       </c>
       <c r="C481" t="str">
-        <v>TIP-TIPTRONGNHMZ</v>
+        <v>TIP-TIPTRONGNHON</v>
       </c>
       <c r="D481" t="str">
         <v/>
@@ -36030,7 +36030,7 @@
         <v>Kìm tháo đá</v>
       </c>
       <c r="C482" t="str">
-        <v>TOO-KIMTHAODALQ</v>
+        <v>TOO-KIMTHAODA</v>
       </c>
       <c r="D482" t="str">
         <v/>
@@ -36104,7 +36104,7 @@
         <v>Bút chấm bi vôi 2 đầu</v>
       </c>
       <c r="C483" t="str">
-        <v>BUT-BUTCHAMBIVCE</v>
+        <v>BUT-BUTCHAMBIVOI</v>
       </c>
       <c r="D483" t="str">
         <v/>
@@ -36178,7 +36178,7 @@
         <v>Bào Mịn 3in1 dài - F</v>
       </c>
       <c r="C484" t="str">
-        <v>DAU-BAOMIN3IN1QL</v>
+        <v>DAU-BAOMIN3IN1DA</v>
       </c>
       <c r="D484" t="str">
         <v/>
@@ -36252,7 +36252,7 @@
         <v>Bào Mịn Dài XXL 5in1 - F</v>
       </c>
       <c r="C485" t="str">
-        <v>DAU-BAOMINDAIXNR</v>
+        <v>DAU-BAOMINDAIXXL</v>
       </c>
       <c r="D485" t="str">
         <v/>
@@ -36326,7 +36326,7 @@
         <v>Bào Mịn Diamond - Đẩy Khoé</v>
       </c>
       <c r="C486" t="str">
-        <v>DAU-BAOMINDIAMLB</v>
+        <v>DAU-BAOMINDIAMON2</v>
       </c>
       <c r="D486" t="str">
         <v/>
@@ -36400,7 +36400,7 @@
         <v>Đèn Hybrid SORAH</v>
       </c>
       <c r="C487" t="str">
-        <v>DOD-DENHYBRIDSSR</v>
+        <v>DOD-DENHYBRIDSOR</v>
       </c>
       <c r="D487" t="str">
         <v/>
@@ -36474,7 +36474,7 @@
         <v>Hũ đựng nhũ</v>
       </c>
       <c r="C488" t="str">
-        <v>TOO-HUDUNGNHUFE</v>
+        <v>TOO-HUDUNGNHU</v>
       </c>
       <c r="D488" t="str">
         <v/>
@@ -36548,7 +36548,7 @@
         <v>Gel đắp - 500ml - Clear</v>
       </c>
       <c r="C489" t="str">
-        <v>GEL-GELDAP500MWS</v>
+        <v>GEL-GELDAP500MLC</v>
       </c>
       <c r="D489" t="str">
         <v/>
@@ -36622,7 +36622,7 @@
         <v>Gel đắp - 500ml - Natural Pink</v>
       </c>
       <c r="C490" t="str">
-        <v>GEL-GELDAP500MZY</v>
+        <v>GEL-GELDAP500MLN</v>
       </c>
       <c r="D490" t="str">
         <v/>
@@ -36696,7 +36696,7 @@
         <v>Gel đắp - 500ml - Milky Pink</v>
       </c>
       <c r="C491" t="str">
-        <v>GEL-GELDAP500MHW</v>
+        <v>GEL-GELDAP500MLM</v>
       </c>
       <c r="D491" t="str">
         <v/>
@@ -36770,7 +36770,7 @@
         <v>Gel đắp - 500ml - Milky White</v>
       </c>
       <c r="C492" t="str">
-        <v>GEL-GELDAP500MBN</v>
+        <v>GEL-GELDAP500MLM2</v>
       </c>
       <c r="D492" t="str">
         <v/>
@@ -36844,7 +36844,7 @@
         <v>Gel đắp - 500ml - Makeup 1</v>
       </c>
       <c r="C493" t="str">
-        <v>GEL-GELDAP500MAC</v>
+        <v>GEL-GELDAP500MLM3</v>
       </c>
       <c r="D493" t="str">
         <v/>
@@ -36918,7 +36918,7 @@
         <v>Gel đắp - 500ml - Makeup 2</v>
       </c>
       <c r="C494" t="str">
-        <v>GEL-GELDAP500MKP</v>
+        <v>GEL-GELDAP500MLM4</v>
       </c>
       <c r="D494" t="str">
         <v/>
@@ -36992,7 +36992,7 @@
         <v>Gel đắp - 500ml - Makeup 3</v>
       </c>
       <c r="C495" t="str">
-        <v>GEL-GELDAP500MFO</v>
+        <v>GEL-GELDAP500MLM5</v>
       </c>
       <c r="D495" t="str">
         <v/>
@@ -37066,7 +37066,7 @@
         <v>Gel đắp - 50ml - Clear</v>
       </c>
       <c r="C496" t="str">
-        <v>GEL-GELDAP50MLDO</v>
+        <v>GEL-GELDAP50MLCL</v>
       </c>
       <c r="D496" t="str">
         <v/>
@@ -37140,7 +37140,7 @@
         <v>Gel đắp - 50ml - Natural Pink</v>
       </c>
       <c r="C497" t="str">
-        <v>GEL-GELDAP50MLPL</v>
+        <v>GEL-GELDAP50MLNA</v>
       </c>
       <c r="D497" t="str">
         <v/>
@@ -37214,7 +37214,7 @@
         <v>Gel đắp - 50ml - Milky Pink</v>
       </c>
       <c r="C498" t="str">
-        <v>GEL-GELDAP50MLUG</v>
+        <v>GEL-GELDAP50MLMI</v>
       </c>
       <c r="D498" t="str">
         <v/>
@@ -37288,7 +37288,7 @@
         <v>Gel đắp - 50ml - Milky White</v>
       </c>
       <c r="C499" t="str">
-        <v>GEL-GELDAP50MLVH</v>
+        <v>GEL-GELDAP50MLMI2</v>
       </c>
       <c r="D499" t="str">
         <v/>
@@ -37362,7 +37362,7 @@
         <v>Gel đắp - 50ml - Makeup ⌗1</v>
       </c>
       <c r="C500" t="str">
-        <v>GEL-GELDAP50MLSM</v>
+        <v>GEL-GELDAP50MLMA</v>
       </c>
       <c r="D500" t="str">
         <v/>
@@ -37436,7 +37436,7 @@
         <v>Gel đắp - 50ml - Makeup ⌗2</v>
       </c>
       <c r="C501" t="str">
-        <v>GEL-GELDAP50MLKR</v>
+        <v>GEL-GELDAP50MLMA2</v>
       </c>
       <c r="D501" t="str">
         <v/>
@@ -37510,7 +37510,7 @@
         <v>Gel đắp - 50ml - Makeup ⌗3</v>
       </c>
       <c r="C502" t="str">
-        <v>GEL-GELDAP50MLZG</v>
+        <v>GEL-GELDAP50MLMA3</v>
       </c>
       <c r="D502" t="str">
         <v/>
@@ -37584,7 +37584,7 @@
         <v>CND Shellac Base Coat</v>
       </c>
       <c r="C503" t="str">
-        <v>TOP-CNDSHELLACQJ</v>
+        <v>TOP-CNDSHELLACBA</v>
       </c>
       <c r="D503" t="str">
         <v/>
@@ -37658,7 +37658,7 @@
         <v>Cồn xanh 80 độ 5L</v>
       </c>
       <c r="C504" t="str">
-        <v>HOA-CONXANH80DWV</v>
+        <v>HOA-CONXANH80DO5</v>
       </c>
       <c r="D504" t="str">
         <v/>
@@ -37732,7 +37732,7 @@
         <v>Thùng 5in1 pedi kit tím (200c)</v>
       </c>
       <c r="C505" t="str">
-        <v>PED-THUNG5IN1PQH</v>
+        <v>PED-THUNG5IN1PED</v>
       </c>
       <c r="D505" t="str">
         <v/>
@@ -37806,7 +37806,7 @@
         <v>Oil vị dứa 500ml</v>
       </c>
       <c r="C506" t="str">
-        <v>HOA-OILVIDUA50IN</v>
+        <v>HOA-OILVIDUA500M</v>
       </c>
       <c r="D506" t="str">
         <v/>
@@ -37880,7 +37880,7 @@
         <v>Hộp Cuticle oil 48c</v>
       </c>
       <c r="C507" t="str">
-        <v>NOE-HOPCUTICLEGP</v>
+        <v>NOE-HOPCUTICLEOI</v>
       </c>
       <c r="D507" t="str">
         <v/>
@@ -37954,7 +37954,7 @@
         <v>Cuticle oil Noel</v>
       </c>
       <c r="C508" t="str">
-        <v>NOE-CUTICLEOILBB</v>
+        <v>NOE-CUTICLEOILNO</v>
       </c>
       <c r="D508" t="str">
         <v/>
@@ -38028,7 +38028,7 @@
         <v>Kem Hộp Đỏ 50ml</v>
       </c>
       <c r="C509" t="str">
-        <v>NOE-KEMHOPDO50PK</v>
+        <v>NOE-KEMHOPDO50ML</v>
       </c>
       <c r="D509" t="str">
         <v/>
@@ -38102,7 +38102,7 @@
         <v>Hộp kem mango vera 72c</v>
       </c>
       <c r="C510" t="str">
-        <v>NOE-HOPKEMMANGFR</v>
+        <v>NOE-HOPKEMMANGOV</v>
       </c>
       <c r="D510" t="str">
         <v/>
@@ -38176,7 +38176,7 @@
         <v>Dầu Massage - Aloe Vera 3.8L</v>
       </c>
       <c r="C511" t="str">
-        <v>PED-DAUMASSAGEDL</v>
+        <v>PED-DAUMASSAGEAL</v>
       </c>
       <c r="D511" t="str">
         <v/>
@@ -38250,7 +38250,7 @@
         <v>Bột Ombre Nude I</v>
       </c>
       <c r="C512" t="str">
-        <v>BOT-BOTOMBRENUFQ</v>
+        <v>BOT-BOTOMBRENUDE</v>
       </c>
       <c r="D512" t="str">
         <v/>
@@ -38324,7 +38324,7 @@
         <v>Bột - Ombre Pink II</v>
       </c>
       <c r="C513" t="str">
-        <v>BOT-BOTOMBREPIRC</v>
+        <v>BOT-BOTOMBREPINK2</v>
       </c>
       <c r="D513" t="str">
         <v/>
@@ -38398,7 +38398,7 @@
         <v>Bào mịn Diamond thông</v>
       </c>
       <c r="C514" t="str">
-        <v>DAU-BAOMINDIAMAN</v>
+        <v>DAU-BAOMINDIAMON3</v>
       </c>
       <c r="D514" t="str">
         <v/>
@@ -38472,7 +38472,7 @@
         <v>Chà chân Nano Glass</v>
       </c>
       <c r="C515" t="str">
-        <v>PED-CHACHANNANPK</v>
+        <v>PED-CHACHANNANOG</v>
       </c>
       <c r="D515" t="str">
         <v/>
@@ -38546,7 +38546,7 @@
         <v>Vòng bi tay trắng Korea 1260</v>
       </c>
       <c r="C516" t="str">
-        <v>DOD-VONGBITAYTPW</v>
+        <v>DOD-VONGBITAYTRA</v>
       </c>
       <c r="D516" t="str">
         <v/>
@@ -38620,7 +38620,7 @@
         <v>Vòng bi tay trắng Korea 1480</v>
       </c>
       <c r="C517" t="str">
-        <v>DOD-VONGBITAYTIM</v>
+        <v>DOD-VONGBITAYTRA2</v>
       </c>
       <c r="D517" t="str">
         <v/>
@@ -38694,7 +38694,7 @@
         <v>Vòng bi tay trắng Korea 1030</v>
       </c>
       <c r="C518" t="str">
-        <v>DOD-VONGBITAYTBA</v>
+        <v>DOD-VONGBITAYTRA3</v>
       </c>
       <c r="D518" t="str">
         <v/>
@@ -38768,7 +38768,7 @@
         <v>Chổi than Korea</v>
       </c>
       <c r="C519" t="str">
-        <v>DOD-CHOITHANKOJW</v>
+        <v>DOD-CHOITHANKORE</v>
       </c>
       <c r="D519" t="str">
         <v/>
@@ -38842,7 +38842,7 @@
         <v>Máy hút bụi Lugx</v>
       </c>
       <c r="C520" t="str">
-        <v>DOD-MAYHUTBUILRS</v>
+        <v>DOD-MAYHUTBUILUG</v>
       </c>
       <c r="D520" t="str">
         <v/>
@@ -38916,7 +38916,7 @@
         <v>Metallic gel liner - Gold</v>
       </c>
       <c r="C521" t="str">
-        <v>DES-METALLICGEDZ</v>
+        <v>DES-METALLICGELL</v>
       </c>
       <c r="D521" t="str">
         <v/>
@@ -38990,7 +38990,7 @@
         <v>Metallic gel liner - Silver</v>
       </c>
       <c r="C522" t="str">
-        <v>DES-METALLICGERO</v>
+        <v>DES-METALLICGELL2</v>
       </c>
       <c r="D522" t="str">
         <v/>
@@ -39064,7 +39064,7 @@
         <v>Metallic gel liner - Rose gold</v>
       </c>
       <c r="C523" t="str">
-        <v>DES-METALLICGELY</v>
+        <v>DES-METALLICGELL3</v>
       </c>
       <c r="D523" t="str">
         <v/>
@@ -39138,7 +39138,7 @@
         <v>Metallic gel liner - Champagne gold</v>
       </c>
       <c r="C524" t="str">
-        <v>DES-METALLICGEKN</v>
+        <v>DES-METALLICGELL4</v>
       </c>
       <c r="D524" t="str">
         <v/>
@@ -39212,7 +39212,7 @@
         <v>Chai primer trống có mác</v>
       </c>
       <c r="C525" t="str">
-        <v>HOA-CHAIPRIMERBD</v>
+        <v>HOA-CHAIPRIMERTR</v>
       </c>
       <c r="D525" t="str">
         <v/>
@@ -39286,7 +39286,7 @@
         <v>Chai bond trống có mác</v>
       </c>
       <c r="C526" t="str">
-        <v>TOO-CHAIBONDTRPR</v>
+        <v>TOO-CHAIBONDTRON</v>
       </c>
       <c r="D526" t="str">
         <v/>
@@ -39360,7 +39360,7 @@
         <v>Gel dặm Ombre</v>
       </c>
       <c r="C527" t="str">
-        <v>DES-GELDAMOMBRJD</v>
+        <v>DES-GELDAMOMBRE</v>
       </c>
       <c r="D527" t="str">
         <v/>
@@ -39434,7 +39434,7 @@
         <v>Reflective gel polish - Gold</v>
       </c>
       <c r="C528" t="str">
-        <v>DES-REFLECTIVESP</v>
+        <v>DES-REFLECTIVEGE</v>
       </c>
       <c r="D528" t="str">
         <v/>
@@ -39508,7 +39508,7 @@
         <v>Reflective gel polish - Silver</v>
       </c>
       <c r="C529" t="str">
-        <v>DES-REFLECTIVEEL</v>
+        <v>DES-REFLECTIVEGE2</v>
       </c>
       <c r="D529" t="str">
         <v/>
@@ -39582,7 +39582,7 @@
         <v>Reflective gel polish - Red</v>
       </c>
       <c r="C530" t="str">
-        <v>DES-REFLECTIVEOQ</v>
+        <v>DES-REFLECTIVEGE3</v>
       </c>
       <c r="D530" t="str">
         <v/>
@@ -39656,7 +39656,7 @@
         <v>Reflective gel polish - Black</v>
       </c>
       <c r="C531" t="str">
-        <v>DES-REFLECTIVEZS</v>
+        <v>DES-REFLECTIVEGE4</v>
       </c>
       <c r="D531" t="str">
         <v/>
@@ -39730,7 +39730,7 @@
         <v>Quyển mẫu sơn SORAH 300</v>
       </c>
       <c r="C532" t="str">
-        <v>SON-QUYENMAUSOGW</v>
+        <v>SON-QUYENMAUSONS</v>
       </c>
       <c r="D532" t="str">
         <v/>

</xml_diff>